<commit_message>
incorporates results with real income growth and variance.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>sp500</t>
   </si>
@@ -28,6 +28,12 @@
     <t>meanMed</t>
   </si>
   <si>
+    <t>rmeanMed</t>
+  </si>
+  <si>
+    <t>rvarMed</t>
+  </si>
+  <si>
     <t>varMed</t>
   </si>
   <si>
@@ -35,6 +41,12 @@
   </si>
   <si>
     <t>meanMean</t>
+  </si>
+  <si>
+    <t>rmeanMean</t>
+  </si>
+  <si>
+    <t>rvarMean</t>
   </si>
   <si>
     <t>varMean</t>
@@ -419,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +486,20 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,43 +510,55 @@
         <v>-0.5516119417239891</v>
       </c>
       <c r="D2">
-        <v>-0.1963170069047047</v>
+        <v>-0.2092594331816208</v>
       </c>
       <c r="E2">
-        <v>-0.2261465468559278</v>
+        <v>-0.2336779003681218</v>
       </c>
       <c r="F2">
-        <v>-0.1998315146732699</v>
+        <v>-0.2145701355275337</v>
       </c>
       <c r="G2">
-        <v>0.030096622112376</v>
+        <v>-0.08321297042119036</v>
       </c>
       <c r="H2">
-        <v>-0.2517913193583597</v>
+        <v>-0.2095226954752926</v>
       </c>
       <c r="I2">
-        <v>0.1294479452297322</v>
+        <v>0.04051949528072252</v>
       </c>
       <c r="J2">
+        <v>-0.2620287312640877</v>
+      </c>
+      <c r="K2">
+        <v>-0.2247677547302831</v>
+      </c>
+      <c r="L2">
+        <v>0.1850431082797975</v>
+      </c>
+      <c r="M2">
+        <v>0.141842926966715</v>
+      </c>
+      <c r="N2">
         <v>6.055881544898674e-17</v>
       </c>
-      <c r="K2">
+      <c r="O2">
         <v>0.0888815068024154</v>
       </c>
-      <c r="N2">
+      <c r="R2">
         <v>-0.1785047152953003</v>
       </c>
-      <c r="O2">
+      <c r="S2">
         <v>-0.1254907045969606</v>
       </c>
-      <c r="P2">
+      <c r="T2">
         <v>-0.3184960359875938</v>
       </c>
-      <c r="Q2">
+      <c r="U2">
         <v>-0.06978520298733354</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -533,613 +569,1005 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.151128568634193</v>
+        <v>0.1348896760872528</v>
       </c>
       <c r="E3">
-        <v>-0.03294665186190318</v>
+        <v>-0.02561662136325203</v>
       </c>
       <c r="F3">
-        <v>0.1722368671770338</v>
+        <v>0.156948984352565</v>
       </c>
       <c r="G3">
-        <v>-0.1139117785445092</v>
+        <v>0.1204933054041833</v>
       </c>
       <c r="H3">
-        <v>-0.06001470703570784</v>
+        <v>0.1474739997240811</v>
       </c>
       <c r="I3">
-        <v>-0.1906166427983052</v>
+        <v>-0.1413595503261372</v>
       </c>
       <c r="J3">
+        <v>-0.06767477476710231</v>
+      </c>
+      <c r="K3">
+        <v>0.156073765348183</v>
+      </c>
+      <c r="L3">
+        <v>-0.2425909640958318</v>
+      </c>
+      <c r="M3">
+        <v>-0.2102505252864032</v>
+      </c>
+      <c r="N3">
         <v>-1.146946634604127e-15</v>
       </c>
-      <c r="K3">
+      <c r="O3">
         <v>-0.1028537241709977</v>
       </c>
-      <c r="N3">
+      <c r="R3">
         <v>0.3724832149705329</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>-0.2206076074987401</v>
       </c>
-      <c r="P3">
+      <c r="T3">
         <v>0.1197012848033941</v>
       </c>
-      <c r="Q3">
+      <c r="U3">
         <v>-0.2361543508333692</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.1963170069047047</v>
+        <v>-0.2092594331816208</v>
       </c>
       <c r="C4">
-        <v>0.151128568634193</v>
+        <v>0.1348896760872528</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.6112954969410819</v>
+        <v>0.6185829412553556</v>
       </c>
       <c r="F4">
-        <v>0.9911905375444228</v>
+        <v>0.3479707316051338</v>
       </c>
       <c r="G4">
-        <v>0.7585789441086639</v>
+        <v>0.4840370449133936</v>
       </c>
       <c r="H4">
-        <v>0.7599429723231145</v>
+        <v>0.9887761441101074</v>
       </c>
       <c r="I4">
-        <v>0.6183745893117345</v>
+        <v>0.7524070446770649</v>
       </c>
       <c r="J4">
-        <v>-3.47614422849979e-15</v>
+        <v>0.760776076742018</v>
       </c>
       <c r="K4">
-        <v>-0.40761574934634</v>
+        <v>0.378557329986096</v>
+      </c>
+      <c r="L4">
+        <v>0.008872324035622799</v>
+      </c>
+      <c r="M4">
+        <v>0.6078512344604591</v>
       </c>
       <c r="N4">
-        <v>0.02771074880163954</v>
+        <v>9.886005373129641e-16</v>
       </c>
       <c r="O4">
-        <v>0.005598090883600013</v>
-      </c>
-      <c r="P4">
-        <v>0.4085591541614382</v>
-      </c>
-      <c r="Q4">
-        <v>-0.277054687168244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>-0.3757849882087373</v>
+      </c>
+      <c r="R4">
+        <v>0.03079923156668005</v>
+      </c>
+      <c r="S4">
+        <v>0.01669189688378036</v>
+      </c>
+      <c r="T4">
+        <v>0.4106640836798853</v>
+      </c>
+      <c r="U4">
+        <v>-0.2656683744986833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.2261465468559278</v>
+        <v>-0.2336779003681218</v>
       </c>
       <c r="C5">
-        <v>-0.03294665186190318</v>
+        <v>-0.02561662136325203</v>
       </c>
       <c r="D5">
-        <v>0.6112954969410819</v>
+        <v>0.6185829412553556</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.633076612114354</v>
+        <v>0.6255379752275011</v>
       </c>
       <c r="G5">
-        <v>0.5857183095245608</v>
+        <v>0.03460697650917294</v>
       </c>
       <c r="H5">
-        <v>0.9154852691648904</v>
+        <v>0.638901492391827</v>
       </c>
       <c r="I5">
-        <v>0.5425833332716857</v>
+        <v>0.5775373434413346</v>
       </c>
       <c r="J5">
-        <v>-2.886495596748317e-15</v>
+        <v>0.913778178556293</v>
       </c>
       <c r="K5">
-        <v>-0.2186963794710823</v>
+        <v>0.510584469680223</v>
+      </c>
+      <c r="L5">
+        <v>-0.09374919980923166</v>
+      </c>
+      <c r="M5">
+        <v>0.5342906816026168</v>
       </c>
       <c r="N5">
-        <v>-0.3110628407845364</v>
+        <v>3.250879470833737e-15</v>
       </c>
       <c r="O5">
-        <v>0.6179951474283341</v>
-      </c>
-      <c r="P5">
-        <v>0.4834515793307295</v>
-      </c>
-      <c r="Q5">
-        <v>0.3768609845399298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>-0.1892989896161553</v>
+      </c>
+      <c r="R5">
+        <v>-0.2928075690273048</v>
+      </c>
+      <c r="S5">
+        <v>0.6212158611861094</v>
+      </c>
+      <c r="T5">
+        <v>0.4823668343378171</v>
+      </c>
+      <c r="U5">
+        <v>0.3779016654917939</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.1998315146732699</v>
+        <v>-0.2145701355275337</v>
       </c>
       <c r="C6">
-        <v>0.1722368671770338</v>
+        <v>0.156948984352565</v>
       </c>
       <c r="D6">
-        <v>0.9911905375444228</v>
+        <v>0.3479707316051338</v>
       </c>
       <c r="E6">
-        <v>0.633076612114354</v>
+        <v>0.6255379752275011</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.7998028157490862</v>
+        <v>-0.3699275118925009</v>
       </c>
       <c r="H6">
-        <v>0.7709178304227629</v>
+        <v>0.3526646861173215</v>
       </c>
       <c r="I6">
-        <v>0.6639970073745511</v>
+        <v>0.1509964810483502</v>
       </c>
       <c r="J6">
-        <v>-1.00289147408951e-15</v>
+        <v>0.5494488785363151</v>
       </c>
       <c r="K6">
-        <v>-0.4545226068573071</v>
+        <v>0.960832683991367</v>
+      </c>
+      <c r="L6">
+        <v>-0.5371589590256646</v>
+      </c>
+      <c r="M6">
+        <v>0.1024701321064308</v>
       </c>
       <c r="N6">
-        <v>0.007538534009168323</v>
+        <v>1.075598055636969e-17</v>
       </c>
       <c r="O6">
-        <v>0.006263331587232059</v>
-      </c>
-      <c r="P6">
-        <v>0.4070767277507206</v>
-      </c>
-      <c r="Q6">
-        <v>-0.27857126049265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>0.0870647243967059</v>
+      </c>
+      <c r="R6">
+        <v>-0.07157168057157286</v>
+      </c>
+      <c r="S6">
+        <v>0.6085117260845799</v>
+      </c>
+      <c r="T6">
+        <v>0.2199901540311984</v>
+      </c>
+      <c r="U6">
+        <v>0.3504819321013322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.030096622112376</v>
+        <v>-0.08321297042119036</v>
       </c>
       <c r="C7">
-        <v>-0.1139117785445092</v>
+        <v>0.1204933054041833</v>
       </c>
       <c r="D7">
-        <v>0.7585789441086639</v>
+        <v>0.4840370449133936</v>
       </c>
       <c r="E7">
-        <v>0.5857183095245608</v>
+        <v>0.03460697650917294</v>
       </c>
       <c r="F7">
-        <v>0.7998028157490862</v>
+        <v>-0.3699275118925009</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.7245252774579077</v>
+        <v>0.5345615238474739</v>
       </c>
       <c r="I7">
-        <v>0.9597883233086776</v>
+        <v>0.6164614039208108</v>
       </c>
       <c r="J7">
-        <v>1.394118077072243e-15</v>
+        <v>0.2548234169723648</v>
       </c>
       <c r="K7">
-        <v>-0.5158992150895064</v>
+        <v>-0.3571964205890246</v>
+      </c>
+      <c r="L7">
+        <v>0.6787391593265508</v>
+      </c>
+      <c r="M7">
+        <v>0.5102591617588177</v>
       </c>
       <c r="N7">
-        <v>-0.2873630886354712</v>
+        <v>-4.150384983988022e-17</v>
       </c>
       <c r="O7">
-        <v>-0.0249441275701304</v>
-      </c>
-      <c r="P7">
-        <v>0.3661876700392565</v>
-      </c>
-      <c r="Q7">
-        <v>-0.2359720691046609</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>-0.4700674422720127</v>
+      </c>
+      <c r="R7">
+        <v>0.1416965554252693</v>
+      </c>
+      <c r="S7">
+        <v>-0.4969404705462893</v>
+      </c>
+      <c r="T7">
+        <v>0.137742416035436</v>
+      </c>
+      <c r="U7">
+        <v>-0.5556484476426126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.2517913193583597</v>
+        <v>-0.2095226954752926</v>
       </c>
       <c r="C8">
-        <v>-0.06001470703570784</v>
+        <v>0.1474739997240811</v>
       </c>
       <c r="D8">
-        <v>0.7599429723231145</v>
+        <v>0.9887761441101074</v>
       </c>
       <c r="E8">
-        <v>0.9154852691648904</v>
+        <v>0.638901492391827</v>
       </c>
       <c r="F8">
-        <v>0.7709178304227629</v>
+        <v>0.3526646861173215</v>
       </c>
       <c r="G8">
-        <v>0.7245252774579077</v>
+        <v>0.5345615238474739</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.6224686017922795</v>
+        <v>0.8009327025158507</v>
       </c>
       <c r="J8">
-        <v>-2.03065013638278e-15</v>
+        <v>0.7779374959173859</v>
       </c>
       <c r="K8">
-        <v>-0.2805377729742224</v>
+        <v>0.3679331998420695</v>
+      </c>
+      <c r="L8">
+        <v>0.09110288629819141</v>
+      </c>
+      <c r="M8">
+        <v>0.6624732165300665</v>
       </c>
       <c r="N8">
-        <v>-0.2148121241976611</v>
+        <v>9.305022531225769e-16</v>
       </c>
       <c r="O8">
-        <v>0.4851358264597269</v>
-      </c>
-      <c r="P8">
-        <v>0.5015717735161225</v>
-      </c>
-      <c r="Q8">
-        <v>0.2314536178572575</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>-0.4105431703048385</v>
+      </c>
+      <c r="R8">
+        <v>0.009308524454840244</v>
+      </c>
+      <c r="S8">
+        <v>0.01933363710994064</v>
+      </c>
+      <c r="T8">
+        <v>0.4186816217349182</v>
+      </c>
+      <c r="U8">
+        <v>-0.2708700541407726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1294479452297322</v>
+        <v>0.04051949528072252</v>
       </c>
       <c r="C9">
-        <v>-0.1906166427983052</v>
+        <v>-0.1413595503261372</v>
       </c>
       <c r="D9">
-        <v>0.6183745893117345</v>
+        <v>0.7524070446770649</v>
       </c>
       <c r="E9">
-        <v>0.5425833332716857</v>
+        <v>0.5775373434413346</v>
       </c>
       <c r="F9">
-        <v>0.6639970073745511</v>
+        <v>0.1509964810483502</v>
       </c>
       <c r="G9">
-        <v>0.9597883233086776</v>
+        <v>0.6164614039208108</v>
       </c>
       <c r="H9">
-        <v>0.6224686017922795</v>
+        <v>0.8009327025158507</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>1.698146867561228e-15</v>
+        <v>0.7161765470191056</v>
       </c>
       <c r="K9">
-        <v>-0.4952954570692921</v>
+        <v>0.1337812835800734</v>
+      </c>
+      <c r="L9">
+        <v>0.4101490551677888</v>
+      </c>
+      <c r="M9">
+        <v>0.9585594711099931</v>
       </c>
       <c r="N9">
-        <v>-0.3808421548875529</v>
+        <v>1.336930211586561e-14</v>
       </c>
       <c r="O9">
-        <v>-0.001921444763778321</v>
-      </c>
-      <c r="P9">
-        <v>0.2778070452760321</v>
-      </c>
-      <c r="Q9">
-        <v>-0.1769080841332104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>-0.4835726891054745</v>
+      </c>
+      <c r="R9">
+        <v>-0.3003137826351839</v>
+      </c>
+      <c r="S9">
+        <v>-0.006100562582623867</v>
+      </c>
+      <c r="T9">
+        <v>0.3687252251634304</v>
+      </c>
+      <c r="U9">
+        <v>-0.2214717228500268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6.055881544898674e-17</v>
+        <v>-0.2620287312640877</v>
       </c>
       <c r="C10">
-        <v>-1.146946634604127e-15</v>
+        <v>-0.06767477476710231</v>
       </c>
       <c r="D10">
-        <v>-3.47614422849979e-15</v>
+        <v>0.760776076742018</v>
       </c>
       <c r="E10">
-        <v>-2.886495596748317e-15</v>
+        <v>0.913778178556293</v>
       </c>
       <c r="F10">
-        <v>-1.00289147408951e-15</v>
+        <v>0.5494488785363151</v>
       </c>
       <c r="G10">
-        <v>1.394118077072243e-15</v>
+        <v>0.2548234169723648</v>
       </c>
       <c r="H10">
-        <v>-2.03065013638278e-15</v>
+        <v>0.7779374959173859</v>
       </c>
       <c r="I10">
-        <v>1.698146867561228e-15</v>
+        <v>0.7161765470191056</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>4.469207541101161e-15</v>
+        <v>0.4965648084821953</v>
+      </c>
+      <c r="L10">
+        <v>-0.002354724311430164</v>
+      </c>
+      <c r="M10">
+        <v>0.6100141352451111</v>
       </c>
       <c r="N10">
-        <v>2.7795804443586e-15</v>
+        <v>-5.281977542673824e-15</v>
       </c>
       <c r="O10">
-        <v>1.980989761816137e-16</v>
-      </c>
-      <c r="P10">
-        <v>1.410169364536039e-15</v>
-      </c>
-      <c r="Q10">
-        <v>8.721150744904445e-16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>-0.2550445976580443</v>
+      </c>
+      <c r="R10">
+        <v>-0.2130689583004609</v>
+      </c>
+      <c r="S10">
+        <v>0.4958701793394653</v>
+      </c>
+      <c r="T10">
+        <v>0.4970141994262009</v>
+      </c>
+      <c r="U10">
+        <v>0.242378062837054</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.0888815068024154</v>
+        <v>-0.2247677547302831</v>
       </c>
       <c r="C11">
-        <v>-0.1028537241709977</v>
+        <v>0.156073765348183</v>
       </c>
       <c r="D11">
-        <v>-0.40761574934634</v>
+        <v>0.378557329986096</v>
       </c>
       <c r="E11">
-        <v>-0.2186963794710823</v>
+        <v>0.510584469680223</v>
       </c>
       <c r="F11">
-        <v>-0.4545226068573071</v>
+        <v>0.960832683991367</v>
       </c>
       <c r="G11">
-        <v>-0.5158992150895064</v>
+        <v>-0.3571964205890246</v>
       </c>
       <c r="H11">
-        <v>-0.2805377729742224</v>
+        <v>0.3679331998420695</v>
       </c>
       <c r="I11">
-        <v>-0.4952954570692921</v>
+        <v>0.1337812835800734</v>
       </c>
       <c r="J11">
-        <v>4.469207541101161e-15</v>
+        <v>0.4965648084821953</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
+      <c r="L11">
+        <v>-0.5988120469409688</v>
+      </c>
+      <c r="M11">
+        <v>0.07939841634919623</v>
+      </c>
       <c r="N11">
-        <v>-0.002206594487502868</v>
+        <v>-1.767202548891276e-16</v>
       </c>
       <c r="O11">
-        <v>0.2946365454871068</v>
-      </c>
-      <c r="P11">
-        <v>-0.07004655851513285</v>
-      </c>
-      <c r="Q11">
-        <v>0.3463609289302713</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>0.08861014568695944</v>
+      </c>
+      <c r="R11">
+        <v>0.003958545550841385</v>
+      </c>
+      <c r="S11">
+        <v>0.5351902183551951</v>
+      </c>
+      <c r="T11">
+        <v>0.154882799832345</v>
+      </c>
+      <c r="U11">
+        <v>0.2765780350478629</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="B12">
+        <v>0.1850431082797975</v>
+      </c>
+      <c r="C12">
+        <v>-0.2425909640958318</v>
+      </c>
+      <c r="D12">
+        <v>0.008872324035622799</v>
+      </c>
+      <c r="E12">
+        <v>-0.09374919980923166</v>
+      </c>
+      <c r="F12">
+        <v>-0.5371589590256646</v>
+      </c>
+      <c r="G12">
+        <v>0.6787391593265508</v>
+      </c>
+      <c r="H12">
+        <v>0.09110288629819141</v>
+      </c>
+      <c r="I12">
+        <v>0.4101490551677888</v>
+      </c>
+      <c r="J12">
+        <v>-0.002354724311430164</v>
+      </c>
+      <c r="K12">
+        <v>-0.5988120469409688</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0.4462844046118539</v>
+      </c>
+      <c r="N12">
+        <v>-4.17312579642012e-16</v>
+      </c>
+      <c r="O12">
+        <v>-0.2063738274963798</v>
+      </c>
+      <c r="R12">
+        <v>-0.1946114723726894</v>
+      </c>
+      <c r="S12">
+        <v>-0.3216842361259434</v>
+      </c>
+      <c r="T12">
+        <v>0.03717555367098489</v>
+      </c>
+      <c r="U12">
+        <v>-0.2871981951759794</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="B13">
+        <v>0.141842926966715</v>
+      </c>
+      <c r="C13">
+        <v>-0.2102505252864032</v>
+      </c>
+      <c r="D13">
+        <v>0.6078512344604591</v>
+      </c>
+      <c r="E13">
+        <v>0.5342906816026168</v>
+      </c>
+      <c r="F13">
+        <v>0.1024701321064308</v>
+      </c>
+      <c r="G13">
+        <v>0.5102591617588177</v>
+      </c>
+      <c r="H13">
+        <v>0.6624732165300665</v>
+      </c>
+      <c r="I13">
+        <v>0.9585594711099931</v>
+      </c>
+      <c r="J13">
+        <v>0.6100141352451111</v>
+      </c>
+      <c r="K13">
+        <v>0.07939841634919623</v>
+      </c>
+      <c r="L13">
+        <v>0.4462844046118539</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1.004977796962125e-14</v>
+      </c>
+      <c r="O13">
+        <v>-0.46226132899843</v>
+      </c>
+      <c r="R13">
+        <v>-0.3938867131283825</v>
+      </c>
+      <c r="S13">
+        <v>0.01531596879256969</v>
+      </c>
+      <c r="T13">
+        <v>0.2851228561516467</v>
+      </c>
+      <c r="U13">
+        <v>-0.1633347047067167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.1785047152953003</v>
+        <v>6.055881544898674e-17</v>
       </c>
       <c r="C14">
-        <v>0.3724832149705329</v>
+        <v>-1.146946634604127e-15</v>
       </c>
       <c r="D14">
-        <v>0.02771074880163954</v>
+        <v>9.886005373129641e-16</v>
       </c>
       <c r="E14">
-        <v>-0.3110628407845364</v>
+        <v>3.250879470833737e-15</v>
       </c>
       <c r="F14">
-        <v>0.007538534009168323</v>
+        <v>1.075598055636969e-17</v>
       </c>
       <c r="G14">
-        <v>-0.2873630886354712</v>
+        <v>-4.150384983988022e-17</v>
       </c>
       <c r="H14">
-        <v>-0.2148121241976611</v>
+        <v>9.305022531225769e-16</v>
       </c>
       <c r="I14">
-        <v>-0.3808421548875529</v>
+        <v>1.336930211586561e-14</v>
       </c>
       <c r="J14">
+        <v>-5.281977542673824e-15</v>
+      </c>
+      <c r="K14">
+        <v>-1.767202548891276e-16</v>
+      </c>
+      <c r="L14">
+        <v>-4.17312579642012e-16</v>
+      </c>
+      <c r="M14">
+        <v>1.004977796962125e-14</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>4.469207541101161e-15</v>
+      </c>
+      <c r="R14">
         <v>2.7795804443586e-15</v>
       </c>
-      <c r="K14">
-        <v>-0.002206594487502868</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>-0.2721965536453438</v>
-      </c>
-      <c r="P14">
-        <v>-0.01915406161276758</v>
-      </c>
-      <c r="Q14">
-        <v>-0.2391338560180774</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="S14">
+        <v>1.980989761816137e-16</v>
+      </c>
+      <c r="T14">
+        <v>1.410169364536039e-15</v>
+      </c>
+      <c r="U14">
+        <v>8.721150744904445e-16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.1254907045969606</v>
+        <v>0.0888815068024154</v>
       </c>
       <c r="C15">
-        <v>-0.2206076074987401</v>
+        <v>-0.1028537241709977</v>
       </c>
       <c r="D15">
-        <v>0.005598090883600013</v>
+        <v>-0.3757849882087373</v>
       </c>
       <c r="E15">
-        <v>0.6179951474283341</v>
+        <v>-0.1892989896161553</v>
       </c>
       <c r="F15">
-        <v>0.006263331587232059</v>
+        <v>0.0870647243967059</v>
       </c>
       <c r="G15">
-        <v>-0.0249441275701304</v>
+        <v>-0.4700674422720127</v>
       </c>
       <c r="H15">
-        <v>0.4851358264597269</v>
+        <v>-0.4105431703048385</v>
       </c>
       <c r="I15">
-        <v>-0.001921444763778321</v>
+        <v>-0.4835726891054745</v>
       </c>
       <c r="J15">
-        <v>1.980989761816137e-16</v>
+        <v>-0.2550445976580443</v>
       </c>
       <c r="K15">
+        <v>0.08861014568695944</v>
+      </c>
+      <c r="L15">
+        <v>-0.2063738274963798</v>
+      </c>
+      <c r="M15">
+        <v>-0.46226132899843</v>
+      </c>
+      <c r="N15">
+        <v>4.469207541101161e-15</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>-0.002206594487502868</v>
+      </c>
+      <c r="S15">
         <v>0.2946365454871068</v>
       </c>
-      <c r="N15">
-        <v>-0.2721965536453438</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>0.1658873665894034</v>
-      </c>
-      <c r="Q15">
-        <v>0.9098052194387964</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="T15">
+        <v>-0.07004655851513285</v>
+      </c>
+      <c r="U15">
+        <v>0.3463609289302713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>-0.3184960359875938</v>
-      </c>
-      <c r="C16">
-        <v>0.1197012848033941</v>
-      </c>
-      <c r="D16">
-        <v>0.4085591541614382</v>
-      </c>
-      <c r="E16">
-        <v>0.4834515793307295</v>
-      </c>
-      <c r="F16">
-        <v>0.4070767277507206</v>
-      </c>
-      <c r="G16">
-        <v>0.3661876700392565</v>
-      </c>
-      <c r="H16">
-        <v>0.5015717735161225</v>
-      </c>
-      <c r="I16">
-        <v>0.2778070452760321</v>
-      </c>
-      <c r="J16">
-        <v>1.410169364536039e-15</v>
-      </c>
-      <c r="K16">
-        <v>-0.07004655851513285</v>
-      </c>
-      <c r="N16">
-        <v>-0.01915406161276758</v>
-      </c>
-      <c r="O16">
-        <v>0.1658873665894034</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>-0.01269413487343376</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>-0.1785047152953003</v>
+      </c>
+      <c r="C18">
+        <v>0.3724832149705329</v>
+      </c>
+      <c r="D18">
+        <v>0.03079923156668005</v>
+      </c>
+      <c r="E18">
+        <v>-0.2928075690273048</v>
+      </c>
+      <c r="F18">
+        <v>-0.07157168057157286</v>
+      </c>
+      <c r="G18">
+        <v>0.1416965554252693</v>
+      </c>
+      <c r="H18">
+        <v>0.009308524454840244</v>
+      </c>
+      <c r="I18">
+        <v>-0.3003137826351839</v>
+      </c>
+      <c r="J18">
+        <v>-0.2130689583004609</v>
+      </c>
+      <c r="K18">
+        <v>0.003958545550841385</v>
+      </c>
+      <c r="L18">
+        <v>-0.1946114723726894</v>
+      </c>
+      <c r="M18">
+        <v>-0.3938867131283825</v>
+      </c>
+      <c r="N18">
+        <v>2.7795804443586e-15</v>
+      </c>
+      <c r="O18">
+        <v>-0.002206594487502868</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>-0.2721965536453438</v>
+      </c>
+      <c r="T18">
+        <v>-0.01915406161276758</v>
+      </c>
+      <c r="U18">
+        <v>-0.2391338560180774</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>-0.1254907045969606</v>
+      </c>
+      <c r="C19">
+        <v>-0.2206076074987401</v>
+      </c>
+      <c r="D19">
+        <v>0.01669189688378036</v>
+      </c>
+      <c r="E19">
+        <v>0.6212158611861094</v>
+      </c>
+      <c r="F19">
+        <v>0.6085117260845799</v>
+      </c>
+      <c r="G19">
+        <v>-0.4969404705462893</v>
+      </c>
+      <c r="H19">
+        <v>0.01933363710994064</v>
+      </c>
+      <c r="I19">
+        <v>-0.006100562582623867</v>
+      </c>
+      <c r="J19">
+        <v>0.4958701793394653</v>
+      </c>
+      <c r="K19">
+        <v>0.5351902183551951</v>
+      </c>
+      <c r="L19">
+        <v>-0.3216842361259434</v>
+      </c>
+      <c r="M19">
+        <v>0.01531596879256969</v>
+      </c>
+      <c r="N19">
+        <v>1.980989761816137e-16</v>
+      </c>
+      <c r="O19">
+        <v>0.2946365454871068</v>
+      </c>
+      <c r="R19">
+        <v>-0.2721965536453438</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0.1658873665894034</v>
+      </c>
+      <c r="U19">
+        <v>0.9098052194387964</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>-0.3184960359875938</v>
+      </c>
+      <c r="C20">
+        <v>0.1197012848033941</v>
+      </c>
+      <c r="D20">
+        <v>0.4106640836798853</v>
+      </c>
+      <c r="E20">
+        <v>0.4823668343378171</v>
+      </c>
+      <c r="F20">
+        <v>0.2199901540311984</v>
+      </c>
+      <c r="G20">
+        <v>0.137742416035436</v>
+      </c>
+      <c r="H20">
+        <v>0.4186816217349182</v>
+      </c>
+      <c r="I20">
+        <v>0.3687252251634304</v>
+      </c>
+      <c r="J20">
+        <v>0.4970141994262009</v>
+      </c>
+      <c r="K20">
+        <v>0.154882799832345</v>
+      </c>
+      <c r="L20">
+        <v>0.03717555367098489</v>
+      </c>
+      <c r="M20">
+        <v>0.2851228561516467</v>
+      </c>
+      <c r="N20">
+        <v>1.410169364536039e-15</v>
+      </c>
+      <c r="O20">
+        <v>-0.07004655851513285</v>
+      </c>
+      <c r="R20">
+        <v>-0.01915406161276758</v>
+      </c>
+      <c r="S20">
+        <v>0.1658873665894034</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>-0.01269413487343376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
         <v>-0.06978520298733354</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <v>-0.2361543508333692</v>
       </c>
-      <c r="D17">
-        <v>-0.277054687168244</v>
-      </c>
-      <c r="E17">
-        <v>0.3768609845399298</v>
-      </c>
-      <c r="F17">
-        <v>-0.27857126049265</v>
-      </c>
-      <c r="G17">
-        <v>-0.2359720691046609</v>
-      </c>
-      <c r="H17">
-        <v>0.2314536178572575</v>
-      </c>
-      <c r="I17">
-        <v>-0.1769080841332104</v>
-      </c>
-      <c r="J17">
+      <c r="D21">
+        <v>-0.2656683744986833</v>
+      </c>
+      <c r="E21">
+        <v>0.3779016654917939</v>
+      </c>
+      <c r="F21">
+        <v>0.3504819321013322</v>
+      </c>
+      <c r="G21">
+        <v>-0.5556484476426126</v>
+      </c>
+      <c r="H21">
+        <v>-0.2708700541407726</v>
+      </c>
+      <c r="I21">
+        <v>-0.2214717228500268</v>
+      </c>
+      <c r="J21">
+        <v>0.242378062837054</v>
+      </c>
+      <c r="K21">
+        <v>0.2765780350478629</v>
+      </c>
+      <c r="L21">
+        <v>-0.2871981951759794</v>
+      </c>
+      <c r="M21">
+        <v>-0.1633347047067167</v>
+      </c>
+      <c r="N21">
         <v>8.721150744904445e-16</v>
       </c>
-      <c r="K17">
+      <c r="O21">
         <v>0.3463609289302713</v>
       </c>
-      <c r="N17">
+      <c r="R21">
         <v>-0.2391338560180774</v>
       </c>
-      <c r="O17">
+      <c r="S21">
         <v>0.9098052194387964</v>
       </c>
-      <c r="P17">
+      <c r="T21">
         <v>-0.01269413487343376</v>
       </c>
-      <c r="Q17">
+      <c r="U21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
drafting halfway on macro section. Need to finish and proofread.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -510,34 +510,34 @@
         <v>-0.5516119417239891</v>
       </c>
       <c r="D2">
-        <v>-0.2092594331816208</v>
+        <v>-0.1609705267258305</v>
       </c>
       <c r="E2">
-        <v>-0.2336779003681218</v>
+        <v>-0.2146382865242739</v>
       </c>
       <c r="F2">
-        <v>-0.2145701355275337</v>
+        <v>-0.2390098332268563</v>
       </c>
       <c r="G2">
-        <v>-0.08321297042119036</v>
+        <v>-0.1318081117631396</v>
       </c>
       <c r="H2">
-        <v>-0.2095226954752926</v>
+        <v>-0.1751586568075148</v>
       </c>
       <c r="I2">
-        <v>0.04051949528072252</v>
+        <v>0.02463671945219919</v>
       </c>
       <c r="J2">
-        <v>-0.2620287312640877</v>
+        <v>-0.2442575912937952</v>
       </c>
       <c r="K2">
-        <v>-0.2247677547302831</v>
+        <v>-0.2755229145892673</v>
       </c>
       <c r="L2">
-        <v>0.1850431082797975</v>
+        <v>0.009011369349083607</v>
       </c>
       <c r="M2">
-        <v>0.141842926966715</v>
+        <v>0.0925382074692313</v>
       </c>
       <c r="N2">
         <v>6.055881544898674e-17</v>
@@ -569,34 +569,34 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1348896760872528</v>
+        <v>0.09593726714713641</v>
       </c>
       <c r="E3">
-        <v>-0.02561662136325203</v>
+        <v>0.006695480955382251</v>
       </c>
       <c r="F3">
-        <v>0.156948984352565</v>
+        <v>0.1790023632918195</v>
       </c>
       <c r="G3">
-        <v>0.1204933054041833</v>
+        <v>0.236592323055357</v>
       </c>
       <c r="H3">
-        <v>0.1474739997240811</v>
+        <v>0.1134940197879655</v>
       </c>
       <c r="I3">
-        <v>-0.1413595503261372</v>
+        <v>-0.03114961804922891</v>
       </c>
       <c r="J3">
-        <v>-0.06767477476710231</v>
+        <v>-0.0457566048628302</v>
       </c>
       <c r="K3">
-        <v>0.156073765348183</v>
+        <v>0.142999274089144</v>
       </c>
       <c r="L3">
-        <v>-0.2425909640958318</v>
+        <v>0.1737101849475536</v>
       </c>
       <c r="M3">
-        <v>-0.2102505252864032</v>
+        <v>-0.01979505732831893</v>
       </c>
       <c r="N3">
         <v>-1.146946634604127e-15</v>
@@ -622,58 +622,58 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.2092594331816208</v>
+        <v>-0.1609705267258305</v>
       </c>
       <c r="C4">
-        <v>0.1348896760872528</v>
+        <v>0.09593726714713641</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.6185829412553556</v>
+        <v>0.6468349212578923</v>
       </c>
       <c r="F4">
-        <v>0.3479707316051338</v>
+        <v>0.1517513741527407</v>
       </c>
       <c r="G4">
-        <v>0.4840370449133936</v>
+        <v>0.8005362249079484</v>
       </c>
       <c r="H4">
-        <v>0.9887761441101074</v>
+        <v>0.992481873816037</v>
       </c>
       <c r="I4">
-        <v>0.7524070446770649</v>
+        <v>0.879975068712724</v>
       </c>
       <c r="J4">
-        <v>0.760776076742018</v>
+        <v>0.7965766664278233</v>
       </c>
       <c r="K4">
-        <v>0.378557329986096</v>
+        <v>0.247022406716849</v>
       </c>
       <c r="L4">
-        <v>0.008872324035622799</v>
+        <v>0.6139816498137851</v>
       </c>
       <c r="M4">
-        <v>0.6078512344604591</v>
+        <v>0.7794274091831108</v>
       </c>
       <c r="N4">
-        <v>9.886005373129641e-16</v>
+        <v>-5.26312476638483e-16</v>
       </c>
       <c r="O4">
-        <v>-0.3757849882087373</v>
+        <v>-0.4844866619882676</v>
       </c>
       <c r="R4">
-        <v>0.03079923156668005</v>
+        <v>-0.03589309818135301</v>
       </c>
       <c r="S4">
-        <v>0.01669189688378036</v>
+        <v>-0.06869523931865897</v>
       </c>
       <c r="T4">
-        <v>0.4106640836798853</v>
+        <v>0.4051407095347814</v>
       </c>
       <c r="U4">
-        <v>-0.2656683744986833</v>
+        <v>-0.3079389633548364</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -681,58 +681,58 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.2336779003681218</v>
+        <v>-0.2146382865242739</v>
       </c>
       <c r="C5">
-        <v>-0.02561662136325203</v>
+        <v>0.006695480955382251</v>
       </c>
       <c r="D5">
-        <v>0.6185829412553556</v>
+        <v>0.6468349212578923</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.6255379752275011</v>
+        <v>0.5872880800836626</v>
       </c>
       <c r="G5">
-        <v>0.03460697650917294</v>
+        <v>0.2893474286312728</v>
       </c>
       <c r="H5">
-        <v>0.638901492391827</v>
+        <v>0.6672795322378595</v>
       </c>
       <c r="I5">
-        <v>0.5775373434413346</v>
+        <v>0.5512808457963762</v>
       </c>
       <c r="J5">
-        <v>0.913778178556293</v>
+        <v>0.9138020468399077</v>
       </c>
       <c r="K5">
-        <v>0.510584469680223</v>
+        <v>0.5629301671802283</v>
       </c>
       <c r="L5">
-        <v>-0.09374919980923166</v>
+        <v>0.2737963524037204</v>
       </c>
       <c r="M5">
-        <v>0.5342906816026168</v>
+        <v>0.5140728904674001</v>
       </c>
       <c r="N5">
-        <v>3.250879470833737e-15</v>
+        <v>-7.810849885615325e-15</v>
       </c>
       <c r="O5">
-        <v>-0.1892989896161553</v>
+        <v>-0.2130141436281778</v>
       </c>
       <c r="R5">
-        <v>-0.2928075690273048</v>
+        <v>-0.280230938060934</v>
       </c>
       <c r="S5">
-        <v>0.6212158611861094</v>
+        <v>0.5469064887048238</v>
       </c>
       <c r="T5">
-        <v>0.4823668343378171</v>
+        <v>0.4333987620781303</v>
       </c>
       <c r="U5">
-        <v>0.3779016654917939</v>
+        <v>0.3026222090640849</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -740,58 +740,58 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.2145701355275337</v>
+        <v>-0.2390098332268563</v>
       </c>
       <c r="C6">
-        <v>0.156948984352565</v>
+        <v>0.1790023632918195</v>
       </c>
       <c r="D6">
-        <v>0.3479707316051338</v>
+        <v>0.1517513741527407</v>
       </c>
       <c r="E6">
-        <v>0.6255379752275011</v>
+        <v>0.5872880800836626</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>-0.3699275118925009</v>
+        <v>-0.09770875581285839</v>
       </c>
       <c r="H6">
-        <v>0.3526646861173215</v>
+        <v>0.1639019505469678</v>
       </c>
       <c r="I6">
-        <v>0.1509964810483502</v>
+        <v>0.0003716899051861331</v>
       </c>
       <c r="J6">
-        <v>0.5494488785363151</v>
+        <v>0.502855144844632</v>
       </c>
       <c r="K6">
-        <v>0.960832683991367</v>
+        <v>0.9588684709491565</v>
       </c>
       <c r="L6">
-        <v>-0.5371589590256646</v>
+        <v>-0.1493617584562276</v>
       </c>
       <c r="M6">
-        <v>0.1024701321064308</v>
+        <v>-0.006990666893042056</v>
       </c>
       <c r="N6">
-        <v>1.075598055636969e-17</v>
+        <v>2.57649465002784e-16</v>
       </c>
       <c r="O6">
-        <v>0.0870647243967059</v>
+        <v>0.0855701284130547</v>
       </c>
       <c r="R6">
-        <v>-0.07157168057157286</v>
+        <v>-0.06116014632225203</v>
       </c>
       <c r="S6">
-        <v>0.6085117260845799</v>
+        <v>0.6117187837479278</v>
       </c>
       <c r="T6">
-        <v>0.2199901540311984</v>
+        <v>0.2210368374975278</v>
       </c>
       <c r="U6">
-        <v>0.3504819321013322</v>
+        <v>0.3544617503524454</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -799,58 +799,58 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.08321297042119036</v>
+        <v>-0.1318081117631396</v>
       </c>
       <c r="C7">
-        <v>0.1204933054041833</v>
+        <v>0.236592323055357</v>
       </c>
       <c r="D7">
-        <v>0.4840370449133936</v>
+        <v>0.8005362249079484</v>
       </c>
       <c r="E7">
-        <v>0.03460697650917294</v>
+        <v>0.2893474286312728</v>
       </c>
       <c r="F7">
-        <v>-0.3699275118925009</v>
+        <v>-0.09770875581285839</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.5345615238474739</v>
+        <v>0.7964976254513817</v>
       </c>
       <c r="I7">
-        <v>0.6164614039208108</v>
+        <v>0.8108052446228973</v>
       </c>
       <c r="J7">
-        <v>0.2548234169723648</v>
+        <v>0.4938463860778851</v>
       </c>
       <c r="K7">
-        <v>-0.3571964205890246</v>
+        <v>-0.02856147293314673</v>
       </c>
       <c r="L7">
-        <v>0.6787391593265508</v>
+        <v>0.7920023106189256</v>
       </c>
       <c r="M7">
-        <v>0.5102591617588177</v>
+        <v>0.719852674429839</v>
       </c>
       <c r="N7">
-        <v>-4.150384983988022e-17</v>
+        <v>9.535275711450758e-16</v>
       </c>
       <c r="O7">
-        <v>-0.4700674422720127</v>
+        <v>-0.5470942344968723</v>
       </c>
       <c r="R7">
-        <v>0.1416965554252693</v>
+        <v>0.1608069006810534</v>
       </c>
       <c r="S7">
-        <v>-0.4969404705462893</v>
+        <v>-0.4059303727331163</v>
       </c>
       <c r="T7">
-        <v>0.137742416035436</v>
+        <v>0.1992734032194558</v>
       </c>
       <c r="U7">
-        <v>-0.5556484476426126</v>
+        <v>-0.5436623410446169</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -858,58 +858,58 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.2095226954752926</v>
+        <v>-0.1751586568075148</v>
       </c>
       <c r="C8">
-        <v>0.1474739997240811</v>
+        <v>0.1134940197879655</v>
       </c>
       <c r="D8">
-        <v>0.9887761441101074</v>
+        <v>0.992481873816037</v>
       </c>
       <c r="E8">
-        <v>0.638901492391827</v>
+        <v>0.6672795322378595</v>
       </c>
       <c r="F8">
-        <v>0.3526646861173215</v>
+        <v>0.1639019505469678</v>
       </c>
       <c r="G8">
-        <v>0.5345615238474739</v>
+        <v>0.7964976254513817</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.8009327025158507</v>
+        <v>0.8831410516690518</v>
       </c>
       <c r="J8">
-        <v>0.7779374959173859</v>
+        <v>0.8062050703183056</v>
       </c>
       <c r="K8">
-        <v>0.3679331998420695</v>
+        <v>0.2679550097626913</v>
       </c>
       <c r="L8">
-        <v>0.09110288629819141</v>
+        <v>0.6081518477431341</v>
       </c>
       <c r="M8">
-        <v>0.6624732165300665</v>
+        <v>0.7908801559917824</v>
       </c>
       <c r="N8">
-        <v>9.305022531225769e-16</v>
+        <v>3.144896282365325e-16</v>
       </c>
       <c r="O8">
-        <v>-0.4105431703048385</v>
+        <v>-0.468465924749046</v>
       </c>
       <c r="R8">
-        <v>0.009308524454840244</v>
+        <v>-0.03594240137942541</v>
       </c>
       <c r="S8">
-        <v>0.01933363710994064</v>
+        <v>-0.06505595629729606</v>
       </c>
       <c r="T8">
-        <v>0.4186816217349182</v>
+        <v>0.3933974245641507</v>
       </c>
       <c r="U8">
-        <v>-0.2708700541407726</v>
+        <v>-0.3064871945736838</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -917,58 +917,58 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.04051949528072252</v>
+        <v>0.02463671945219919</v>
       </c>
       <c r="C9">
-        <v>-0.1413595503261372</v>
+        <v>-0.03114961804922891</v>
       </c>
       <c r="D9">
-        <v>0.7524070446770649</v>
+        <v>0.879975068712724</v>
       </c>
       <c r="E9">
-        <v>0.5775373434413346</v>
+        <v>0.5512808457963762</v>
       </c>
       <c r="F9">
-        <v>0.1509964810483502</v>
+        <v>0.0003716899051861331</v>
       </c>
       <c r="G9">
-        <v>0.6164614039208108</v>
+        <v>0.8108052446228973</v>
       </c>
       <c r="H9">
-        <v>0.8009327025158507</v>
+        <v>0.8831410516690518</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.7161765470191056</v>
+        <v>0.7085765328289897</v>
       </c>
       <c r="K9">
-        <v>0.1337812835800734</v>
+        <v>0.07508672573744717</v>
       </c>
       <c r="L9">
-        <v>0.4101490551677888</v>
+        <v>0.7775634838244121</v>
       </c>
       <c r="M9">
-        <v>0.9585594711099931</v>
+        <v>0.9678760915982535</v>
       </c>
       <c r="N9">
-        <v>1.336930211586561e-14</v>
+        <v>8.12849579998413e-15</v>
       </c>
       <c r="O9">
-        <v>-0.4835726891054745</v>
+        <v>-0.5546927522474058</v>
       </c>
       <c r="R9">
-        <v>-0.3003137826351839</v>
+        <v>-0.2162934290481094</v>
       </c>
       <c r="S9">
-        <v>-0.006100562582623867</v>
+        <v>-0.1304860423842069</v>
       </c>
       <c r="T9">
-        <v>0.3687252251634304</v>
+        <v>0.300194367852684</v>
       </c>
       <c r="U9">
-        <v>-0.2214717228500268</v>
+        <v>-0.306152546074295</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -976,58 +976,58 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.2620287312640877</v>
+        <v>-0.2442575912937952</v>
       </c>
       <c r="C10">
-        <v>-0.06767477476710231</v>
+        <v>-0.0457566048628302</v>
       </c>
       <c r="D10">
-        <v>0.760776076742018</v>
+        <v>0.7965766664278233</v>
       </c>
       <c r="E10">
-        <v>0.913778178556293</v>
+        <v>0.9138020468399077</v>
       </c>
       <c r="F10">
-        <v>0.5494488785363151</v>
+        <v>0.502855144844632</v>
       </c>
       <c r="G10">
-        <v>0.2548234169723648</v>
+        <v>0.4938463860778851</v>
       </c>
       <c r="H10">
-        <v>0.7779374959173859</v>
+        <v>0.8062050703183056</v>
       </c>
       <c r="I10">
-        <v>0.7161765470191056</v>
+        <v>0.7085765328289897</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.4965648084821953</v>
+        <v>0.55554696291363</v>
       </c>
       <c r="L10">
-        <v>-0.002354724311430164</v>
+        <v>0.3727458451678964</v>
       </c>
       <c r="M10">
-        <v>0.6100141352451111</v>
+        <v>0.6266383697311377</v>
       </c>
       <c r="N10">
-        <v>-5.281977542673824e-15</v>
+        <v>5.597603306782835e-15</v>
       </c>
       <c r="O10">
-        <v>-0.2550445976580443</v>
+        <v>-0.2970439799879107</v>
       </c>
       <c r="R10">
-        <v>-0.2130689583004609</v>
+        <v>-0.2043475672720929</v>
       </c>
       <c r="S10">
-        <v>0.4958701793394653</v>
+        <v>0.4155624733203104</v>
       </c>
       <c r="T10">
-        <v>0.4970141994262009</v>
+        <v>0.4637893251987291</v>
       </c>
       <c r="U10">
-        <v>0.242378062837054</v>
+        <v>0.1648409968246075</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1035,58 +1035,58 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.2247677547302831</v>
+        <v>-0.2755229145892673</v>
       </c>
       <c r="C11">
-        <v>0.156073765348183</v>
+        <v>0.142999274089144</v>
       </c>
       <c r="D11">
-        <v>0.378557329986096</v>
+        <v>0.247022406716849</v>
       </c>
       <c r="E11">
-        <v>0.510584469680223</v>
+        <v>0.5629301671802283</v>
       </c>
       <c r="F11">
-        <v>0.960832683991367</v>
+        <v>0.9588684709491565</v>
       </c>
       <c r="G11">
-        <v>-0.3571964205890246</v>
+        <v>-0.02856147293314673</v>
       </c>
       <c r="H11">
-        <v>0.3679331998420695</v>
+        <v>0.2679550097626913</v>
       </c>
       <c r="I11">
-        <v>0.1337812835800734</v>
+        <v>0.07508672573744717</v>
       </c>
       <c r="J11">
-        <v>0.4965648084821953</v>
+        <v>0.55554696291363</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>-0.5988120469409688</v>
+        <v>-0.1697350189515449</v>
       </c>
       <c r="M11">
-        <v>0.07939841634919623</v>
+        <v>0.04463684494335034</v>
       </c>
       <c r="N11">
-        <v>-1.767202548891276e-16</v>
+        <v>-3.663853772685152e-17</v>
       </c>
       <c r="O11">
-        <v>0.08861014568695944</v>
+        <v>0.1048326526071779</v>
       </c>
       <c r="R11">
-        <v>0.003958545550841385</v>
+        <v>-0.02022194646378487</v>
       </c>
       <c r="S11">
-        <v>0.5351902183551951</v>
+        <v>0.5449871295609625</v>
       </c>
       <c r="T11">
-        <v>0.154882799832345</v>
+        <v>0.2412286367885081</v>
       </c>
       <c r="U11">
-        <v>0.2765780350478629</v>
+        <v>0.2638080676402369</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1094,58 +1094,58 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1850431082797975</v>
+        <v>0.009011369349083607</v>
       </c>
       <c r="C12">
-        <v>-0.2425909640958318</v>
+        <v>0.1737101849475536</v>
       </c>
       <c r="D12">
-        <v>0.008872324035622799</v>
+        <v>0.6139816498137851</v>
       </c>
       <c r="E12">
-        <v>-0.09374919980923166</v>
+        <v>0.2737963524037204</v>
       </c>
       <c r="F12">
-        <v>-0.5371589590256646</v>
+        <v>-0.1493617584562276</v>
       </c>
       <c r="G12">
-        <v>0.6787391593265508</v>
+        <v>0.7920023106189256</v>
       </c>
       <c r="H12">
-        <v>0.09110288629819141</v>
+        <v>0.6081518477431341</v>
       </c>
       <c r="I12">
-        <v>0.4101490551677888</v>
+        <v>0.7775634838244121</v>
       </c>
       <c r="J12">
-        <v>-0.002354724311430164</v>
+        <v>0.3727458451678964</v>
       </c>
       <c r="K12">
-        <v>-0.5988120469409688</v>
+        <v>-0.1697350189515449</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.4462844046118539</v>
+        <v>0.7920607960994264</v>
       </c>
       <c r="N12">
-        <v>-4.17312579642012e-16</v>
+        <v>-6.417188599869865e-15</v>
       </c>
       <c r="O12">
-        <v>-0.2063738274963798</v>
+        <v>-0.4530916816463709</v>
       </c>
       <c r="R12">
-        <v>-0.1946114723726894</v>
+        <v>-0.1030604501630649</v>
       </c>
       <c r="S12">
-        <v>-0.3216842361259434</v>
+        <v>-0.2610189723011284</v>
       </c>
       <c r="T12">
-        <v>0.03717555367098489</v>
+        <v>0.1513992691542027</v>
       </c>
       <c r="U12">
-        <v>-0.2871981951759794</v>
+        <v>-0.3676193604901473</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1153,58 +1153,58 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.141842926966715</v>
+        <v>0.0925382074692313</v>
       </c>
       <c r="C13">
-        <v>-0.2102505252864032</v>
+        <v>-0.01979505732831893</v>
       </c>
       <c r="D13">
-        <v>0.6078512344604591</v>
+        <v>0.7794274091831108</v>
       </c>
       <c r="E13">
-        <v>0.5342906816026168</v>
+        <v>0.5140728904674001</v>
       </c>
       <c r="F13">
-        <v>0.1024701321064308</v>
+        <v>-0.006990666893042056</v>
       </c>
       <c r="G13">
-        <v>0.5102591617588177</v>
+        <v>0.719852674429839</v>
       </c>
       <c r="H13">
-        <v>0.6624732165300665</v>
+        <v>0.7908801559917824</v>
       </c>
       <c r="I13">
-        <v>0.9585594711099931</v>
+        <v>0.9678760915982535</v>
       </c>
       <c r="J13">
-        <v>0.6100141352451111</v>
+        <v>0.6266383697311377</v>
       </c>
       <c r="K13">
-        <v>0.07939841634919623</v>
+        <v>0.04463684494335034</v>
       </c>
       <c r="L13">
-        <v>0.4462844046118539</v>
+        <v>0.7920607960994264</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>1.004977796962125e-14</v>
+        <v>-1.202197081870329e-16</v>
       </c>
       <c r="O13">
-        <v>-0.46226132899843</v>
+        <v>-0.5644056674894997</v>
       </c>
       <c r="R13">
-        <v>-0.3938867131283825</v>
+        <v>-0.2804808943433733</v>
       </c>
       <c r="S13">
-        <v>0.01531596879256969</v>
+        <v>-0.115748703784505</v>
       </c>
       <c r="T13">
-        <v>0.2851228561516467</v>
+        <v>0.2140391375821556</v>
       </c>
       <c r="U13">
-        <v>-0.1633347047067167</v>
+        <v>-0.261741111092062</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1218,34 +1218,34 @@
         <v>-1.146946634604127e-15</v>
       </c>
       <c r="D14">
-        <v>9.886005373129641e-16</v>
+        <v>-5.26312476638483e-16</v>
       </c>
       <c r="E14">
-        <v>3.250879470833737e-15</v>
+        <v>-7.810849885615325e-15</v>
       </c>
       <c r="F14">
-        <v>1.075598055636969e-17</v>
+        <v>2.57649465002784e-16</v>
       </c>
       <c r="G14">
-        <v>-4.150384983988022e-17</v>
+        <v>9.535275711450758e-16</v>
       </c>
       <c r="H14">
-        <v>9.305022531225769e-16</v>
+        <v>3.144896282365325e-16</v>
       </c>
       <c r="I14">
-        <v>1.336930211586561e-14</v>
+        <v>8.12849579998413e-15</v>
       </c>
       <c r="J14">
-        <v>-5.281977542673824e-15</v>
+        <v>5.597603306782835e-15</v>
       </c>
       <c r="K14">
-        <v>-1.767202548891276e-16</v>
+        <v>-3.663853772685152e-17</v>
       </c>
       <c r="L14">
-        <v>-4.17312579642012e-16</v>
+        <v>-6.417188599869865e-15</v>
       </c>
       <c r="M14">
-        <v>1.004977796962125e-14</v>
+        <v>-1.202197081870329e-16</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1277,34 +1277,34 @@
         <v>-0.1028537241709977</v>
       </c>
       <c r="D15">
-        <v>-0.3757849882087373</v>
+        <v>-0.4844866619882676</v>
       </c>
       <c r="E15">
-        <v>-0.1892989896161553</v>
+        <v>-0.2130141436281778</v>
       </c>
       <c r="F15">
-        <v>0.0870647243967059</v>
+        <v>0.0855701284130547</v>
       </c>
       <c r="G15">
-        <v>-0.4700674422720127</v>
+        <v>-0.5470942344968723</v>
       </c>
       <c r="H15">
-        <v>-0.4105431703048385</v>
+        <v>-0.468465924749046</v>
       </c>
       <c r="I15">
-        <v>-0.4835726891054745</v>
+        <v>-0.5546927522474058</v>
       </c>
       <c r="J15">
-        <v>-0.2550445976580443</v>
+        <v>-0.2970439799879107</v>
       </c>
       <c r="K15">
-        <v>0.08861014568695944</v>
+        <v>0.1048326526071779</v>
       </c>
       <c r="L15">
-        <v>-0.2063738274963798</v>
+        <v>-0.4530916816463709</v>
       </c>
       <c r="M15">
-        <v>-0.46226132899843</v>
+        <v>-0.5644056674894997</v>
       </c>
       <c r="N15">
         <v>4.469207541101161e-15</v>
@@ -1346,34 +1346,34 @@
         <v>0.3724832149705329</v>
       </c>
       <c r="D18">
-        <v>0.03079923156668005</v>
+        <v>-0.03589309818135301</v>
       </c>
       <c r="E18">
-        <v>-0.2928075690273048</v>
+        <v>-0.280230938060934</v>
       </c>
       <c r="F18">
-        <v>-0.07157168057157286</v>
+        <v>-0.06116014632225203</v>
       </c>
       <c r="G18">
-        <v>0.1416965554252693</v>
+        <v>0.1608069006810534</v>
       </c>
       <c r="H18">
-        <v>0.009308524454840244</v>
+        <v>-0.03594240137942541</v>
       </c>
       <c r="I18">
-        <v>-0.3003137826351839</v>
+        <v>-0.2162934290481094</v>
       </c>
       <c r="J18">
-        <v>-0.2130689583004609</v>
+        <v>-0.2043475672720929</v>
       </c>
       <c r="K18">
-        <v>0.003958545550841385</v>
+        <v>-0.02022194646378487</v>
       </c>
       <c r="L18">
-        <v>-0.1946114723726894</v>
+        <v>-0.1030604501630649</v>
       </c>
       <c r="M18">
-        <v>-0.3938867131283825</v>
+        <v>-0.2804808943433733</v>
       </c>
       <c r="N18">
         <v>2.7795804443586e-15</v>
@@ -1405,34 +1405,34 @@
         <v>-0.2206076074987401</v>
       </c>
       <c r="D19">
-        <v>0.01669189688378036</v>
+        <v>-0.06869523931865897</v>
       </c>
       <c r="E19">
-        <v>0.6212158611861094</v>
+        <v>0.5469064887048238</v>
       </c>
       <c r="F19">
-        <v>0.6085117260845799</v>
+        <v>0.6117187837479278</v>
       </c>
       <c r="G19">
-        <v>-0.4969404705462893</v>
+        <v>-0.4059303727331163</v>
       </c>
       <c r="H19">
-        <v>0.01933363710994064</v>
+        <v>-0.06505595629729606</v>
       </c>
       <c r="I19">
-        <v>-0.006100562582623867</v>
+        <v>-0.1304860423842069</v>
       </c>
       <c r="J19">
-        <v>0.4958701793394653</v>
+        <v>0.4155624733203104</v>
       </c>
       <c r="K19">
-        <v>0.5351902183551951</v>
+        <v>0.5449871295609625</v>
       </c>
       <c r="L19">
-        <v>-0.3216842361259434</v>
+        <v>-0.2610189723011284</v>
       </c>
       <c r="M19">
-        <v>0.01531596879256969</v>
+        <v>-0.115748703784505</v>
       </c>
       <c r="N19">
         <v>1.980989761816137e-16</v>
@@ -1464,34 +1464,34 @@
         <v>0.1197012848033941</v>
       </c>
       <c r="D20">
-        <v>0.4106640836798853</v>
+        <v>0.4051407095347814</v>
       </c>
       <c r="E20">
-        <v>0.4823668343378171</v>
+        <v>0.4333987620781303</v>
       </c>
       <c r="F20">
-        <v>0.2199901540311984</v>
+        <v>0.2210368374975278</v>
       </c>
       <c r="G20">
-        <v>0.137742416035436</v>
+        <v>0.1992734032194558</v>
       </c>
       <c r="H20">
-        <v>0.4186816217349182</v>
+        <v>0.3933974245641507</v>
       </c>
       <c r="I20">
-        <v>0.3687252251634304</v>
+        <v>0.300194367852684</v>
       </c>
       <c r="J20">
-        <v>0.4970141994262009</v>
+        <v>0.4637893251987291</v>
       </c>
       <c r="K20">
-        <v>0.154882799832345</v>
+        <v>0.2412286367885081</v>
       </c>
       <c r="L20">
-        <v>0.03717555367098489</v>
+        <v>0.1513992691542027</v>
       </c>
       <c r="M20">
-        <v>0.2851228561516467</v>
+        <v>0.2140391375821556</v>
       </c>
       <c r="N20">
         <v>1.410169364536039e-15</v>
@@ -1523,34 +1523,34 @@
         <v>-0.2361543508333692</v>
       </c>
       <c r="D21">
-        <v>-0.2656683744986833</v>
+        <v>-0.3079389633548364</v>
       </c>
       <c r="E21">
-        <v>0.3779016654917939</v>
+        <v>0.3026222090640849</v>
       </c>
       <c r="F21">
-        <v>0.3504819321013322</v>
+        <v>0.3544617503524454</v>
       </c>
       <c r="G21">
-        <v>-0.5556484476426126</v>
+        <v>-0.5436623410446169</v>
       </c>
       <c r="H21">
-        <v>-0.2708700541407726</v>
+        <v>-0.3064871945736838</v>
       </c>
       <c r="I21">
-        <v>-0.2214717228500268</v>
+        <v>-0.306152546074295</v>
       </c>
       <c r="J21">
-        <v>0.242378062837054</v>
+        <v>0.1648409968246075</v>
       </c>
       <c r="K21">
-        <v>0.2765780350478629</v>
+        <v>0.2638080676402369</v>
       </c>
       <c r="L21">
-        <v>-0.2871981951759794</v>
+        <v>-0.3676193604901473</v>
       </c>
       <c r="M21">
-        <v>-0.1633347047067167</v>
+        <v>-0.261741111092062</v>
       </c>
       <c r="N21">
         <v>8.721150744904445e-16</v>

</xml_diff>

<commit_message>
added do_all python codes.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -22,10 +22,13 @@
     <t>VIXCLS</t>
   </si>
   <si>
+    <t>meanMed</t>
+  </si>
+  <si>
     <t>iqrMed</t>
   </si>
   <si>
-    <t>meanMed</t>
+    <t>varMed</t>
   </si>
   <si>
     <t>rmeanMed</t>
@@ -34,22 +37,19 @@
     <t>rvarMed</t>
   </si>
   <si>
-    <t>varMed</t>
+    <t>meanMean</t>
   </si>
   <si>
     <t>iqrMean</t>
   </si>
   <si>
-    <t>meanMean</t>
+    <t>varMean</t>
   </si>
   <si>
     <t>rmeanMean</t>
   </si>
   <si>
     <t>rvarMean</t>
-  </si>
-  <si>
-    <t>varMean</t>
   </si>
   <si>
     <t>kurtEstMed</t>
@@ -510,34 +510,34 @@
         <v>-0.5516119417239891</v>
       </c>
       <c r="D2">
+        <v>-0.2146382865242739</v>
+      </c>
+      <c r="E2">
         <v>-0.1609705267258305</v>
       </c>
-      <c r="E2">
-        <v>-0.2146382865242739</v>
-      </c>
       <c r="F2">
+        <v>-0.1751586568075148</v>
+      </c>
+      <c r="G2">
         <v>-0.2390098332268563</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-0.1318081117631396</v>
       </c>
-      <c r="H2">
-        <v>-0.1751586568075148</v>
-      </c>
       <c r="I2">
+        <v>-0.2442575912937952</v>
+      </c>
+      <c r="J2">
         <v>0.02463671945219919</v>
       </c>
-      <c r="J2">
-        <v>-0.2442575912937952</v>
-      </c>
       <c r="K2">
+        <v>0.0925382074692313</v>
+      </c>
+      <c r="L2">
         <v>-0.2755229145892673</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.009011369349083607</v>
-      </c>
-      <c r="M2">
-        <v>0.0925382074692313</v>
       </c>
       <c r="N2">
         <v>6.055881544898674e-17</v>
@@ -569,34 +569,34 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <v>0.006695480955382251</v>
+      </c>
+      <c r="E3">
         <v>0.09593726714713641</v>
       </c>
-      <c r="E3">
-        <v>0.006695480955382251</v>
-      </c>
       <c r="F3">
+        <v>0.1134940197879655</v>
+      </c>
+      <c r="G3">
         <v>0.1790023632918195</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.236592323055357</v>
       </c>
-      <c r="H3">
-        <v>0.1134940197879655</v>
-      </c>
       <c r="I3">
+        <v>-0.0457566048628302</v>
+      </c>
+      <c r="J3">
         <v>-0.03114961804922891</v>
       </c>
-      <c r="J3">
-        <v>-0.0457566048628302</v>
-      </c>
       <c r="K3">
+        <v>-0.01979505732831893</v>
+      </c>
+      <c r="L3">
         <v>0.142999274089144</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.1737101849475536</v>
-      </c>
-      <c r="M3">
-        <v>-0.01979505732831893</v>
       </c>
       <c r="N3">
         <v>-1.146946634604127e-15</v>
@@ -622,10 +622,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.1609705267258305</v>
+        <v>-0.2146382865242739</v>
       </c>
       <c r="C4">
-        <v>0.09593726714713641</v>
+        <v>0.006695480955382251</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -634,46 +634,46 @@
         <v>0.6468349212578923</v>
       </c>
       <c r="F4">
-        <v>0.1517513741527407</v>
+        <v>0.6672795322378595</v>
       </c>
       <c r="G4">
-        <v>0.8005362249079484</v>
+        <v>0.5872880800836626</v>
       </c>
       <c r="H4">
-        <v>0.992481873816037</v>
+        <v>0.2893474286312728</v>
       </c>
       <c r="I4">
-        <v>0.879975068712724</v>
+        <v>0.9138020468399077</v>
       </c>
       <c r="J4">
-        <v>0.7965766664278233</v>
+        <v>0.5512808457963762</v>
       </c>
       <c r="K4">
-        <v>0.247022406716849</v>
+        <v>0.5140728904674001</v>
       </c>
       <c r="L4">
-        <v>0.6139816498137851</v>
+        <v>0.5629301671802283</v>
       </c>
       <c r="M4">
-        <v>0.7794274091831108</v>
+        <v>0.2737963524037204</v>
       </c>
       <c r="N4">
-        <v>-5.26312476638483e-16</v>
+        <v>-7.810849885615325e-15</v>
       </c>
       <c r="O4">
-        <v>-0.4844866619882676</v>
+        <v>-0.2130141436281778</v>
       </c>
       <c r="R4">
-        <v>-0.03589309818135301</v>
+        <v>-0.280230938060934</v>
       </c>
       <c r="S4">
-        <v>-0.06869523931865897</v>
+        <v>0.5469064887048238</v>
       </c>
       <c r="T4">
-        <v>0.4051407095347814</v>
+        <v>0.4333987620781303</v>
       </c>
       <c r="U4">
-        <v>-0.3079389633548364</v>
+        <v>0.3026222090640849</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -681,10 +681,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.2146382865242739</v>
+        <v>-0.1609705267258305</v>
       </c>
       <c r="C5">
-        <v>0.006695480955382251</v>
+        <v>0.09593726714713641</v>
       </c>
       <c r="D5">
         <v>0.6468349212578923</v>
@@ -693,46 +693,46 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.5872880800836626</v>
+        <v>0.992481873816037</v>
       </c>
       <c r="G5">
-        <v>0.2893474286312728</v>
+        <v>0.1517513741527407</v>
       </c>
       <c r="H5">
-        <v>0.6672795322378595</v>
+        <v>0.8005362249079484</v>
       </c>
       <c r="I5">
-        <v>0.5512808457963762</v>
+        <v>0.7965766664278233</v>
       </c>
       <c r="J5">
-        <v>0.9138020468399077</v>
+        <v>0.879975068712724</v>
       </c>
       <c r="K5">
-        <v>0.5629301671802283</v>
+        <v>0.7794274091831108</v>
       </c>
       <c r="L5">
-        <v>0.2737963524037204</v>
+        <v>0.247022406716849</v>
       </c>
       <c r="M5">
-        <v>0.5140728904674001</v>
+        <v>0.6139816498137851</v>
       </c>
       <c r="N5">
-        <v>-7.810849885615325e-15</v>
+        <v>-5.26312476638483e-16</v>
       </c>
       <c r="O5">
-        <v>-0.2130141436281778</v>
+        <v>-0.4844866619882676</v>
       </c>
       <c r="R5">
-        <v>-0.280230938060934</v>
+        <v>-0.03589309818135301</v>
       </c>
       <c r="S5">
-        <v>0.5469064887048238</v>
+        <v>-0.06869523931865897</v>
       </c>
       <c r="T5">
-        <v>0.4333987620781303</v>
+        <v>0.4051407095347814</v>
       </c>
       <c r="U5">
-        <v>0.3026222090640849</v>
+        <v>-0.3079389633548364</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -740,58 +740,58 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.2390098332268563</v>
+        <v>-0.1751586568075148</v>
       </c>
       <c r="C6">
-        <v>0.1790023632918195</v>
+        <v>0.1134940197879655</v>
       </c>
       <c r="D6">
-        <v>0.1517513741527407</v>
+        <v>0.6672795322378595</v>
       </c>
       <c r="E6">
-        <v>0.5872880800836626</v>
+        <v>0.992481873816037</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>-0.09770875581285839</v>
+        <v>0.1639019505469678</v>
       </c>
       <c r="H6">
-        <v>0.1639019505469678</v>
+        <v>0.7964976254513817</v>
       </c>
       <c r="I6">
-        <v>0.0003716899051861331</v>
+        <v>0.8062050703183056</v>
       </c>
       <c r="J6">
-        <v>0.502855144844632</v>
+        <v>0.8831410516690518</v>
       </c>
       <c r="K6">
-        <v>0.9588684709491565</v>
+        <v>0.7908801559917824</v>
       </c>
       <c r="L6">
-        <v>-0.1493617584562276</v>
+        <v>0.2679550097626913</v>
       </c>
       <c r="M6">
-        <v>-0.006990666893042056</v>
+        <v>0.6081518477431341</v>
       </c>
       <c r="N6">
-        <v>2.57649465002784e-16</v>
+        <v>3.144896282365325e-16</v>
       </c>
       <c r="O6">
-        <v>0.0855701284130547</v>
+        <v>-0.468465924749046</v>
       </c>
       <c r="R6">
-        <v>-0.06116014632225203</v>
+        <v>-0.03594240137942541</v>
       </c>
       <c r="S6">
-        <v>0.6117187837479278</v>
+        <v>-0.06505595629729606</v>
       </c>
       <c r="T6">
-        <v>0.2210368374975278</v>
+        <v>0.3933974245641507</v>
       </c>
       <c r="U6">
-        <v>0.3544617503524454</v>
+        <v>-0.3064871945736838</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -799,58 +799,58 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.1318081117631396</v>
+        <v>-0.2390098332268563</v>
       </c>
       <c r="C7">
-        <v>0.236592323055357</v>
+        <v>0.1790023632918195</v>
       </c>
       <c r="D7">
-        <v>0.8005362249079484</v>
+        <v>0.5872880800836626</v>
       </c>
       <c r="E7">
-        <v>0.2893474286312728</v>
+        <v>0.1517513741527407</v>
       </c>
       <c r="F7">
+        <v>0.1639019505469678</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>-0.09770875581285839</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0.7964976254513817</v>
-      </c>
       <c r="I7">
-        <v>0.8108052446228973</v>
+        <v>0.502855144844632</v>
       </c>
       <c r="J7">
-        <v>0.4938463860778851</v>
+        <v>0.0003716899051861331</v>
       </c>
       <c r="K7">
-        <v>-0.02856147293314673</v>
+        <v>-0.006990666893042056</v>
       </c>
       <c r="L7">
-        <v>0.7920023106189256</v>
+        <v>0.9588684709491565</v>
       </c>
       <c r="M7">
-        <v>0.719852674429839</v>
+        <v>-0.1493617584562276</v>
       </c>
       <c r="N7">
-        <v>9.535275711450758e-16</v>
+        <v>2.57649465002784e-16</v>
       </c>
       <c r="O7">
-        <v>-0.5470942344968723</v>
+        <v>0.0855701284130547</v>
       </c>
       <c r="R7">
-        <v>0.1608069006810534</v>
+        <v>-0.06116014632225203</v>
       </c>
       <c r="S7">
-        <v>-0.4059303727331163</v>
+        <v>0.6117187837479278</v>
       </c>
       <c r="T7">
-        <v>0.1992734032194558</v>
+        <v>0.2210368374975278</v>
       </c>
       <c r="U7">
-        <v>-0.5436623410446169</v>
+        <v>0.3544617503524454</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -858,58 +858,58 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.1751586568075148</v>
+        <v>-0.1318081117631396</v>
       </c>
       <c r="C8">
-        <v>0.1134940197879655</v>
+        <v>0.236592323055357</v>
       </c>
       <c r="D8">
-        <v>0.992481873816037</v>
+        <v>0.2893474286312728</v>
       </c>
       <c r="E8">
-        <v>0.6672795322378595</v>
+        <v>0.8005362249079484</v>
       </c>
       <c r="F8">
-        <v>0.1639019505469678</v>
+        <v>0.7964976254513817</v>
       </c>
       <c r="G8">
-        <v>0.7964976254513817</v>
+        <v>-0.09770875581285839</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.8831410516690518</v>
+        <v>0.4938463860778851</v>
       </c>
       <c r="J8">
-        <v>0.8062050703183056</v>
+        <v>0.8108052446228973</v>
       </c>
       <c r="K8">
-        <v>0.2679550097626913</v>
+        <v>0.719852674429839</v>
       </c>
       <c r="L8">
-        <v>0.6081518477431341</v>
+        <v>-0.02856147293314673</v>
       </c>
       <c r="M8">
-        <v>0.7908801559917824</v>
+        <v>0.7920023106189256</v>
       </c>
       <c r="N8">
-        <v>3.144896282365325e-16</v>
+        <v>9.535275711450758e-16</v>
       </c>
       <c r="O8">
-        <v>-0.468465924749046</v>
+        <v>-0.5470942344968723</v>
       </c>
       <c r="R8">
-        <v>-0.03594240137942541</v>
+        <v>0.1608069006810534</v>
       </c>
       <c r="S8">
-        <v>-0.06505595629729606</v>
+        <v>-0.4059303727331163</v>
       </c>
       <c r="T8">
-        <v>0.3933974245641507</v>
+        <v>0.1992734032194558</v>
       </c>
       <c r="U8">
-        <v>-0.3064871945736838</v>
+        <v>-0.5436623410446169</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -917,25 +917,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.02463671945219919</v>
+        <v>-0.2442575912937952</v>
       </c>
       <c r="C9">
-        <v>-0.03114961804922891</v>
+        <v>-0.0457566048628302</v>
       </c>
       <c r="D9">
-        <v>0.879975068712724</v>
+        <v>0.9138020468399077</v>
       </c>
       <c r="E9">
-        <v>0.5512808457963762</v>
+        <v>0.7965766664278233</v>
       </c>
       <c r="F9">
-        <v>0.0003716899051861331</v>
+        <v>0.8062050703183056</v>
       </c>
       <c r="G9">
-        <v>0.8108052446228973</v>
+        <v>0.502855144844632</v>
       </c>
       <c r="H9">
-        <v>0.8831410516690518</v>
+        <v>0.4938463860778851</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -944,31 +944,31 @@
         <v>0.7085765328289897</v>
       </c>
       <c r="K9">
-        <v>0.07508672573744717</v>
+        <v>0.6266383697311377</v>
       </c>
       <c r="L9">
-        <v>0.7775634838244121</v>
+        <v>0.55554696291363</v>
       </c>
       <c r="M9">
-        <v>0.9678760915982535</v>
+        <v>0.3727458451678964</v>
       </c>
       <c r="N9">
-        <v>8.12849579998413e-15</v>
+        <v>5.597603306782835e-15</v>
       </c>
       <c r="O9">
-        <v>-0.5546927522474058</v>
+        <v>-0.2970439799879107</v>
       </c>
       <c r="R9">
-        <v>-0.2162934290481094</v>
+        <v>-0.2043475672720929</v>
       </c>
       <c r="S9">
-        <v>-0.1304860423842069</v>
+        <v>0.4155624733203104</v>
       </c>
       <c r="T9">
-        <v>0.300194367852684</v>
+        <v>0.4637893251987291</v>
       </c>
       <c r="U9">
-        <v>-0.306152546074295</v>
+        <v>0.1648409968246075</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -976,25 +976,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.2442575912937952</v>
+        <v>0.02463671945219919</v>
       </c>
       <c r="C10">
-        <v>-0.0457566048628302</v>
+        <v>-0.03114961804922891</v>
       </c>
       <c r="D10">
-        <v>0.7965766664278233</v>
+        <v>0.5512808457963762</v>
       </c>
       <c r="E10">
-        <v>0.9138020468399077</v>
+        <v>0.879975068712724</v>
       </c>
       <c r="F10">
-        <v>0.502855144844632</v>
+        <v>0.8831410516690518</v>
       </c>
       <c r="G10">
-        <v>0.4938463860778851</v>
+        <v>0.0003716899051861331</v>
       </c>
       <c r="H10">
-        <v>0.8062050703183056</v>
+        <v>0.8108052446228973</v>
       </c>
       <c r="I10">
         <v>0.7085765328289897</v>
@@ -1003,31 +1003,31 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.55554696291363</v>
+        <v>0.9678760915982535</v>
       </c>
       <c r="L10">
-        <v>0.3727458451678964</v>
+        <v>0.07508672573744717</v>
       </c>
       <c r="M10">
-        <v>0.6266383697311377</v>
+        <v>0.7775634838244121</v>
       </c>
       <c r="N10">
-        <v>5.597603306782835e-15</v>
+        <v>8.12849579998413e-15</v>
       </c>
       <c r="O10">
-        <v>-0.2970439799879107</v>
+        <v>-0.5546927522474058</v>
       </c>
       <c r="R10">
-        <v>-0.2043475672720929</v>
+        <v>-0.2162934290481094</v>
       </c>
       <c r="S10">
-        <v>0.4155624733203104</v>
+        <v>-0.1304860423842069</v>
       </c>
       <c r="T10">
-        <v>0.4637893251987291</v>
+        <v>0.300194367852684</v>
       </c>
       <c r="U10">
-        <v>0.1648409968246075</v>
+        <v>-0.306152546074295</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1035,58 +1035,58 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.2755229145892673</v>
+        <v>0.0925382074692313</v>
       </c>
       <c r="C11">
-        <v>0.142999274089144</v>
+        <v>-0.01979505732831893</v>
       </c>
       <c r="D11">
-        <v>0.247022406716849</v>
+        <v>0.5140728904674001</v>
       </c>
       <c r="E11">
-        <v>0.5629301671802283</v>
+        <v>0.7794274091831108</v>
       </c>
       <c r="F11">
-        <v>0.9588684709491565</v>
+        <v>0.7908801559917824</v>
       </c>
       <c r="G11">
-        <v>-0.02856147293314673</v>
+        <v>-0.006990666893042056</v>
       </c>
       <c r="H11">
-        <v>0.2679550097626913</v>
+        <v>0.719852674429839</v>
       </c>
       <c r="I11">
-        <v>0.07508672573744717</v>
+        <v>0.6266383697311377</v>
       </c>
       <c r="J11">
-        <v>0.55554696291363</v>
+        <v>0.9678760915982535</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>-0.1697350189515449</v>
+        <v>0.04463684494335034</v>
       </c>
       <c r="M11">
-        <v>0.04463684494335034</v>
+        <v>0.7920607960994264</v>
       </c>
       <c r="N11">
-        <v>-3.663853772685152e-17</v>
+        <v>-1.202197081870329e-16</v>
       </c>
       <c r="O11">
-        <v>0.1048326526071779</v>
+        <v>-0.5644056674894997</v>
       </c>
       <c r="R11">
-        <v>-0.02022194646378487</v>
+        <v>-0.2804808943433733</v>
       </c>
       <c r="S11">
-        <v>0.5449871295609625</v>
+        <v>-0.115748703784505</v>
       </c>
       <c r="T11">
-        <v>0.2412286367885081</v>
+        <v>0.2140391375821556</v>
       </c>
       <c r="U11">
-        <v>0.2638080676402369</v>
+        <v>-0.261741111092062</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1094,58 +1094,58 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.009011369349083607</v>
+        <v>-0.2755229145892673</v>
       </c>
       <c r="C12">
-        <v>0.1737101849475536</v>
+        <v>0.142999274089144</v>
       </c>
       <c r="D12">
-        <v>0.6139816498137851</v>
+        <v>0.5629301671802283</v>
       </c>
       <c r="E12">
-        <v>0.2737963524037204</v>
+        <v>0.247022406716849</v>
       </c>
       <c r="F12">
-        <v>-0.1493617584562276</v>
+        <v>0.2679550097626913</v>
       </c>
       <c r="G12">
-        <v>0.7920023106189256</v>
+        <v>0.9588684709491565</v>
       </c>
       <c r="H12">
-        <v>0.6081518477431341</v>
+        <v>-0.02856147293314673</v>
       </c>
       <c r="I12">
-        <v>0.7775634838244121</v>
+        <v>0.55554696291363</v>
       </c>
       <c r="J12">
-        <v>0.3727458451678964</v>
+        <v>0.07508672573744717</v>
       </c>
       <c r="K12">
+        <v>0.04463684494335034</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>-0.1697350189515449</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0.7920607960994264</v>
-      </c>
       <c r="N12">
-        <v>-6.417188599869865e-15</v>
+        <v>-3.663853772685152e-17</v>
       </c>
       <c r="O12">
-        <v>-0.4530916816463709</v>
+        <v>0.1048326526071779</v>
       </c>
       <c r="R12">
-        <v>-0.1030604501630649</v>
+        <v>-0.02022194646378487</v>
       </c>
       <c r="S12">
-        <v>-0.2610189723011284</v>
+        <v>0.5449871295609625</v>
       </c>
       <c r="T12">
-        <v>0.1513992691542027</v>
+        <v>0.2412286367885081</v>
       </c>
       <c r="U12">
-        <v>-0.3676193604901473</v>
+        <v>0.2638080676402369</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1153,58 +1153,58 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.0925382074692313</v>
+        <v>0.009011369349083607</v>
       </c>
       <c r="C13">
-        <v>-0.01979505732831893</v>
+        <v>0.1737101849475536</v>
       </c>
       <c r="D13">
-        <v>0.7794274091831108</v>
+        <v>0.2737963524037204</v>
       </c>
       <c r="E13">
-        <v>0.5140728904674001</v>
+        <v>0.6139816498137851</v>
       </c>
       <c r="F13">
-        <v>-0.006990666893042056</v>
+        <v>0.6081518477431341</v>
       </c>
       <c r="G13">
-        <v>0.719852674429839</v>
+        <v>-0.1493617584562276</v>
       </c>
       <c r="H13">
-        <v>0.7908801559917824</v>
+        <v>0.7920023106189256</v>
       </c>
       <c r="I13">
-        <v>0.9678760915982535</v>
+        <v>0.3727458451678964</v>
       </c>
       <c r="J13">
-        <v>0.6266383697311377</v>
+        <v>0.7775634838244121</v>
       </c>
       <c r="K13">
-        <v>0.04463684494335034</v>
+        <v>0.7920607960994264</v>
       </c>
       <c r="L13">
-        <v>0.7920607960994264</v>
+        <v>-0.1697350189515449</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-1.202197081870329e-16</v>
+        <v>-6.417188599869865e-15</v>
       </c>
       <c r="O13">
-        <v>-0.5644056674894997</v>
+        <v>-0.4530916816463709</v>
       </c>
       <c r="R13">
-        <v>-0.2804808943433733</v>
+        <v>-0.1030604501630649</v>
       </c>
       <c r="S13">
-        <v>-0.115748703784505</v>
+        <v>-0.2610189723011284</v>
       </c>
       <c r="T13">
-        <v>0.2140391375821556</v>
+        <v>0.1513992691542027</v>
       </c>
       <c r="U13">
-        <v>-0.261741111092062</v>
+        <v>-0.3676193604901473</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1218,34 +1218,34 @@
         <v>-1.146946634604127e-15</v>
       </c>
       <c r="D14">
+        <v>-7.810849885615325e-15</v>
+      </c>
+      <c r="E14">
         <v>-5.26312476638483e-16</v>
       </c>
-      <c r="E14">
-        <v>-7.810849885615325e-15</v>
-      </c>
       <c r="F14">
+        <v>3.144896282365325e-16</v>
+      </c>
+      <c r="G14">
         <v>2.57649465002784e-16</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>9.535275711450758e-16</v>
       </c>
-      <c r="H14">
-        <v>3.144896282365325e-16</v>
-      </c>
       <c r="I14">
+        <v>5.597603306782835e-15</v>
+      </c>
+      <c r="J14">
         <v>8.12849579998413e-15</v>
       </c>
-      <c r="J14">
-        <v>5.597603306782835e-15</v>
-      </c>
       <c r="K14">
+        <v>-1.202197081870329e-16</v>
+      </c>
+      <c r="L14">
         <v>-3.663853772685152e-17</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>-6.417188599869865e-15</v>
-      </c>
-      <c r="M14">
-        <v>-1.202197081870329e-16</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1277,34 +1277,34 @@
         <v>-0.1028537241709977</v>
       </c>
       <c r="D15">
+        <v>-0.2130141436281778</v>
+      </c>
+      <c r="E15">
         <v>-0.4844866619882676</v>
       </c>
-      <c r="E15">
-        <v>-0.2130141436281778</v>
-      </c>
       <c r="F15">
+        <v>-0.468465924749046</v>
+      </c>
+      <c r="G15">
         <v>0.0855701284130547</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>-0.5470942344968723</v>
       </c>
-      <c r="H15">
-        <v>-0.468465924749046</v>
-      </c>
       <c r="I15">
+        <v>-0.2970439799879107</v>
+      </c>
+      <c r="J15">
         <v>-0.5546927522474058</v>
       </c>
-      <c r="J15">
-        <v>-0.2970439799879107</v>
-      </c>
       <c r="K15">
+        <v>-0.5644056674894997</v>
+      </c>
+      <c r="L15">
         <v>0.1048326526071779</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>-0.4530916816463709</v>
-      </c>
-      <c r="M15">
-        <v>-0.5644056674894997</v>
       </c>
       <c r="N15">
         <v>4.469207541101161e-15</v>
@@ -1346,34 +1346,34 @@
         <v>0.3724832149705329</v>
       </c>
       <c r="D18">
+        <v>-0.280230938060934</v>
+      </c>
+      <c r="E18">
         <v>-0.03589309818135301</v>
       </c>
-      <c r="E18">
-        <v>-0.280230938060934</v>
-      </c>
       <c r="F18">
+        <v>-0.03594240137942541</v>
+      </c>
+      <c r="G18">
         <v>-0.06116014632225203</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.1608069006810534</v>
       </c>
-      <c r="H18">
-        <v>-0.03594240137942541</v>
-      </c>
       <c r="I18">
+        <v>-0.2043475672720929</v>
+      </c>
+      <c r="J18">
         <v>-0.2162934290481094</v>
       </c>
-      <c r="J18">
-        <v>-0.2043475672720929</v>
-      </c>
       <c r="K18">
+        <v>-0.2804808943433733</v>
+      </c>
+      <c r="L18">
         <v>-0.02022194646378487</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>-0.1030604501630649</v>
-      </c>
-      <c r="M18">
-        <v>-0.2804808943433733</v>
       </c>
       <c r="N18">
         <v>2.7795804443586e-15</v>
@@ -1405,34 +1405,34 @@
         <v>-0.2206076074987401</v>
       </c>
       <c r="D19">
+        <v>0.5469064887048238</v>
+      </c>
+      <c r="E19">
         <v>-0.06869523931865897</v>
       </c>
-      <c r="E19">
-        <v>0.5469064887048238</v>
-      </c>
       <c r="F19">
+        <v>-0.06505595629729606</v>
+      </c>
+      <c r="G19">
         <v>0.6117187837479278</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>-0.4059303727331163</v>
       </c>
-      <c r="H19">
-        <v>-0.06505595629729606</v>
-      </c>
       <c r="I19">
+        <v>0.4155624733203104</v>
+      </c>
+      <c r="J19">
         <v>-0.1304860423842069</v>
       </c>
-      <c r="J19">
-        <v>0.4155624733203104</v>
-      </c>
       <c r="K19">
+        <v>-0.115748703784505</v>
+      </c>
+      <c r="L19">
         <v>0.5449871295609625</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>-0.2610189723011284</v>
-      </c>
-      <c r="M19">
-        <v>-0.115748703784505</v>
       </c>
       <c r="N19">
         <v>1.980989761816137e-16</v>
@@ -1464,34 +1464,34 @@
         <v>0.1197012848033941</v>
       </c>
       <c r="D20">
+        <v>0.4333987620781303</v>
+      </c>
+      <c r="E20">
         <v>0.4051407095347814</v>
       </c>
-      <c r="E20">
-        <v>0.4333987620781303</v>
-      </c>
       <c r="F20">
+        <v>0.3933974245641507</v>
+      </c>
+      <c r="G20">
         <v>0.2210368374975278</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>0.1992734032194558</v>
       </c>
-      <c r="H20">
-        <v>0.3933974245641507</v>
-      </c>
       <c r="I20">
+        <v>0.4637893251987291</v>
+      </c>
+      <c r="J20">
         <v>0.300194367852684</v>
       </c>
-      <c r="J20">
-        <v>0.4637893251987291</v>
-      </c>
       <c r="K20">
+        <v>0.2140391375821556</v>
+      </c>
+      <c r="L20">
         <v>0.2412286367885081</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>0.1513992691542027</v>
-      </c>
-      <c r="M20">
-        <v>0.2140391375821556</v>
       </c>
       <c r="N20">
         <v>1.410169364536039e-15</v>
@@ -1523,34 +1523,34 @@
         <v>-0.2361543508333692</v>
       </c>
       <c r="D21">
+        <v>0.3026222090640849</v>
+      </c>
+      <c r="E21">
         <v>-0.3079389633548364</v>
       </c>
-      <c r="E21">
-        <v>0.3026222090640849</v>
-      </c>
       <c r="F21">
+        <v>-0.3064871945736838</v>
+      </c>
+      <c r="G21">
         <v>0.3544617503524454</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>-0.5436623410446169</v>
       </c>
-      <c r="H21">
-        <v>-0.3064871945736838</v>
-      </c>
       <c r="I21">
+        <v>0.1648409968246075</v>
+      </c>
+      <c r="J21">
         <v>-0.306152546074295</v>
       </c>
-      <c r="J21">
-        <v>0.1648409968246075</v>
-      </c>
       <c r="K21">
+        <v>-0.261741111092062</v>
+      </c>
+      <c r="L21">
         <v>0.2638080676402369</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>-0.3676193604901473</v>
-      </c>
-      <c r="M21">
-        <v>-0.261741111092062</v>
       </c>
       <c r="N21">
         <v>8.721150744904445e-16</v>

</xml_diff>

<commit_message>
added a folder for the draft of the slides of presentation on march 30.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -510,34 +510,34 @@
         <v>-0.5516119417239891</v>
       </c>
       <c r="D2">
-        <v>-0.2146382865242739</v>
+        <v>-0.2100097071880278</v>
       </c>
       <c r="E2">
-        <v>-0.1609705267258305</v>
+        <v>-0.1397562947531871</v>
       </c>
       <c r="F2">
-        <v>-0.1751586568075148</v>
+        <v>-0.1350151204931508</v>
       </c>
       <c r="G2">
-        <v>-0.2390098332268563</v>
+        <v>-0.2423937982455314</v>
       </c>
       <c r="H2">
-        <v>-0.1318081117631396</v>
+        <v>-0.1237654066428298</v>
       </c>
       <c r="I2">
-        <v>-0.2442575912937952</v>
+        <v>-0.2139266899315793</v>
       </c>
       <c r="J2">
-        <v>0.02463671945219919</v>
+        <v>0.04865741612991594</v>
       </c>
       <c r="K2">
-        <v>0.0925382074692313</v>
+        <v>0.109217188323338</v>
       </c>
       <c r="L2">
-        <v>-0.2755229145892673</v>
+        <v>-0.2641546473894593</v>
       </c>
       <c r="M2">
-        <v>0.009011369349083607</v>
+        <v>0.01962844121283543</v>
       </c>
       <c r="N2">
         <v>6.055881544898674e-17</v>
@@ -569,34 +569,34 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.006695480955382251</v>
+        <v>-0.01509990977053945</v>
       </c>
       <c r="E3">
-        <v>0.09593726714713641</v>
+        <v>0.08162223061345381</v>
       </c>
       <c r="F3">
-        <v>0.1134940197879655</v>
+        <v>0.08730196051608709</v>
       </c>
       <c r="G3">
-        <v>0.1790023632918195</v>
+        <v>0.1770781441752131</v>
       </c>
       <c r="H3">
-        <v>0.236592323055357</v>
+        <v>0.1997201598806487</v>
       </c>
       <c r="I3">
-        <v>-0.0457566048628302</v>
+        <v>-0.0873917012978082</v>
       </c>
       <c r="J3">
-        <v>-0.03114961804922891</v>
+        <v>-0.06407932926335395</v>
       </c>
       <c r="K3">
-        <v>-0.01979505732831893</v>
+        <v>-0.04380620175755993</v>
       </c>
       <c r="L3">
-        <v>0.142999274089144</v>
+        <v>0.1332748837988889</v>
       </c>
       <c r="M3">
-        <v>0.1737101849475536</v>
+        <v>0.1533272690361234</v>
       </c>
       <c r="N3">
         <v>-1.146946634604127e-15</v>
@@ -622,58 +622,58 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.2146382865242739</v>
+        <v>-0.2100097071880278</v>
       </c>
       <c r="C4">
-        <v>0.006695480955382251</v>
+        <v>-0.01509990977053945</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.6468349212578923</v>
+        <v>0.6015365415393672</v>
       </c>
       <c r="F4">
-        <v>0.6672795322378595</v>
+        <v>0.622839780508571</v>
       </c>
       <c r="G4">
-        <v>0.5872880800836626</v>
+        <v>0.6052692578710602</v>
       </c>
       <c r="H4">
-        <v>0.2893474286312728</v>
+        <v>0.3043785453484635</v>
       </c>
       <c r="I4">
-        <v>0.9138020468399077</v>
+        <v>0.9089834684659657</v>
       </c>
       <c r="J4">
-        <v>0.5512808457963762</v>
+        <v>0.5539968224811245</v>
       </c>
       <c r="K4">
-        <v>0.5140728904674001</v>
+        <v>0.52576023735489</v>
       </c>
       <c r="L4">
-        <v>0.5629301671802283</v>
+        <v>0.5646147259402614</v>
       </c>
       <c r="M4">
-        <v>0.2737963524037204</v>
+        <v>0.2943428061408312</v>
       </c>
       <c r="N4">
-        <v>-7.810849885615325e-15</v>
+        <v>-2.920454072657055e-15</v>
       </c>
       <c r="O4">
-        <v>-0.2130141436281778</v>
+        <v>-0.2044140082319981</v>
       </c>
       <c r="R4">
-        <v>-0.280230938060934</v>
+        <v>-0.2806621929417707</v>
       </c>
       <c r="S4">
-        <v>0.5469064887048238</v>
+        <v>0.563808953974267</v>
       </c>
       <c r="T4">
-        <v>0.4333987620781303</v>
+        <v>0.4401659758900596</v>
       </c>
       <c r="U4">
-        <v>0.3026222090640849</v>
+        <v>0.3157102365176738</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -681,58 +681,58 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.1609705267258305</v>
+        <v>-0.1397562947531871</v>
       </c>
       <c r="C5">
-        <v>0.09593726714713641</v>
+        <v>0.08162223061345381</v>
       </c>
       <c r="D5">
-        <v>0.6468349212578923</v>
+        <v>0.6015365415393672</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.992481873816037</v>
+        <v>0.9900306049985805</v>
       </c>
       <c r="G5">
-        <v>0.1517513741527407</v>
+        <v>0.1257176556239894</v>
       </c>
       <c r="H5">
-        <v>0.8005362249079484</v>
+        <v>0.8177480993505468</v>
       </c>
       <c r="I5">
-        <v>0.7965766664278233</v>
+        <v>0.7676081924089456</v>
       </c>
       <c r="J5">
-        <v>0.879975068712724</v>
+        <v>0.8777559965761299</v>
       </c>
       <c r="K5">
-        <v>0.7794274091831108</v>
+        <v>0.7745478205579475</v>
       </c>
       <c r="L5">
-        <v>0.247022406716849</v>
+        <v>0.2102515205998472</v>
       </c>
       <c r="M5">
-        <v>0.6139816498137851</v>
+        <v>0.607083010218251</v>
       </c>
       <c r="N5">
-        <v>-5.26312476638483e-16</v>
+        <v>3.336680005718555e-15</v>
       </c>
       <c r="O5">
-        <v>-0.4844866619882676</v>
+        <v>-0.4942361054572194</v>
       </c>
       <c r="R5">
-        <v>-0.03589309818135301</v>
+        <v>-0.042330879022222</v>
       </c>
       <c r="S5">
-        <v>-0.06869523931865897</v>
+        <v>-0.1172357904798116</v>
       </c>
       <c r="T5">
-        <v>0.4051407095347814</v>
+        <v>0.3925835194979616</v>
       </c>
       <c r="U5">
-        <v>-0.3079389633548364</v>
+        <v>-0.3500317328095502</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -740,58 +740,58 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.1751586568075148</v>
+        <v>-0.1350151204931508</v>
       </c>
       <c r="C6">
-        <v>0.1134940197879655</v>
+        <v>0.08730196051608709</v>
       </c>
       <c r="D6">
-        <v>0.6672795322378595</v>
+        <v>0.622839780508571</v>
       </c>
       <c r="E6">
-        <v>0.992481873816037</v>
+        <v>0.9900306049985805</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.1639019505469678</v>
+        <v>0.1369577931509407</v>
       </c>
       <c r="H6">
-        <v>0.7964976254513817</v>
+        <v>0.8322900178196406</v>
       </c>
       <c r="I6">
-        <v>0.8062050703183056</v>
+        <v>0.7825289384836726</v>
       </c>
       <c r="J6">
-        <v>0.8831410516690518</v>
+        <v>0.8959704693059219</v>
       </c>
       <c r="K6">
-        <v>0.7908801559917824</v>
+        <v>0.8039190036363218</v>
       </c>
       <c r="L6">
-        <v>0.2679550097626913</v>
+        <v>0.2290172208916044</v>
       </c>
       <c r="M6">
-        <v>0.6081518477431341</v>
+        <v>0.6212141847421688</v>
       </c>
       <c r="N6">
-        <v>3.144896282365325e-16</v>
+        <v>7.666083750325158e-16</v>
       </c>
       <c r="O6">
-        <v>-0.468465924749046</v>
+        <v>-0.487397570104229</v>
       </c>
       <c r="R6">
-        <v>-0.03594240137942541</v>
+        <v>-0.03211179235540852</v>
       </c>
       <c r="S6">
-        <v>-0.06505595629729606</v>
+        <v>-0.1002609806753609</v>
       </c>
       <c r="T6">
-        <v>0.3933974245641507</v>
+        <v>0.3640726428403179</v>
       </c>
       <c r="U6">
-        <v>-0.3064871945736838</v>
+        <v>-0.33213038900801</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -799,58 +799,58 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.2390098332268563</v>
+        <v>-0.2423937982455314</v>
       </c>
       <c r="C7">
-        <v>0.1790023632918195</v>
+        <v>0.1770781441752131</v>
       </c>
       <c r="D7">
-        <v>0.5872880800836626</v>
+        <v>0.6052692578710602</v>
       </c>
       <c r="E7">
-        <v>0.1517513741527407</v>
+        <v>0.1257176556239894</v>
       </c>
       <c r="F7">
-        <v>0.1639019505469678</v>
+        <v>0.1369577931509407</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>-0.09770875581285839</v>
+        <v>-0.0827955260901168</v>
       </c>
       <c r="I7">
-        <v>0.502855144844632</v>
+        <v>0.4895566543418153</v>
       </c>
       <c r="J7">
-        <v>0.0003716899051861331</v>
+        <v>0.006393420111500975</v>
       </c>
       <c r="K7">
-        <v>-0.006990666893042056</v>
+        <v>0.01793778858604152</v>
       </c>
       <c r="L7">
-        <v>0.9588684709491565</v>
+        <v>0.9586818989706541</v>
       </c>
       <c r="M7">
-        <v>-0.1493617584562276</v>
+        <v>-0.1173559079185561</v>
       </c>
       <c r="N7">
-        <v>2.57649465002784e-16</v>
+        <v>2.041337486133197e-16</v>
       </c>
       <c r="O7">
-        <v>0.0855701284130547</v>
+        <v>0.09051725814192106</v>
       </c>
       <c r="R7">
-        <v>-0.06116014632225203</v>
+        <v>-0.0687034405025222</v>
       </c>
       <c r="S7">
-        <v>0.6117187837479278</v>
+        <v>0.6193672897256314</v>
       </c>
       <c r="T7">
-        <v>0.2210368374975278</v>
+        <v>0.2438475521930638</v>
       </c>
       <c r="U7">
-        <v>0.3544617503524454</v>
+        <v>0.3593642545909256</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -858,58 +858,58 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.1318081117631396</v>
+        <v>-0.1237654066428298</v>
       </c>
       <c r="C8">
-        <v>0.236592323055357</v>
+        <v>0.1997201598806487</v>
       </c>
       <c r="D8">
-        <v>0.2893474286312728</v>
+        <v>0.3043785453484635</v>
       </c>
       <c r="E8">
-        <v>0.8005362249079484</v>
+        <v>0.8177480993505468</v>
       </c>
       <c r="F8">
-        <v>0.7964976254513817</v>
+        <v>0.8322900178196406</v>
       </c>
       <c r="G8">
-        <v>-0.09770875581285839</v>
+        <v>-0.0827955260901168</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.4938463860778851</v>
+        <v>0.5183839700041073</v>
       </c>
       <c r="J8">
-        <v>0.8108052446228973</v>
+        <v>0.8143982873320751</v>
       </c>
       <c r="K8">
-        <v>0.719852674429839</v>
+        <v>0.7161035345579564</v>
       </c>
       <c r="L8">
-        <v>-0.02856147293314673</v>
+        <v>-0.01930103596191794</v>
       </c>
       <c r="M8">
-        <v>0.7920023106189256</v>
+        <v>0.778931576145244</v>
       </c>
       <c r="N8">
-        <v>9.535275711450758e-16</v>
+        <v>-6.631039802115322e-16</v>
       </c>
       <c r="O8">
-        <v>-0.5470942344968723</v>
+        <v>-0.5516707609764604</v>
       </c>
       <c r="R8">
-        <v>0.1608069006810534</v>
+        <v>0.1490765808683637</v>
       </c>
       <c r="S8">
-        <v>-0.4059303727331163</v>
+        <v>-0.3819145055213614</v>
       </c>
       <c r="T8">
-        <v>0.1992734032194558</v>
+        <v>0.1864068206580604</v>
       </c>
       <c r="U8">
-        <v>-0.5436623410446169</v>
+        <v>-0.5215930626895318</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -917,58 +917,58 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.2442575912937952</v>
+        <v>-0.2139266899315793</v>
       </c>
       <c r="C9">
-        <v>-0.0457566048628302</v>
+        <v>-0.0873917012978082</v>
       </c>
       <c r="D9">
-        <v>0.9138020468399077</v>
+        <v>0.9089834684659657</v>
       </c>
       <c r="E9">
-        <v>0.7965766664278233</v>
+        <v>0.7676081924089456</v>
       </c>
       <c r="F9">
-        <v>0.8062050703183056</v>
+        <v>0.7825289384836726</v>
       </c>
       <c r="G9">
-        <v>0.502855144844632</v>
+        <v>0.4895566543418153</v>
       </c>
       <c r="H9">
-        <v>0.4938463860778851</v>
+        <v>0.5183839700041073</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.7085765328289897</v>
+        <v>0.7292238056940705</v>
       </c>
       <c r="K9">
-        <v>0.6266383697311377</v>
+        <v>0.6581600365985067</v>
       </c>
       <c r="L9">
-        <v>0.55554696291363</v>
+        <v>0.5269665846687024</v>
       </c>
       <c r="M9">
-        <v>0.3727458451678964</v>
+        <v>0.4125547930126223</v>
       </c>
       <c r="N9">
-        <v>5.597603306782835e-15</v>
+        <v>7.807518436920194e-16</v>
       </c>
       <c r="O9">
-        <v>-0.2970439799879107</v>
+        <v>-0.3007117501436224</v>
       </c>
       <c r="R9">
-        <v>-0.2043475672720929</v>
+        <v>-0.2181396823853521</v>
       </c>
       <c r="S9">
-        <v>0.4155624733203104</v>
+        <v>0.4226321700395524</v>
       </c>
       <c r="T9">
-        <v>0.4637893251987291</v>
+        <v>0.4603379440818752</v>
       </c>
       <c r="U9">
-        <v>0.1648409968246075</v>
+        <v>0.1740207184735122</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -976,58 +976,58 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.02463671945219919</v>
+        <v>0.04865741612991594</v>
       </c>
       <c r="C10">
-        <v>-0.03114961804922891</v>
+        <v>-0.06407932926335395</v>
       </c>
       <c r="D10">
-        <v>0.5512808457963762</v>
+        <v>0.5539968224811245</v>
       </c>
       <c r="E10">
-        <v>0.879975068712724</v>
+        <v>0.8777559965761299</v>
       </c>
       <c r="F10">
-        <v>0.8831410516690518</v>
+        <v>0.8959704693059219</v>
       </c>
       <c r="G10">
-        <v>0.0003716899051861331</v>
+        <v>0.006393420111500975</v>
       </c>
       <c r="H10">
-        <v>0.8108052446228973</v>
+        <v>0.8143982873320751</v>
       </c>
       <c r="I10">
-        <v>0.7085765328289897</v>
+        <v>0.7292238056940705</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.9678760915982535</v>
+        <v>0.9654431488146151</v>
       </c>
       <c r="L10">
-        <v>0.07508672573744717</v>
+        <v>0.07050475755270486</v>
       </c>
       <c r="M10">
-        <v>0.7775634838244121</v>
+        <v>0.7697349593525429</v>
       </c>
       <c r="N10">
-        <v>8.12849579998413e-15</v>
+        <v>9.948215812580311e-15</v>
       </c>
       <c r="O10">
-        <v>-0.5546927522474058</v>
+        <v>-0.5377701809645062</v>
       </c>
       <c r="R10">
-        <v>-0.2162934290481094</v>
+        <v>-0.2268680819084783</v>
       </c>
       <c r="S10">
-        <v>-0.1304860423842069</v>
+        <v>-0.1195319569650822</v>
       </c>
       <c r="T10">
-        <v>0.300194367852684</v>
+        <v>0.2836745318532706</v>
       </c>
       <c r="U10">
-        <v>-0.306152546074295</v>
+        <v>-0.2919061767525117</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1035,58 +1035,58 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.0925382074692313</v>
+        <v>0.109217188323338</v>
       </c>
       <c r="C11">
-        <v>-0.01979505732831893</v>
+        <v>-0.04380620175755993</v>
       </c>
       <c r="D11">
-        <v>0.5140728904674001</v>
+        <v>0.52576023735489</v>
       </c>
       <c r="E11">
-        <v>0.7794274091831108</v>
+        <v>0.7745478205579475</v>
       </c>
       <c r="F11">
-        <v>0.7908801559917824</v>
+        <v>0.8039190036363218</v>
       </c>
       <c r="G11">
-        <v>-0.006990666893042056</v>
+        <v>0.01793778858604152</v>
       </c>
       <c r="H11">
-        <v>0.719852674429839</v>
+        <v>0.7161035345579564</v>
       </c>
       <c r="I11">
-        <v>0.6266383697311377</v>
+        <v>0.6581600365985067</v>
       </c>
       <c r="J11">
-        <v>0.9678760915982535</v>
+        <v>0.9654431488146151</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.04463684494335034</v>
+        <v>0.0630568220275609</v>
       </c>
       <c r="M11">
-        <v>0.7920607960994264</v>
+        <v>0.7819199761477985</v>
       </c>
       <c r="N11">
-        <v>-1.202197081870329e-16</v>
+        <v>2.136580471001812e-15</v>
       </c>
       <c r="O11">
-        <v>-0.5644056674894997</v>
+        <v>-0.5305931793137654</v>
       </c>
       <c r="R11">
-        <v>-0.2804808943433733</v>
+        <v>-0.2928939929855898</v>
       </c>
       <c r="S11">
-        <v>-0.115748703784505</v>
+        <v>-0.09199152183265459</v>
       </c>
       <c r="T11">
-        <v>0.2140391375821556</v>
+        <v>0.2060365383140566</v>
       </c>
       <c r="U11">
-        <v>-0.261741111092062</v>
+        <v>-0.2405096388005949</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1094,58 +1094,58 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.2755229145892673</v>
+        <v>-0.2641546473894593</v>
       </c>
       <c r="C12">
-        <v>0.142999274089144</v>
+        <v>0.1332748837988889</v>
       </c>
       <c r="D12">
-        <v>0.5629301671802283</v>
+        <v>0.5646147259402614</v>
       </c>
       <c r="E12">
-        <v>0.247022406716849</v>
+        <v>0.2102515205998472</v>
       </c>
       <c r="F12">
-        <v>0.2679550097626913</v>
+        <v>0.2290172208916044</v>
       </c>
       <c r="G12">
-        <v>0.9588684709491565</v>
+        <v>0.9586818989706541</v>
       </c>
       <c r="H12">
-        <v>-0.02856147293314673</v>
+        <v>-0.01930103596191794</v>
       </c>
       <c r="I12">
-        <v>0.55554696291363</v>
+        <v>0.5269665846687024</v>
       </c>
       <c r="J12">
-        <v>0.07508672573744717</v>
+        <v>0.07050475755270486</v>
       </c>
       <c r="K12">
-        <v>0.04463684494335034</v>
+        <v>0.0630568220275609</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>-0.1697350189515449</v>
+        <v>-0.1462537487898222</v>
       </c>
       <c r="N12">
-        <v>-3.663853772685152e-17</v>
+        <v>1.143879312308305e-16</v>
       </c>
       <c r="O12">
-        <v>0.1048326526071779</v>
+        <v>0.1085129844232405</v>
       </c>
       <c r="R12">
-        <v>-0.02022194646378487</v>
+        <v>-0.01903605818527438</v>
       </c>
       <c r="S12">
-        <v>0.5449871295609625</v>
+        <v>0.5471289431832419</v>
       </c>
       <c r="T12">
-        <v>0.2412286367885081</v>
+        <v>0.2467166122058998</v>
       </c>
       <c r="U12">
-        <v>0.2638080676402369</v>
+        <v>0.2641093728914577</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1153,58 +1153,58 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.009011369349083607</v>
+        <v>0.01962844121283543</v>
       </c>
       <c r="C13">
-        <v>0.1737101849475536</v>
+        <v>0.1533272690361234</v>
       </c>
       <c r="D13">
-        <v>0.2737963524037204</v>
+        <v>0.2943428061408312</v>
       </c>
       <c r="E13">
-        <v>0.6139816498137851</v>
+        <v>0.607083010218251</v>
       </c>
       <c r="F13">
-        <v>0.6081518477431341</v>
+        <v>0.6212141847421688</v>
       </c>
       <c r="G13">
-        <v>-0.1493617584562276</v>
+        <v>-0.1173559079185561</v>
       </c>
       <c r="H13">
-        <v>0.7920023106189256</v>
+        <v>0.778931576145244</v>
       </c>
       <c r="I13">
-        <v>0.3727458451678964</v>
+        <v>0.4125547930126223</v>
       </c>
       <c r="J13">
-        <v>0.7775634838244121</v>
+        <v>0.7697349593525429</v>
       </c>
       <c r="K13">
-        <v>0.7920607960994264</v>
+        <v>0.7819199761477985</v>
       </c>
       <c r="L13">
-        <v>-0.1697350189515449</v>
+        <v>-0.1462537487898222</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-6.417188599869865e-15</v>
+        <v>-3.663626190122911e-15</v>
       </c>
       <c r="O13">
-        <v>-0.4530916816463709</v>
+        <v>-0.4190085292392897</v>
       </c>
       <c r="R13">
-        <v>-0.1030604501630649</v>
+        <v>-0.1226664923885096</v>
       </c>
       <c r="S13">
-        <v>-0.2610189723011284</v>
+        <v>-0.2273234080895403</v>
       </c>
       <c r="T13">
-        <v>0.1513992691542027</v>
+        <v>0.1391403236753642</v>
       </c>
       <c r="U13">
-        <v>-0.3676193604901473</v>
+        <v>-0.3333457373732241</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1218,34 +1218,34 @@
         <v>-1.146946634604127e-15</v>
       </c>
       <c r="D14">
-        <v>-7.810849885615325e-15</v>
+        <v>-2.920454072657055e-15</v>
       </c>
       <c r="E14">
-        <v>-5.26312476638483e-16</v>
+        <v>3.336680005718555e-15</v>
       </c>
       <c r="F14">
-        <v>3.144896282365325e-16</v>
+        <v>7.666083750325158e-16</v>
       </c>
       <c r="G14">
-        <v>2.57649465002784e-16</v>
+        <v>2.041337486133197e-16</v>
       </c>
       <c r="H14">
-        <v>9.535275711450758e-16</v>
+        <v>-6.631039802115322e-16</v>
       </c>
       <c r="I14">
-        <v>5.597603306782835e-15</v>
+        <v>7.807518436920194e-16</v>
       </c>
       <c r="J14">
-        <v>8.12849579998413e-15</v>
+        <v>9.948215812580311e-15</v>
       </c>
       <c r="K14">
-        <v>-1.202197081870329e-16</v>
+        <v>2.136580471001812e-15</v>
       </c>
       <c r="L14">
-        <v>-3.663853772685152e-17</v>
+        <v>1.143879312308305e-16</v>
       </c>
       <c r="M14">
-        <v>-6.417188599869865e-15</v>
+        <v>-3.663626190122911e-15</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1277,34 +1277,34 @@
         <v>-0.1028537241709977</v>
       </c>
       <c r="D15">
-        <v>-0.2130141436281778</v>
+        <v>-0.2044140082319981</v>
       </c>
       <c r="E15">
-        <v>-0.4844866619882676</v>
+        <v>-0.4942361054572194</v>
       </c>
       <c r="F15">
-        <v>-0.468465924749046</v>
+        <v>-0.487397570104229</v>
       </c>
       <c r="G15">
-        <v>0.0855701284130547</v>
+        <v>0.09051725814192106</v>
       </c>
       <c r="H15">
-        <v>-0.5470942344968723</v>
+        <v>-0.5516707609764604</v>
       </c>
       <c r="I15">
-        <v>-0.2970439799879107</v>
+        <v>-0.3007117501436224</v>
       </c>
       <c r="J15">
-        <v>-0.5546927522474058</v>
+        <v>-0.5377701809645062</v>
       </c>
       <c r="K15">
-        <v>-0.5644056674894997</v>
+        <v>-0.5305931793137654</v>
       </c>
       <c r="L15">
-        <v>0.1048326526071779</v>
+        <v>0.1085129844232405</v>
       </c>
       <c r="M15">
-        <v>-0.4530916816463709</v>
+        <v>-0.4190085292392897</v>
       </c>
       <c r="N15">
         <v>4.469207541101161e-15</v>
@@ -1346,34 +1346,34 @@
         <v>0.3724832149705329</v>
       </c>
       <c r="D18">
-        <v>-0.280230938060934</v>
+        <v>-0.2806621929417707</v>
       </c>
       <c r="E18">
-        <v>-0.03589309818135301</v>
+        <v>-0.042330879022222</v>
       </c>
       <c r="F18">
-        <v>-0.03594240137942541</v>
+        <v>-0.03211179235540852</v>
       </c>
       <c r="G18">
-        <v>-0.06116014632225203</v>
+        <v>-0.0687034405025222</v>
       </c>
       <c r="H18">
-        <v>0.1608069006810534</v>
+        <v>0.1490765808683637</v>
       </c>
       <c r="I18">
-        <v>-0.2043475672720929</v>
+        <v>-0.2181396823853521</v>
       </c>
       <c r="J18">
-        <v>-0.2162934290481094</v>
+        <v>-0.2268680819084783</v>
       </c>
       <c r="K18">
-        <v>-0.2804808943433733</v>
+        <v>-0.2928939929855898</v>
       </c>
       <c r="L18">
-        <v>-0.02022194646378487</v>
+        <v>-0.01903605818527438</v>
       </c>
       <c r="M18">
-        <v>-0.1030604501630649</v>
+        <v>-0.1226664923885096</v>
       </c>
       <c r="N18">
         <v>2.7795804443586e-15</v>
@@ -1405,34 +1405,34 @@
         <v>-0.2206076074987401</v>
       </c>
       <c r="D19">
-        <v>0.5469064887048238</v>
+        <v>0.563808953974267</v>
       </c>
       <c r="E19">
-        <v>-0.06869523931865897</v>
+        <v>-0.1172357904798116</v>
       </c>
       <c r="F19">
-        <v>-0.06505595629729606</v>
+        <v>-0.1002609806753609</v>
       </c>
       <c r="G19">
-        <v>0.6117187837479278</v>
+        <v>0.6193672897256314</v>
       </c>
       <c r="H19">
-        <v>-0.4059303727331163</v>
+        <v>-0.3819145055213614</v>
       </c>
       <c r="I19">
-        <v>0.4155624733203104</v>
+        <v>0.4226321700395524</v>
       </c>
       <c r="J19">
-        <v>-0.1304860423842069</v>
+        <v>-0.1195319569650822</v>
       </c>
       <c r="K19">
-        <v>-0.115748703784505</v>
+        <v>-0.09199152183265459</v>
       </c>
       <c r="L19">
-        <v>0.5449871295609625</v>
+        <v>0.5471289431832419</v>
       </c>
       <c r="M19">
-        <v>-0.2610189723011284</v>
+        <v>-0.2273234080895403</v>
       </c>
       <c r="N19">
         <v>1.980989761816137e-16</v>
@@ -1464,34 +1464,34 @@
         <v>0.1197012848033941</v>
       </c>
       <c r="D20">
-        <v>0.4333987620781303</v>
+        <v>0.4401659758900596</v>
       </c>
       <c r="E20">
-        <v>0.4051407095347814</v>
+        <v>0.3925835194979616</v>
       </c>
       <c r="F20">
-        <v>0.3933974245641507</v>
+        <v>0.3640726428403179</v>
       </c>
       <c r="G20">
-        <v>0.2210368374975278</v>
+        <v>0.2438475521930638</v>
       </c>
       <c r="H20">
-        <v>0.1992734032194558</v>
+        <v>0.1864068206580604</v>
       </c>
       <c r="I20">
-        <v>0.4637893251987291</v>
+        <v>0.4603379440818752</v>
       </c>
       <c r="J20">
-        <v>0.300194367852684</v>
+        <v>0.2836745318532706</v>
       </c>
       <c r="K20">
-        <v>0.2140391375821556</v>
+        <v>0.2060365383140566</v>
       </c>
       <c r="L20">
-        <v>0.2412286367885081</v>
+        <v>0.2467166122058998</v>
       </c>
       <c r="M20">
-        <v>0.1513992691542027</v>
+        <v>0.1391403236753642</v>
       </c>
       <c r="N20">
         <v>1.410169364536039e-15</v>
@@ -1523,34 +1523,34 @@
         <v>-0.2361543508333692</v>
       </c>
       <c r="D21">
-        <v>0.3026222090640849</v>
+        <v>0.3157102365176738</v>
       </c>
       <c r="E21">
-        <v>-0.3079389633548364</v>
+        <v>-0.3500317328095502</v>
       </c>
       <c r="F21">
-        <v>-0.3064871945736838</v>
+        <v>-0.33213038900801</v>
       </c>
       <c r="G21">
-        <v>0.3544617503524454</v>
+        <v>0.3593642545909256</v>
       </c>
       <c r="H21">
-        <v>-0.5436623410446169</v>
+        <v>-0.5215930626895318</v>
       </c>
       <c r="I21">
-        <v>0.1648409968246075</v>
+        <v>0.1740207184735122</v>
       </c>
       <c r="J21">
-        <v>-0.306152546074295</v>
+        <v>-0.2919061767525117</v>
       </c>
       <c r="K21">
-        <v>-0.261741111092062</v>
+        <v>-0.2405096388005949</v>
       </c>
       <c r="L21">
-        <v>0.2638080676402369</v>
+        <v>0.2641093728914577</v>
       </c>
       <c r="M21">
-        <v>-0.3676193604901473</v>
+        <v>-0.3333457373732241</v>
       </c>
       <c r="N21">
         <v>8.721150744904445e-16</v>

</xml_diff>

<commit_message>
1. slides text draft. 2. updated data till June 2019. sample increases. Reestimate density. 3. draft updated.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -507,55 +507,58 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.5516119417239891</v>
+        <v>-0.5607082011729043</v>
       </c>
       <c r="D2">
-        <v>-0.2100097071880278</v>
+        <v>-0.08028107925293226</v>
       </c>
       <c r="E2">
-        <v>-0.1397562947531871</v>
+        <v>-0.06451676150671957</v>
       </c>
       <c r="F2">
-        <v>-0.1350151204931508</v>
+        <v>-0.05591325661825367</v>
       </c>
       <c r="G2">
-        <v>-0.2423937982455314</v>
+        <v>-0.1289602411770273</v>
       </c>
       <c r="H2">
-        <v>-0.1237654066428298</v>
+        <v>-0.08107859177575918</v>
       </c>
       <c r="I2">
-        <v>-0.2139266899315793</v>
+        <v>-0.1336208874169375</v>
       </c>
       <c r="J2">
-        <v>0.04865741612991594</v>
+        <v>0.1212748770636073</v>
       </c>
       <c r="K2">
-        <v>0.109217188323338</v>
+        <v>0.1669514769051775</v>
       </c>
       <c r="L2">
-        <v>-0.2641546473894593</v>
+        <v>-0.1580570607631968</v>
       </c>
       <c r="M2">
-        <v>0.01962844121283543</v>
+        <v>0.03604911749963439</v>
       </c>
       <c r="N2">
-        <v>6.055881544898674e-17</v>
+        <v>-1.087096885153984e-16</v>
       </c>
       <c r="O2">
-        <v>0.0888815068024154</v>
+        <v>-0.1853868407917172</v>
+      </c>
+      <c r="Q2">
+        <v>0.0424264846503711</v>
       </c>
       <c r="R2">
-        <v>-0.1785047152953003</v>
+        <v>-0.2845345830205061</v>
       </c>
       <c r="S2">
-        <v>-0.1254907045969606</v>
+        <v>-0.1355720031208364</v>
       </c>
       <c r="T2">
-        <v>-0.3184960359875938</v>
+        <v>-0.3204245567604783</v>
       </c>
       <c r="U2">
-        <v>-0.06978520298733354</v>
+        <v>-0.05011482699256612</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -563,58 +566,61 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.5516119417239891</v>
+        <v>-0.5607082011729043</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>-0.01509990977053945</v>
+        <v>0.01759041093037989</v>
       </c>
       <c r="E3">
-        <v>0.08162223061345381</v>
+        <v>-0.0389481114345613</v>
       </c>
       <c r="F3">
-        <v>0.08730196051608709</v>
+        <v>-0.04520710184843514</v>
       </c>
       <c r="G3">
-        <v>0.1770781441752131</v>
+        <v>0.17154646284977</v>
       </c>
       <c r="H3">
-        <v>0.1997201598806487</v>
+        <v>0.01769585812541223</v>
       </c>
       <c r="I3">
-        <v>-0.0873917012978082</v>
+        <v>-0.09550244895406114</v>
       </c>
       <c r="J3">
-        <v>-0.06407932926335395</v>
+        <v>-0.1728841612412639</v>
       </c>
       <c r="K3">
-        <v>-0.04380620175755993</v>
+        <v>-0.1510466670382437</v>
       </c>
       <c r="L3">
-        <v>0.1332748837988889</v>
+        <v>0.128872195788243</v>
       </c>
       <c r="M3">
-        <v>0.1533272690361234</v>
+        <v>0.04297091481733515</v>
       </c>
       <c r="N3">
-        <v>-1.146946634604127e-15</v>
+        <v>-2.715101058052503e-15</v>
       </c>
       <c r="O3">
-        <v>-0.1028537241709977</v>
+        <v>0.2381854107749196</v>
+      </c>
+      <c r="Q3">
+        <v>-0.08536749808907217</v>
       </c>
       <c r="R3">
-        <v>0.3724832149705329</v>
+        <v>0.2275216406864242</v>
       </c>
       <c r="S3">
-        <v>-0.2206076074987401</v>
+        <v>-0.06565099558862902</v>
       </c>
       <c r="T3">
-        <v>0.1197012848033941</v>
+        <v>0.2347338694710326</v>
       </c>
       <c r="U3">
-        <v>-0.2361543508333692</v>
+        <v>-0.103413443050865</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -622,58 +628,61 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.2100097071880278</v>
+        <v>-0.08028107925293226</v>
       </c>
       <c r="C4">
-        <v>-0.01509990977053945</v>
+        <v>0.01759041093037989</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.6015365415393672</v>
+        <v>0.3420098061521938</v>
       </c>
       <c r="F4">
-        <v>0.622839780508571</v>
+        <v>0.353135168584302</v>
       </c>
       <c r="G4">
-        <v>0.6052692578710602</v>
+        <v>0.580610016843249</v>
       </c>
       <c r="H4">
-        <v>0.3043785453484635</v>
+        <v>-0.07265401819163401</v>
       </c>
       <c r="I4">
-        <v>0.9089834684659657</v>
+        <v>0.8725898785101567</v>
       </c>
       <c r="J4">
-        <v>0.5539968224811245</v>
+        <v>0.1998123665698788</v>
       </c>
       <c r="K4">
-        <v>0.52576023735489</v>
+        <v>0.2025017344299468</v>
       </c>
       <c r="L4">
-        <v>0.5646147259402614</v>
+        <v>0.5101667631379072</v>
       </c>
       <c r="M4">
-        <v>0.2943428061408312</v>
+        <v>-0.003420558237110482</v>
       </c>
       <c r="N4">
-        <v>-2.920454072657055e-15</v>
+        <v>-2.333815279120254e-15</v>
       </c>
       <c r="O4">
-        <v>-0.2044140082319981</v>
+        <v>0.2550174770674759</v>
+      </c>
+      <c r="Q4">
+        <v>-0.2734415972929674</v>
       </c>
       <c r="R4">
-        <v>-0.2806621929417707</v>
+        <v>-0.309148673882749</v>
       </c>
       <c r="S4">
-        <v>0.563808953974267</v>
+        <v>0.6547319683147949</v>
       </c>
       <c r="T4">
-        <v>0.4401659758900596</v>
+        <v>0.5665499698028594</v>
       </c>
       <c r="U4">
-        <v>0.3157102365176738</v>
+        <v>0.3944381554315087</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -681,58 +690,61 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.1397562947531871</v>
+        <v>-0.06451676150671957</v>
       </c>
       <c r="C5">
-        <v>0.08162223061345381</v>
+        <v>-0.0389481114345613</v>
       </c>
       <c r="D5">
-        <v>0.6015365415393672</v>
+        <v>0.3420098061521938</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.9900306049985805</v>
+        <v>0.9911163314339113</v>
       </c>
       <c r="G5">
-        <v>0.1257176556239894</v>
+        <v>0.07709134557571934</v>
       </c>
       <c r="H5">
-        <v>0.8177480993505468</v>
+        <v>0.8002955906427053</v>
       </c>
       <c r="I5">
-        <v>0.7676081924089456</v>
+        <v>0.6463343830641423</v>
       </c>
       <c r="J5">
-        <v>0.8777559965761299</v>
+        <v>0.8715252866363846</v>
       </c>
       <c r="K5">
-        <v>0.7745478205579475</v>
+        <v>0.7867844224644608</v>
       </c>
       <c r="L5">
-        <v>0.2102515205998472</v>
+        <v>0.1777355721812599</v>
       </c>
       <c r="M5">
-        <v>0.607083010218251</v>
+        <v>0.6304443735716682</v>
       </c>
       <c r="N5">
-        <v>3.336680005718555e-15</v>
+        <v>3.925747808330758e-15</v>
       </c>
       <c r="O5">
-        <v>-0.4942361054572194</v>
+        <v>-0.5750751645819933</v>
+      </c>
+      <c r="Q5">
+        <v>-0.6877130441236282</v>
       </c>
       <c r="R5">
-        <v>-0.042330879022222</v>
+        <v>0.0661792759032966</v>
       </c>
       <c r="S5">
-        <v>-0.1172357904798116</v>
+        <v>-0.2284291431118642</v>
       </c>
       <c r="T5">
-        <v>0.3925835194979616</v>
+        <v>0.1287674320613623</v>
       </c>
       <c r="U5">
-        <v>-0.3500317328095502</v>
+        <v>-0.438189018297981</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -740,58 +752,61 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.1350151204931508</v>
+        <v>-0.05591325661825367</v>
       </c>
       <c r="C6">
-        <v>0.08730196051608709</v>
+        <v>-0.04520710184843514</v>
       </c>
       <c r="D6">
-        <v>0.622839780508571</v>
+        <v>0.353135168584302</v>
       </c>
       <c r="E6">
-        <v>0.9900306049985805</v>
+        <v>0.9911163314339113</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.1369577931509407</v>
+        <v>0.07395560470160355</v>
       </c>
       <c r="H6">
-        <v>0.8322900178196406</v>
+        <v>0.8161702251891376</v>
       </c>
       <c r="I6">
-        <v>0.7825289384836726</v>
+        <v>0.6541207049692819</v>
       </c>
       <c r="J6">
-        <v>0.8959704693059219</v>
+        <v>0.8891462131489527</v>
       </c>
       <c r="K6">
-        <v>0.8039190036363218</v>
+        <v>0.8122046680302711</v>
       </c>
       <c r="L6">
-        <v>0.2290172208916044</v>
+        <v>0.1807232220615936</v>
       </c>
       <c r="M6">
-        <v>0.6212141847421688</v>
+        <v>0.6455048211576415</v>
       </c>
       <c r="N6">
-        <v>7.666083750325158e-16</v>
+        <v>1.018567689104012e-15</v>
       </c>
       <c r="O6">
-        <v>-0.487397570104229</v>
+        <v>-0.6092447830373894</v>
+      </c>
+      <c r="Q6">
+        <v>-0.7115213322650167</v>
       </c>
       <c r="R6">
-        <v>-0.03211179235540852</v>
+        <v>0.07805401158856294</v>
       </c>
       <c r="S6">
-        <v>-0.1002609806753609</v>
+        <v>-0.2290330136221738</v>
       </c>
       <c r="T6">
-        <v>0.3640726428403179</v>
+        <v>0.1095712728080283</v>
       </c>
       <c r="U6">
-        <v>-0.33213038900801</v>
+        <v>-0.4354082049902045</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -799,58 +814,61 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.2423937982455314</v>
+        <v>-0.1289602411770273</v>
       </c>
       <c r="C7">
-        <v>0.1770781441752131</v>
+        <v>0.17154646284977</v>
       </c>
       <c r="D7">
-        <v>0.6052692578710602</v>
+        <v>0.580610016843249</v>
       </c>
       <c r="E7">
-        <v>0.1257176556239894</v>
+        <v>0.07709134557571934</v>
       </c>
       <c r="F7">
-        <v>0.1369577931509407</v>
+        <v>0.07395560470160355</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>-0.0827955260901168</v>
+        <v>-0.1398429802650279</v>
       </c>
       <c r="I7">
-        <v>0.4895566543418153</v>
+        <v>0.4818880281947166</v>
       </c>
       <c r="J7">
-        <v>0.006393420111500975</v>
+        <v>-0.04658204859367849</v>
       </c>
       <c r="K7">
-        <v>0.01793778858604152</v>
+        <v>-0.02976883674366824</v>
       </c>
       <c r="L7">
-        <v>0.9586818989706541</v>
+        <v>0.9538235177682507</v>
       </c>
       <c r="M7">
-        <v>-0.1173559079185561</v>
+        <v>-0.1399548127558044</v>
       </c>
       <c r="N7">
-        <v>2.041337486133197e-16</v>
+        <v>2.537854193292807e-16</v>
       </c>
       <c r="O7">
-        <v>0.09051725814192106</v>
+        <v>0.3683856840504274</v>
+      </c>
+      <c r="Q7">
+        <v>-0.1473399084798726</v>
       </c>
       <c r="R7">
-        <v>-0.0687034405025222</v>
+        <v>-0.1337922073884447</v>
       </c>
       <c r="S7">
-        <v>0.6193672897256314</v>
+        <v>0.5851904671733715</v>
       </c>
       <c r="T7">
-        <v>0.2438475521930638</v>
+        <v>0.239705259217227</v>
       </c>
       <c r="U7">
-        <v>0.3593642545909256</v>
+        <v>0.3710403620010034</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -858,58 +876,61 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.1237654066428298</v>
+        <v>-0.08107859177575918</v>
       </c>
       <c r="C8">
-        <v>0.1997201598806487</v>
+        <v>0.01769585812541223</v>
       </c>
       <c r="D8">
-        <v>0.3043785453484635</v>
+        <v>-0.07265401819163401</v>
       </c>
       <c r="E8">
-        <v>0.8177480993505468</v>
+        <v>0.8002955906427053</v>
       </c>
       <c r="F8">
-        <v>0.8322900178196406</v>
+        <v>0.8161702251891376</v>
       </c>
       <c r="G8">
-        <v>-0.0827955260901168</v>
+        <v>-0.1398429802650279</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.5183839700041073</v>
+        <v>0.2754120436524903</v>
       </c>
       <c r="J8">
-        <v>0.8143982873320751</v>
+        <v>0.846761988204267</v>
       </c>
       <c r="K8">
-        <v>0.7161035345579564</v>
+        <v>0.7631818664317043</v>
       </c>
       <c r="L8">
-        <v>-0.01930103596191794</v>
+        <v>-0.05804359256587605</v>
       </c>
       <c r="M8">
-        <v>0.778931576145244</v>
+        <v>0.8254033223257329</v>
       </c>
       <c r="N8">
-        <v>-6.631039802115322e-16</v>
+        <v>3.340238619119773e-15</v>
       </c>
       <c r="O8">
-        <v>-0.5516707609764604</v>
+        <v>-0.78734837908404</v>
+      </c>
+      <c r="Q8">
+        <v>-0.6862980439282563</v>
       </c>
       <c r="R8">
-        <v>0.1490765808683637</v>
+        <v>0.2793358451268426</v>
       </c>
       <c r="S8">
-        <v>-0.3819145055213614</v>
+        <v>-0.522759205609126</v>
       </c>
       <c r="T8">
-        <v>0.1864068206580604</v>
+        <v>-0.1896673385614313</v>
       </c>
       <c r="U8">
-        <v>-0.5215930626895318</v>
+        <v>-0.601619071820568</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -917,58 +938,61 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.2139266899315793</v>
+        <v>-0.1336208874169375</v>
       </c>
       <c r="C9">
-        <v>-0.0873917012978082</v>
+        <v>-0.09550244895406114</v>
       </c>
       <c r="D9">
-        <v>0.9089834684659657</v>
+        <v>0.8725898785101567</v>
       </c>
       <c r="E9">
-        <v>0.7676081924089456</v>
+        <v>0.6463343830641423</v>
       </c>
       <c r="F9">
-        <v>0.7825289384836726</v>
+        <v>0.6541207049692819</v>
       </c>
       <c r="G9">
-        <v>0.4895566543418153</v>
+        <v>0.4818880281947166</v>
       </c>
       <c r="H9">
-        <v>0.5183839700041073</v>
+        <v>0.2754120436524903</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.7292238056940705</v>
+        <v>0.5109744879001165</v>
       </c>
       <c r="K9">
-        <v>0.6581600365985067</v>
+        <v>0.4665181780328841</v>
       </c>
       <c r="L9">
-        <v>0.5269665846687024</v>
+        <v>0.5076179904358895</v>
       </c>
       <c r="M9">
-        <v>0.4125547930126223</v>
+        <v>0.2213529491100038</v>
       </c>
       <c r="N9">
-        <v>7.807518436920194e-16</v>
+        <v>5.01264877179206e-15</v>
       </c>
       <c r="O9">
-        <v>-0.3007117501436224</v>
+        <v>-0.04380453715060845</v>
+      </c>
+      <c r="Q9">
+        <v>-0.4962758952683891</v>
       </c>
       <c r="R9">
-        <v>-0.2181396823853521</v>
+        <v>-0.1897581480668075</v>
       </c>
       <c r="S9">
-        <v>0.4226321700395524</v>
+        <v>0.4703521727627966</v>
       </c>
       <c r="T9">
-        <v>0.4603379440818752</v>
+        <v>0.4664317794183128</v>
       </c>
       <c r="U9">
-        <v>0.1740207184735122</v>
+        <v>0.1897228087810305</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -976,58 +1000,61 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.04865741612991594</v>
+        <v>0.1212748770636073</v>
       </c>
       <c r="C10">
-        <v>-0.06407932926335395</v>
+        <v>-0.1728841612412639</v>
       </c>
       <c r="D10">
-        <v>0.5539968224811245</v>
+        <v>0.1998123665698788</v>
       </c>
       <c r="E10">
-        <v>0.8777559965761299</v>
+        <v>0.8715252866363846</v>
       </c>
       <c r="F10">
-        <v>0.8959704693059219</v>
+        <v>0.8891462131489527</v>
       </c>
       <c r="G10">
-        <v>0.006393420111500975</v>
+        <v>-0.04658204859367849</v>
       </c>
       <c r="H10">
-        <v>0.8143982873320751</v>
+        <v>0.846761988204267</v>
       </c>
       <c r="I10">
-        <v>0.7292238056940705</v>
+        <v>0.5109744879001165</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.9654431488146151</v>
+        <v>0.9714663814495552</v>
       </c>
       <c r="L10">
-        <v>0.07050475755270486</v>
+        <v>0.03527371022733559</v>
       </c>
       <c r="M10">
-        <v>0.7697349593525429</v>
+        <v>0.8166295398196073</v>
       </c>
       <c r="N10">
-        <v>9.948215812580311e-15</v>
+        <v>-4.40903262349265e-15</v>
       </c>
       <c r="O10">
-        <v>-0.5377701809645062</v>
+        <v>-0.715416787759944</v>
+      </c>
+      <c r="Q10">
+        <v>-0.6810723571717774</v>
       </c>
       <c r="R10">
-        <v>-0.2268680819084783</v>
+        <v>-0.08794789747066932</v>
       </c>
       <c r="S10">
-        <v>-0.1195319569650822</v>
+        <v>-0.3091615646000345</v>
       </c>
       <c r="T10">
-        <v>0.2836745318532706</v>
+        <v>-0.07865315985536867</v>
       </c>
       <c r="U10">
-        <v>-0.2919061767525117</v>
+        <v>-0.409787731256156</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1035,58 +1062,61 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.109217188323338</v>
+        <v>0.1669514769051775</v>
       </c>
       <c r="C11">
-        <v>-0.04380620175755993</v>
+        <v>-0.1510466670382437</v>
       </c>
       <c r="D11">
-        <v>0.52576023735489</v>
+        <v>0.2025017344299468</v>
       </c>
       <c r="E11">
-        <v>0.7745478205579475</v>
+        <v>0.7867844224644608</v>
       </c>
       <c r="F11">
-        <v>0.8039190036363218</v>
+        <v>0.8122046680302711</v>
       </c>
       <c r="G11">
-        <v>0.01793778858604152</v>
+        <v>-0.02976883674366824</v>
       </c>
       <c r="H11">
-        <v>0.7161035345579564</v>
+        <v>0.7631818664317043</v>
       </c>
       <c r="I11">
-        <v>0.6581600365985067</v>
+        <v>0.4665181780328841</v>
       </c>
       <c r="J11">
-        <v>0.9654431488146151</v>
+        <v>0.9714663814495552</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.0630568220275609</v>
+        <v>0.03558639420618973</v>
       </c>
       <c r="M11">
-        <v>0.7819199761477985</v>
+        <v>0.8206947611547886</v>
       </c>
       <c r="N11">
-        <v>2.136580471001812e-15</v>
+        <v>7.872665950443372e-15</v>
       </c>
       <c r="O11">
-        <v>-0.5305931793137654</v>
+        <v>-0.6746596761889718</v>
+      </c>
+      <c r="Q11">
+        <v>-0.6606718909079263</v>
       </c>
       <c r="R11">
-        <v>-0.2928939929855898</v>
+        <v>-0.1577182903303236</v>
       </c>
       <c r="S11">
-        <v>-0.09199152183265459</v>
+        <v>-0.2794921083792307</v>
       </c>
       <c r="T11">
-        <v>0.2060365383140566</v>
+        <v>-0.1056212839727931</v>
       </c>
       <c r="U11">
-        <v>-0.2405096388005949</v>
+        <v>-0.3571116473215276</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1094,58 +1124,61 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.2641546473894593</v>
+        <v>-0.1580570607631968</v>
       </c>
       <c r="C12">
-        <v>0.1332748837988889</v>
+        <v>0.128872195788243</v>
       </c>
       <c r="D12">
-        <v>0.5646147259402614</v>
+        <v>0.5101667631379072</v>
       </c>
       <c r="E12">
-        <v>0.2102515205998472</v>
+        <v>0.1777355721812599</v>
       </c>
       <c r="F12">
-        <v>0.2290172208916044</v>
+        <v>0.1807232220615936</v>
       </c>
       <c r="G12">
-        <v>0.9586818989706541</v>
+        <v>0.9538235177682507</v>
       </c>
       <c r="H12">
-        <v>-0.01930103596191794</v>
+        <v>-0.05804359256587605</v>
       </c>
       <c r="I12">
-        <v>0.5269665846687024</v>
+        <v>0.5076179904358895</v>
       </c>
       <c r="J12">
-        <v>0.07050475755270486</v>
+        <v>0.03527371022733559</v>
       </c>
       <c r="K12">
-        <v>0.0630568220275609</v>
+        <v>0.03558639420618973</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>-0.1462537487898222</v>
+        <v>-0.1469416240727789</v>
       </c>
       <c r="N12">
-        <v>1.143879312308305e-16</v>
+        <v>1.250638284875952e-17</v>
       </c>
       <c r="O12">
-        <v>0.1085129844232405</v>
+        <v>0.2787716536428464</v>
+      </c>
+      <c r="Q12">
+        <v>-0.2078773839524954</v>
       </c>
       <c r="R12">
-        <v>-0.01903605818527438</v>
+        <v>-0.08212577364749574</v>
       </c>
       <c r="S12">
-        <v>0.5471289431832419</v>
+        <v>0.4994559237697548</v>
       </c>
       <c r="T12">
-        <v>0.2467166122058998</v>
+        <v>0.2026330678233056</v>
       </c>
       <c r="U12">
-        <v>0.2641093728914577</v>
+        <v>0.268460120312103</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1153,58 +1186,61 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.01962844121283543</v>
+        <v>0.03604911749963439</v>
       </c>
       <c r="C13">
-        <v>0.1533272690361234</v>
+        <v>0.04297091481733515</v>
       </c>
       <c r="D13">
-        <v>0.2943428061408312</v>
+        <v>-0.003420558237110482</v>
       </c>
       <c r="E13">
-        <v>0.607083010218251</v>
+        <v>0.6304443735716682</v>
       </c>
       <c r="F13">
-        <v>0.6212141847421688</v>
+        <v>0.6455048211576415</v>
       </c>
       <c r="G13">
-        <v>-0.1173559079185561</v>
+        <v>-0.1399548127558044</v>
       </c>
       <c r="H13">
-        <v>0.778931576145244</v>
+        <v>0.8254033223257329</v>
       </c>
       <c r="I13">
-        <v>0.4125547930126223</v>
+        <v>0.2213529491100038</v>
       </c>
       <c r="J13">
-        <v>0.7697349593525429</v>
+        <v>0.8166295398196073</v>
       </c>
       <c r="K13">
-        <v>0.7819199761477985</v>
+        <v>0.8206947611547886</v>
       </c>
       <c r="L13">
-        <v>-0.1462537487898222</v>
+        <v>-0.1469416240727789</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-3.663626190122911e-15</v>
+        <v>-7.508266900537718e-15</v>
       </c>
       <c r="O13">
-        <v>-0.4190085292392897</v>
+        <v>-0.6941122480774149</v>
+      </c>
+      <c r="Q13">
+        <v>-0.5113888272020113</v>
       </c>
       <c r="R13">
-        <v>-0.1226664923885096</v>
+        <v>0.002584792154808971</v>
       </c>
       <c r="S13">
-        <v>-0.2273234080895403</v>
+        <v>-0.376821317133906</v>
       </c>
       <c r="T13">
-        <v>0.1391403236753642</v>
+        <v>-0.1667968886159874</v>
       </c>
       <c r="U13">
-        <v>-0.3333457373732241</v>
+        <v>-0.4106821211872534</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1212,58 +1248,61 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6.055881544898674e-17</v>
+        <v>-1.087096885153984e-16</v>
       </c>
       <c r="C14">
-        <v>-1.146946634604127e-15</v>
+        <v>-2.715101058052503e-15</v>
       </c>
       <c r="D14">
-        <v>-2.920454072657055e-15</v>
+        <v>-2.333815279120254e-15</v>
       </c>
       <c r="E14">
-        <v>3.336680005718555e-15</v>
+        <v>3.925747808330758e-15</v>
       </c>
       <c r="F14">
-        <v>7.666083750325158e-16</v>
+        <v>1.018567689104012e-15</v>
       </c>
       <c r="G14">
-        <v>2.041337486133197e-16</v>
+        <v>2.537854193292807e-16</v>
       </c>
       <c r="H14">
-        <v>-6.631039802115322e-16</v>
+        <v>3.340238619119773e-15</v>
       </c>
       <c r="I14">
-        <v>7.807518436920194e-16</v>
+        <v>5.01264877179206e-15</v>
       </c>
       <c r="J14">
-        <v>9.948215812580311e-15</v>
+        <v>-4.40903262349265e-15</v>
       </c>
       <c r="K14">
-        <v>2.136580471001812e-15</v>
+        <v>7.872665950443372e-15</v>
       </c>
       <c r="L14">
-        <v>1.143879312308305e-16</v>
+        <v>1.250638284875952e-17</v>
       </c>
       <c r="M14">
-        <v>-3.663626190122911e-15</v>
+        <v>-7.508266900537718e-15</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>4.469207541101161e-15</v>
+        <v>9.395915572035722e-16</v>
+      </c>
+      <c r="Q14">
+        <v>5.35279227359119e-15</v>
       </c>
       <c r="R14">
-        <v>2.7795804443586e-15</v>
+        <v>1.19330235870952e-15</v>
       </c>
       <c r="S14">
-        <v>1.980989761816137e-16</v>
+        <v>-6.835900981806389e-16</v>
       </c>
       <c r="T14">
-        <v>1.410169364536039e-15</v>
+        <v>-1.280626059053519e-15</v>
       </c>
       <c r="U14">
-        <v>8.721150744904445e-16</v>
+        <v>-1.510002358127825e-15</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1271,58 +1310,61 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.0888815068024154</v>
+        <v>-0.1853868407917172</v>
       </c>
       <c r="C15">
-        <v>-0.1028537241709977</v>
+        <v>0.2381854107749196</v>
       </c>
       <c r="D15">
-        <v>-0.2044140082319981</v>
+        <v>0.2550174770674759</v>
       </c>
       <c r="E15">
-        <v>-0.4942361054572194</v>
+        <v>-0.5750751645819933</v>
       </c>
       <c r="F15">
-        <v>-0.487397570104229</v>
+        <v>-0.6092447830373894</v>
       </c>
       <c r="G15">
-        <v>0.09051725814192106</v>
+        <v>0.3683856840504274</v>
       </c>
       <c r="H15">
-        <v>-0.5516707609764604</v>
+        <v>-0.78734837908404</v>
       </c>
       <c r="I15">
-        <v>-0.3007117501436224</v>
+        <v>-0.04380453715060845</v>
       </c>
       <c r="J15">
-        <v>-0.5377701809645062</v>
+        <v>-0.715416787759944</v>
       </c>
       <c r="K15">
-        <v>-0.5305931793137654</v>
+        <v>-0.6746596761889718</v>
       </c>
       <c r="L15">
-        <v>0.1085129844232405</v>
+        <v>0.2787716536428464</v>
       </c>
       <c r="M15">
-        <v>-0.4190085292392897</v>
+        <v>-0.6941122480774149</v>
       </c>
       <c r="N15">
-        <v>4.469207541101161e-15</v>
+        <v>9.395915572035722e-16</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
+      <c r="Q15">
+        <v>0.3572962238144697</v>
+      </c>
       <c r="R15">
-        <v>-0.002206594487502868</v>
+        <v>-0.2325343984874021</v>
       </c>
       <c r="S15">
-        <v>0.2946365454871068</v>
+        <v>0.6128724850007402</v>
       </c>
       <c r="T15">
-        <v>-0.07004655851513285</v>
+        <v>0.2462513035246475</v>
       </c>
       <c r="U15">
-        <v>0.3463609289302713</v>
+        <v>0.6227221058909642</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1334,64 +1376,124 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>0.0424264846503711</v>
+      </c>
+      <c r="C17">
+        <v>-0.08536749808907217</v>
+      </c>
+      <c r="D17">
+        <v>-0.2734415972929674</v>
+      </c>
+      <c r="E17">
+        <v>-0.6877130441236282</v>
+      </c>
+      <c r="F17">
+        <v>-0.7115213322650167</v>
+      </c>
+      <c r="G17">
+        <v>-0.1473399084798726</v>
+      </c>
+      <c r="H17">
+        <v>-0.6862980439282563</v>
+      </c>
+      <c r="I17">
+        <v>-0.4962758952683891</v>
+      </c>
+      <c r="J17">
+        <v>-0.6810723571717774</v>
+      </c>
+      <c r="K17">
+        <v>-0.6606718909079263</v>
+      </c>
+      <c r="L17">
+        <v>-0.2078773839524954</v>
+      </c>
+      <c r="M17">
+        <v>-0.5113888272020113</v>
+      </c>
+      <c r="N17">
+        <v>5.35279227359119e-15</v>
+      </c>
+      <c r="O17">
+        <v>0.3572962238144697</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>-0.08617877791966425</v>
+      </c>
+      <c r="S17">
+        <v>0.2253213926909598</v>
+      </c>
+      <c r="T17">
+        <v>0.07647764970540155</v>
+      </c>
+      <c r="U17">
+        <v>0.3819160385100963</v>
+      </c>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.1785047152953003</v>
+        <v>-0.2845345830205061</v>
       </c>
       <c r="C18">
-        <v>0.3724832149705329</v>
+        <v>0.2275216406864242</v>
       </c>
       <c r="D18">
-        <v>-0.2806621929417707</v>
+        <v>-0.309148673882749</v>
       </c>
       <c r="E18">
-        <v>-0.042330879022222</v>
+        <v>0.0661792759032966</v>
       </c>
       <c r="F18">
-        <v>-0.03211179235540852</v>
+        <v>0.07805401158856294</v>
       </c>
       <c r="G18">
-        <v>-0.0687034405025222</v>
+        <v>-0.1337922073884447</v>
       </c>
       <c r="H18">
-        <v>0.1490765808683637</v>
+        <v>0.2793358451268426</v>
       </c>
       <c r="I18">
-        <v>-0.2181396823853521</v>
+        <v>-0.1897581480668075</v>
       </c>
       <c r="J18">
-        <v>-0.2268680819084783</v>
+        <v>-0.08794789747066932</v>
       </c>
       <c r="K18">
-        <v>-0.2928939929855898</v>
+        <v>-0.1577182903303236</v>
       </c>
       <c r="L18">
-        <v>-0.01903605818527438</v>
+        <v>-0.08212577364749574</v>
       </c>
       <c r="M18">
-        <v>-0.1226664923885096</v>
+        <v>0.002584792154808971</v>
       </c>
       <c r="N18">
-        <v>2.7795804443586e-15</v>
+        <v>1.19330235870952e-15</v>
       </c>
       <c r="O18">
-        <v>-0.002206594487502868</v>
+        <v>-0.2325343984874021</v>
+      </c>
+      <c r="Q18">
+        <v>-0.08617877791966425</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
       <c r="S18">
-        <v>-0.2721965536453438</v>
+        <v>-0.2800757300459217</v>
       </c>
       <c r="T18">
-        <v>-0.01915406161276758</v>
+        <v>-0.01196058651824267</v>
       </c>
       <c r="U18">
-        <v>-0.2391338560180774</v>
+        <v>-0.2827927281285642</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1399,58 +1501,61 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-0.1254907045969606</v>
+        <v>-0.1355720031208364</v>
       </c>
       <c r="C19">
-        <v>-0.2206076074987401</v>
+        <v>-0.06565099558862902</v>
       </c>
       <c r="D19">
-        <v>0.563808953974267</v>
+        <v>0.6547319683147949</v>
       </c>
       <c r="E19">
-        <v>-0.1172357904798116</v>
+        <v>-0.2284291431118642</v>
       </c>
       <c r="F19">
-        <v>-0.1002609806753609</v>
+        <v>-0.2290330136221738</v>
       </c>
       <c r="G19">
-        <v>0.6193672897256314</v>
+        <v>0.5851904671733715</v>
       </c>
       <c r="H19">
-        <v>-0.3819145055213614</v>
+        <v>-0.522759205609126</v>
       </c>
       <c r="I19">
-        <v>0.4226321700395524</v>
+        <v>0.4703521727627966</v>
       </c>
       <c r="J19">
-        <v>-0.1195319569650822</v>
+        <v>-0.3091615646000345</v>
       </c>
       <c r="K19">
-        <v>-0.09199152183265459</v>
+        <v>-0.2794921083792307</v>
       </c>
       <c r="L19">
-        <v>0.5471289431832419</v>
+        <v>0.4994559237697548</v>
       </c>
       <c r="M19">
-        <v>-0.2273234080895403</v>
+        <v>-0.376821317133906</v>
       </c>
       <c r="N19">
-        <v>1.980989761816137e-16</v>
+        <v>-6.835900981806389e-16</v>
       </c>
       <c r="O19">
-        <v>0.2946365454871068</v>
+        <v>0.6128724850007402</v>
+      </c>
+      <c r="Q19">
+        <v>0.2253213926909598</v>
       </c>
       <c r="R19">
-        <v>-0.2721965536453438</v>
+        <v>-0.2800757300459217</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19">
-        <v>0.1658873665894034</v>
+        <v>0.4031479931589017</v>
       </c>
       <c r="U19">
-        <v>0.9098052194387964</v>
+        <v>0.8936576820698581</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1458,58 +1563,61 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.3184960359875938</v>
+        <v>-0.3204245567604783</v>
       </c>
       <c r="C20">
-        <v>0.1197012848033941</v>
+        <v>0.2347338694710326</v>
       </c>
       <c r="D20">
-        <v>0.4401659758900596</v>
+        <v>0.5665499698028594</v>
       </c>
       <c r="E20">
-        <v>0.3925835194979616</v>
+        <v>0.1287674320613623</v>
       </c>
       <c r="F20">
-        <v>0.3640726428403179</v>
+        <v>0.1095712728080283</v>
       </c>
       <c r="G20">
-        <v>0.2438475521930638</v>
+        <v>0.239705259217227</v>
       </c>
       <c r="H20">
-        <v>0.1864068206580604</v>
+        <v>-0.1896673385614313</v>
       </c>
       <c r="I20">
-        <v>0.4603379440818752</v>
+        <v>0.4664317794183128</v>
       </c>
       <c r="J20">
-        <v>0.2836745318532706</v>
+        <v>-0.07865315985536867</v>
       </c>
       <c r="K20">
-        <v>0.2060365383140566</v>
+        <v>-0.1056212839727931</v>
       </c>
       <c r="L20">
-        <v>0.2467166122058998</v>
+        <v>0.2026330678233056</v>
       </c>
       <c r="M20">
-        <v>0.1391403236753642</v>
+        <v>-0.1667968886159874</v>
       </c>
       <c r="N20">
-        <v>1.410169364536039e-15</v>
+        <v>-1.280626059053519e-15</v>
       </c>
       <c r="O20">
-        <v>-0.07004655851513285</v>
+        <v>0.2462513035246475</v>
+      </c>
+      <c r="Q20">
+        <v>0.07647764970540155</v>
       </c>
       <c r="R20">
-        <v>-0.01915406161276758</v>
+        <v>-0.01196058651824267</v>
       </c>
       <c r="S20">
-        <v>0.1658873665894034</v>
+        <v>0.4031479931589017</v>
       </c>
       <c r="T20">
         <v>1</v>
       </c>
       <c r="U20">
-        <v>-0.01269413487343376</v>
+        <v>0.1811080554343676</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1517,55 +1625,58 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-0.06978520298733354</v>
+        <v>-0.05011482699256612</v>
       </c>
       <c r="C21">
-        <v>-0.2361543508333692</v>
+        <v>-0.103413443050865</v>
       </c>
       <c r="D21">
-        <v>0.3157102365176738</v>
+        <v>0.3944381554315087</v>
       </c>
       <c r="E21">
-        <v>-0.3500317328095502</v>
+        <v>-0.438189018297981</v>
       </c>
       <c r="F21">
-        <v>-0.33213038900801</v>
+        <v>-0.4354082049902045</v>
       </c>
       <c r="G21">
-        <v>0.3593642545909256</v>
+        <v>0.3710403620010034</v>
       </c>
       <c r="H21">
-        <v>-0.5215930626895318</v>
+        <v>-0.601619071820568</v>
       </c>
       <c r="I21">
-        <v>0.1740207184735122</v>
+        <v>0.1897228087810305</v>
       </c>
       <c r="J21">
-        <v>-0.2919061767525117</v>
+        <v>-0.409787731256156</v>
       </c>
       <c r="K21">
-        <v>-0.2405096388005949</v>
+        <v>-0.3571116473215276</v>
       </c>
       <c r="L21">
-        <v>0.2641093728914577</v>
+        <v>0.268460120312103</v>
       </c>
       <c r="M21">
-        <v>-0.3333457373732241</v>
+        <v>-0.4106821211872534</v>
       </c>
       <c r="N21">
-        <v>8.721150744904445e-16</v>
+        <v>-1.510002358127825e-15</v>
       </c>
       <c r="O21">
-        <v>0.3463609289302713</v>
+        <v>0.6227221058909642</v>
+      </c>
+      <c r="Q21">
+        <v>0.3819160385100963</v>
       </c>
       <c r="R21">
-        <v>-0.2391338560180774</v>
+        <v>-0.2827927281285642</v>
       </c>
       <c r="S21">
-        <v>0.9098052194387964</v>
+        <v>0.8936576820698581</v>
       </c>
       <c r="T21">
-        <v>-0.01269413487343376</v>
+        <v>0.1811080554343676</v>
       </c>
       <c r="U21">
         <v>1</v>

</xml_diff>

<commit_message>
redo the macro correlation analysis using yearly return of sp500 instead of monthly. Now showing more obvious correlation of countercyclical risks and skewness. Correlation being high for high-education. Plus generational/age/income differences.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>sp500</t>
   </si>
@@ -55,25 +55,13 @@
     <t>kurtEstMed</t>
   </si>
   <si>
-    <t>meanEstMed</t>
-  </si>
-  <si>
     <t>skewEstMed</t>
   </si>
   <si>
-    <t>varEstMed</t>
-  </si>
-  <si>
     <t>kurtEstMean</t>
   </si>
   <si>
-    <t>meanEstMean</t>
-  </si>
-  <si>
     <t>skewEstMean</t>
-  </si>
-  <si>
-    <t>varEstMean</t>
   </si>
 </sst>
 </file>
@@ -431,13 +419,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,20 +474,8 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,66 +483,54 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.5607082011729043</v>
+        <v>-0.6793485726317077</v>
       </c>
       <c r="D2">
-        <v>-0.08028107925293226</v>
+        <v>-0.07483363088081939</v>
       </c>
       <c r="E2">
-        <v>-0.06451676150671957</v>
+        <v>0.0605837209325372</v>
       </c>
       <c r="F2">
-        <v>-0.05591325661825367</v>
+        <v>0.09165378621206373</v>
       </c>
       <c r="G2">
-        <v>-0.1289602411770273</v>
+        <v>-0.562449651783383</v>
       </c>
       <c r="H2">
-        <v>-0.08107859177575918</v>
+        <v>0.1464443784388182</v>
       </c>
       <c r="I2">
-        <v>-0.1336208874169375</v>
+        <v>0.02185912962278377</v>
       </c>
       <c r="J2">
-        <v>0.1212748770636073</v>
+        <v>0.2710843207654442</v>
       </c>
       <c r="K2">
-        <v>0.1669514769051775</v>
+        <v>0.2647490013995931</v>
       </c>
       <c r="L2">
-        <v>-0.1580570607631968</v>
+        <v>-0.5866536696558399</v>
       </c>
       <c r="M2">
-        <v>0.03604911749963439</v>
+        <v>0.162241127660825</v>
       </c>
       <c r="N2">
-        <v>-1.087096885153984e-16</v>
-      </c>
-      <c r="O2">
-        <v>-0.1853868407917172</v>
+        <v>2.249869722626098e-16</v>
+      </c>
+      <c r="P2">
+        <v>-0.08806881822253153</v>
       </c>
       <c r="Q2">
-        <v>0.0424264846503711</v>
-      </c>
-      <c r="R2">
-        <v>-0.2845345830205061</v>
-      </c>
-      <c r="S2">
-        <v>-0.1355720031208364</v>
-      </c>
-      <c r="T2">
-        <v>-0.3204245567604783</v>
-      </c>
-      <c r="U2">
-        <v>-0.05011482699256612</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>-0.1895151414319372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.5607082011729043</v>
+        <v>-0.6793485726317077</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -604,31 +568,19 @@
       <c r="N3">
         <v>-2.715101058052503e-15</v>
       </c>
-      <c r="O3">
-        <v>0.2381854107749196</v>
+      <c r="P3">
+        <v>0.2275216406864242</v>
       </c>
       <c r="Q3">
-        <v>-0.08536749808907217</v>
-      </c>
-      <c r="R3">
-        <v>0.2275216406864242</v>
-      </c>
-      <c r="S3">
-        <v>-0.06565099558862902</v>
-      </c>
-      <c r="T3">
         <v>0.2347338694710326</v>
       </c>
-      <c r="U3">
-        <v>-0.103413443050865</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.08028107925293226</v>
+        <v>-0.07483363088081939</v>
       </c>
       <c r="C4">
         <v>0.01759041093037989</v>
@@ -666,31 +618,19 @@
       <c r="N4">
         <v>-2.333815279120254e-15</v>
       </c>
-      <c r="O4">
-        <v>0.2550174770674759</v>
+      <c r="P4">
+        <v>-0.309148673882749</v>
       </c>
       <c r="Q4">
-        <v>-0.2734415972929674</v>
-      </c>
-      <c r="R4">
-        <v>-0.309148673882749</v>
-      </c>
-      <c r="S4">
-        <v>0.6547319683147949</v>
-      </c>
-      <c r="T4">
         <v>0.5665499698028594</v>
       </c>
-      <c r="U4">
-        <v>0.3944381554315087</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.06451676150671957</v>
+        <v>0.0605837209325372</v>
       </c>
       <c r="C5">
         <v>-0.0389481114345613</v>
@@ -728,31 +668,19 @@
       <c r="N5">
         <v>3.925747808330758e-15</v>
       </c>
-      <c r="O5">
-        <v>-0.5750751645819933</v>
+      <c r="P5">
+        <v>0.0661792759032966</v>
       </c>
       <c r="Q5">
-        <v>-0.6877130441236282</v>
-      </c>
-      <c r="R5">
-        <v>0.0661792759032966</v>
-      </c>
-      <c r="S5">
-        <v>-0.2284291431118642</v>
-      </c>
-      <c r="T5">
         <v>0.1287674320613623</v>
       </c>
-      <c r="U5">
-        <v>-0.438189018297981</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.05591325661825367</v>
+        <v>0.09165378621206373</v>
       </c>
       <c r="C6">
         <v>-0.04520710184843514</v>
@@ -790,31 +718,19 @@
       <c r="N6">
         <v>1.018567689104012e-15</v>
       </c>
-      <c r="O6">
-        <v>-0.6092447830373894</v>
+      <c r="P6">
+        <v>0.07805401158856294</v>
       </c>
       <c r="Q6">
-        <v>-0.7115213322650167</v>
-      </c>
-      <c r="R6">
-        <v>0.07805401158856294</v>
-      </c>
-      <c r="S6">
-        <v>-0.2290330136221738</v>
-      </c>
-      <c r="T6">
         <v>0.1095712728080283</v>
       </c>
-      <c r="U6">
-        <v>-0.4354082049902045</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.1289602411770273</v>
+        <v>-0.562449651783383</v>
       </c>
       <c r="C7">
         <v>0.17154646284977</v>
@@ -852,31 +768,19 @@
       <c r="N7">
         <v>2.537854193292807e-16</v>
       </c>
-      <c r="O7">
-        <v>0.3683856840504274</v>
+      <c r="P7">
+        <v>-0.1337922073884447</v>
       </c>
       <c r="Q7">
-        <v>-0.1473399084798726</v>
-      </c>
-      <c r="R7">
-        <v>-0.1337922073884447</v>
-      </c>
-      <c r="S7">
-        <v>0.5851904671733715</v>
-      </c>
-      <c r="T7">
         <v>0.239705259217227</v>
       </c>
-      <c r="U7">
-        <v>0.3710403620010034</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.08107859177575918</v>
+        <v>0.1464443784388182</v>
       </c>
       <c r="C8">
         <v>0.01769585812541223</v>
@@ -914,31 +818,19 @@
       <c r="N8">
         <v>3.340238619119773e-15</v>
       </c>
-      <c r="O8">
-        <v>-0.78734837908404</v>
+      <c r="P8">
+        <v>0.2793358451268426</v>
       </c>
       <c r="Q8">
-        <v>-0.6862980439282563</v>
-      </c>
-      <c r="R8">
-        <v>0.2793358451268426</v>
-      </c>
-      <c r="S8">
-        <v>-0.522759205609126</v>
-      </c>
-      <c r="T8">
         <v>-0.1896673385614313</v>
       </c>
-      <c r="U8">
-        <v>-0.601619071820568</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.1336208874169375</v>
+        <v>0.02185912962278377</v>
       </c>
       <c r="C9">
         <v>-0.09550244895406114</v>
@@ -976,31 +868,19 @@
       <c r="N9">
         <v>5.01264877179206e-15</v>
       </c>
-      <c r="O9">
-        <v>-0.04380453715060845</v>
+      <c r="P9">
+        <v>-0.1897581480668075</v>
       </c>
       <c r="Q9">
-        <v>-0.4962758952683891</v>
-      </c>
-      <c r="R9">
-        <v>-0.1897581480668075</v>
-      </c>
-      <c r="S9">
-        <v>0.4703521727627966</v>
-      </c>
-      <c r="T9">
         <v>0.4664317794183128</v>
       </c>
-      <c r="U9">
-        <v>0.1897228087810305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1212748770636073</v>
+        <v>0.2710843207654442</v>
       </c>
       <c r="C10">
         <v>-0.1728841612412639</v>
@@ -1038,31 +918,19 @@
       <c r="N10">
         <v>-4.40903262349265e-15</v>
       </c>
-      <c r="O10">
-        <v>-0.715416787759944</v>
+      <c r="P10">
+        <v>-0.08794789747066932</v>
       </c>
       <c r="Q10">
-        <v>-0.6810723571717774</v>
-      </c>
-      <c r="R10">
-        <v>-0.08794789747066932</v>
-      </c>
-      <c r="S10">
-        <v>-0.3091615646000345</v>
-      </c>
-      <c r="T10">
         <v>-0.07865315985536867</v>
       </c>
-      <c r="U10">
-        <v>-0.409787731256156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.1669514769051775</v>
+        <v>0.2647490013995931</v>
       </c>
       <c r="C11">
         <v>-0.1510466670382437</v>
@@ -1100,31 +968,19 @@
       <c r="N11">
         <v>7.872665950443372e-15</v>
       </c>
-      <c r="O11">
-        <v>-0.6746596761889718</v>
+      <c r="P11">
+        <v>-0.1577182903303236</v>
       </c>
       <c r="Q11">
-        <v>-0.6606718909079263</v>
-      </c>
-      <c r="R11">
-        <v>-0.1577182903303236</v>
-      </c>
-      <c r="S11">
-        <v>-0.2794921083792307</v>
-      </c>
-      <c r="T11">
         <v>-0.1056212839727931</v>
       </c>
-      <c r="U11">
-        <v>-0.3571116473215276</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.1580570607631968</v>
+        <v>-0.5866536696558399</v>
       </c>
       <c r="C12">
         <v>0.128872195788243</v>
@@ -1162,31 +1018,19 @@
       <c r="N12">
         <v>1.250638284875952e-17</v>
       </c>
-      <c r="O12">
-        <v>0.2787716536428464</v>
+      <c r="P12">
+        <v>-0.08212577364749574</v>
       </c>
       <c r="Q12">
-        <v>-0.2078773839524954</v>
-      </c>
-      <c r="R12">
-        <v>-0.08212577364749574</v>
-      </c>
-      <c r="S12">
-        <v>0.4994559237697548</v>
-      </c>
-      <c r="T12">
         <v>0.2026330678233056</v>
       </c>
-      <c r="U12">
-        <v>0.268460120312103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.03604911749963439</v>
+        <v>0.162241127660825</v>
       </c>
       <c r="C13">
         <v>0.04297091481733515</v>
@@ -1224,31 +1068,19 @@
       <c r="N13">
         <v>-7.508266900537718e-15</v>
       </c>
-      <c r="O13">
-        <v>-0.6941122480774149</v>
+      <c r="P13">
+        <v>0.002584792154808971</v>
       </c>
       <c r="Q13">
-        <v>-0.5113888272020113</v>
-      </c>
-      <c r="R13">
-        <v>0.002584792154808971</v>
-      </c>
-      <c r="S13">
-        <v>-0.376821317133906</v>
-      </c>
-      <c r="T13">
         <v>-0.1667968886159874</v>
       </c>
-      <c r="U13">
-        <v>-0.4106821211872534</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-1.087096885153984e-16</v>
+        <v>2.249869722626098e-16</v>
       </c>
       <c r="C14">
         <v>-2.715101058052503e-15</v>
@@ -1286,399 +1118,115 @@
       <c r="N14">
         <v>1</v>
       </c>
-      <c r="O14">
-        <v>9.395915572035722e-16</v>
+      <c r="P14">
+        <v>1.19330235870952e-15</v>
       </c>
       <c r="Q14">
-        <v>5.35279227359119e-15</v>
-      </c>
-      <c r="R14">
-        <v>1.19330235870952e-15</v>
-      </c>
-      <c r="S14">
-        <v>-6.835900981806389e-16</v>
-      </c>
-      <c r="T14">
         <v>-1.280626059053519e-15</v>
       </c>
-      <c r="U14">
-        <v>-1.510002358127825e-15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>-0.1853868407917172</v>
-      </c>
-      <c r="C15">
-        <v>0.2381854107749196</v>
-      </c>
-      <c r="D15">
-        <v>0.2550174770674759</v>
-      </c>
-      <c r="E15">
-        <v>-0.5750751645819933</v>
-      </c>
-      <c r="F15">
-        <v>-0.6092447830373894</v>
-      </c>
-      <c r="G15">
-        <v>0.3683856840504274</v>
-      </c>
-      <c r="H15">
-        <v>-0.78734837908404</v>
-      </c>
-      <c r="I15">
-        <v>-0.04380453715060845</v>
-      </c>
-      <c r="J15">
-        <v>-0.715416787759944</v>
-      </c>
-      <c r="K15">
-        <v>-0.6746596761889718</v>
-      </c>
-      <c r="L15">
-        <v>0.2787716536428464</v>
-      </c>
-      <c r="M15">
-        <v>-0.6941122480774149</v>
-      </c>
-      <c r="N15">
-        <v>9.395915572035722e-16</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>0.3572962238144697</v>
-      </c>
-      <c r="R15">
-        <v>-0.2325343984874021</v>
-      </c>
-      <c r="S15">
-        <v>0.6128724850007402</v>
-      </c>
-      <c r="T15">
-        <v>0.2462513035246475</v>
-      </c>
-      <c r="U15">
-        <v>0.6227221058909642</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="B16">
+        <v>-0.08806881822253153</v>
+      </c>
+      <c r="C16">
+        <v>0.2275216406864242</v>
+      </c>
+      <c r="D16">
+        <v>-0.309148673882749</v>
+      </c>
+      <c r="E16">
+        <v>0.0661792759032966</v>
+      </c>
+      <c r="F16">
+        <v>0.07805401158856294</v>
+      </c>
+      <c r="G16">
+        <v>-0.1337922073884447</v>
+      </c>
+      <c r="H16">
+        <v>0.2793358451268426</v>
+      </c>
+      <c r="I16">
+        <v>-0.1897581480668075</v>
+      </c>
+      <c r="J16">
+        <v>-0.08794789747066932</v>
+      </c>
+      <c r="K16">
+        <v>-0.1577182903303236</v>
+      </c>
+      <c r="L16">
+        <v>-0.08212577364749574</v>
+      </c>
+      <c r="M16">
+        <v>0.002584792154808971</v>
+      </c>
+      <c r="N16">
+        <v>1.19330235870952e-15</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>-0.01196058651824267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.0424264846503711</v>
+        <v>-0.1895151414319372</v>
       </c>
       <c r="C17">
-        <v>-0.08536749808907217</v>
+        <v>0.2347338694710326</v>
       </c>
       <c r="D17">
-        <v>-0.2734415972929674</v>
+        <v>0.5665499698028594</v>
       </c>
       <c r="E17">
-        <v>-0.6877130441236282</v>
+        <v>0.1287674320613623</v>
       </c>
       <c r="F17">
-        <v>-0.7115213322650167</v>
+        <v>0.1095712728080283</v>
       </c>
       <c r="G17">
-        <v>-0.1473399084798726</v>
+        <v>0.239705259217227</v>
       </c>
       <c r="H17">
-        <v>-0.6862980439282563</v>
+        <v>-0.1896673385614313</v>
       </c>
       <c r="I17">
-        <v>-0.4962758952683891</v>
+        <v>0.4664317794183128</v>
       </c>
       <c r="J17">
-        <v>-0.6810723571717774</v>
+        <v>-0.07865315985536867</v>
       </c>
       <c r="K17">
-        <v>-0.6606718909079263</v>
+        <v>-0.1056212839727931</v>
       </c>
       <c r="L17">
-        <v>-0.2078773839524954</v>
+        <v>0.2026330678233056</v>
       </c>
       <c r="M17">
-        <v>-0.5113888272020113</v>
+        <v>-0.1667968886159874</v>
       </c>
       <c r="N17">
-        <v>5.35279227359119e-15</v>
-      </c>
-      <c r="O17">
-        <v>0.3572962238144697</v>
+        <v>-1.280626059053519e-15</v>
+      </c>
+      <c r="P17">
+        <v>-0.01196058651824267</v>
       </c>
       <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17">
-        <v>-0.08617877791966425</v>
-      </c>
-      <c r="S17">
-        <v>0.2253213926909598</v>
-      </c>
-      <c r="T17">
-        <v>0.07647764970540155</v>
-      </c>
-      <c r="U17">
-        <v>0.3819160385100963</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>-0.2845345830205061</v>
-      </c>
-      <c r="C18">
-        <v>0.2275216406864242</v>
-      </c>
-      <c r="D18">
-        <v>-0.309148673882749</v>
-      </c>
-      <c r="E18">
-        <v>0.0661792759032966</v>
-      </c>
-      <c r="F18">
-        <v>0.07805401158856294</v>
-      </c>
-      <c r="G18">
-        <v>-0.1337922073884447</v>
-      </c>
-      <c r="H18">
-        <v>0.2793358451268426</v>
-      </c>
-      <c r="I18">
-        <v>-0.1897581480668075</v>
-      </c>
-      <c r="J18">
-        <v>-0.08794789747066932</v>
-      </c>
-      <c r="K18">
-        <v>-0.1577182903303236</v>
-      </c>
-      <c r="L18">
-        <v>-0.08212577364749574</v>
-      </c>
-      <c r="M18">
-        <v>0.002584792154808971</v>
-      </c>
-      <c r="N18">
-        <v>1.19330235870952e-15</v>
-      </c>
-      <c r="O18">
-        <v>-0.2325343984874021</v>
-      </c>
-      <c r="Q18">
-        <v>-0.08617877791966425</v>
-      </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>-0.2800757300459217</v>
-      </c>
-      <c r="T18">
-        <v>-0.01196058651824267</v>
-      </c>
-      <c r="U18">
-        <v>-0.2827927281285642</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>-0.1355720031208364</v>
-      </c>
-      <c r="C19">
-        <v>-0.06565099558862902</v>
-      </c>
-      <c r="D19">
-        <v>0.6547319683147949</v>
-      </c>
-      <c r="E19">
-        <v>-0.2284291431118642</v>
-      </c>
-      <c r="F19">
-        <v>-0.2290330136221738</v>
-      </c>
-      <c r="G19">
-        <v>0.5851904671733715</v>
-      </c>
-      <c r="H19">
-        <v>-0.522759205609126</v>
-      </c>
-      <c r="I19">
-        <v>0.4703521727627966</v>
-      </c>
-      <c r="J19">
-        <v>-0.3091615646000345</v>
-      </c>
-      <c r="K19">
-        <v>-0.2794921083792307</v>
-      </c>
-      <c r="L19">
-        <v>0.4994559237697548</v>
-      </c>
-      <c r="M19">
-        <v>-0.376821317133906</v>
-      </c>
-      <c r="N19">
-        <v>-6.835900981806389e-16</v>
-      </c>
-      <c r="O19">
-        <v>0.6128724850007402</v>
-      </c>
-      <c r="Q19">
-        <v>0.2253213926909598</v>
-      </c>
-      <c r="R19">
-        <v>-0.2800757300459217</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19">
-        <v>0.4031479931589017</v>
-      </c>
-      <c r="U19">
-        <v>0.8936576820698581</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>-0.3204245567604783</v>
-      </c>
-      <c r="C20">
-        <v>0.2347338694710326</v>
-      </c>
-      <c r="D20">
-        <v>0.5665499698028594</v>
-      </c>
-      <c r="E20">
-        <v>0.1287674320613623</v>
-      </c>
-      <c r="F20">
-        <v>0.1095712728080283</v>
-      </c>
-      <c r="G20">
-        <v>0.239705259217227</v>
-      </c>
-      <c r="H20">
-        <v>-0.1896673385614313</v>
-      </c>
-      <c r="I20">
-        <v>0.4664317794183128</v>
-      </c>
-      <c r="J20">
-        <v>-0.07865315985536867</v>
-      </c>
-      <c r="K20">
-        <v>-0.1056212839727931</v>
-      </c>
-      <c r="L20">
-        <v>0.2026330678233056</v>
-      </c>
-      <c r="M20">
-        <v>-0.1667968886159874</v>
-      </c>
-      <c r="N20">
-        <v>-1.280626059053519e-15</v>
-      </c>
-      <c r="O20">
-        <v>0.2462513035246475</v>
-      </c>
-      <c r="Q20">
-        <v>0.07647764970540155</v>
-      </c>
-      <c r="R20">
-        <v>-0.01196058651824267</v>
-      </c>
-      <c r="S20">
-        <v>0.4031479931589017</v>
-      </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
-      <c r="U20">
-        <v>0.1811080554343676</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>-0.05011482699256612</v>
-      </c>
-      <c r="C21">
-        <v>-0.103413443050865</v>
-      </c>
-      <c r="D21">
-        <v>0.3944381554315087</v>
-      </c>
-      <c r="E21">
-        <v>-0.438189018297981</v>
-      </c>
-      <c r="F21">
-        <v>-0.4354082049902045</v>
-      </c>
-      <c r="G21">
-        <v>0.3710403620010034</v>
-      </c>
-      <c r="H21">
-        <v>-0.601619071820568</v>
-      </c>
-      <c r="I21">
-        <v>0.1897228087810305</v>
-      </c>
-      <c r="J21">
-        <v>-0.409787731256156</v>
-      </c>
-      <c r="K21">
-        <v>-0.3571116473215276</v>
-      </c>
-      <c r="L21">
-        <v>0.268460120312103</v>
-      </c>
-      <c r="M21">
-        <v>-0.4106821211872534</v>
-      </c>
-      <c r="N21">
-        <v>-1.510002358127825e-15</v>
-      </c>
-      <c r="O21">
-        <v>0.6227221058909642</v>
-      </c>
-      <c r="Q21">
-        <v>0.3819160385100963</v>
-      </c>
-      <c r="R21">
-        <v>-0.2827927281285642</v>
-      </c>
-      <c r="S21">
-        <v>0.8936576820698581</v>
-      </c>
-      <c r="T21">
-        <v>0.1811080554343676</v>
-      </c>
-      <c r="U21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generate correlation tables for different group. Key question: marginal investers countercylical risks and skewness or not?
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>sp500</t>
   </si>
@@ -22,46 +22,40 @@
     <t>VIXCLS</t>
   </si>
   <si>
-    <t>meanMed</t>
+    <t>expMed</t>
   </si>
   <si>
     <t>iqrMed</t>
   </si>
   <si>
+    <t>skewMed</t>
+  </si>
+  <si>
     <t>varMed</t>
   </si>
   <si>
-    <t>rmeanMed</t>
+    <t>rexpMed</t>
   </si>
   <si>
     <t>rvarMed</t>
   </si>
   <si>
-    <t>meanMean</t>
+    <t>expMean</t>
   </si>
   <si>
     <t>iqrMean</t>
   </si>
   <si>
+    <t>skewMean</t>
+  </si>
+  <si>
     <t>varMean</t>
   </si>
   <si>
-    <t>rmeanMean</t>
+    <t>rexpMean</t>
   </si>
   <si>
     <t>rvarMean</t>
-  </si>
-  <si>
-    <t>kurtEstMed</t>
-  </si>
-  <si>
-    <t>skewEstMed</t>
-  </si>
-  <si>
-    <t>kurtEstMean</t>
-  </si>
-  <si>
-    <t>skewEstMean</t>
   </si>
 </sst>
 </file>
@@ -419,13 +413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,14 +462,8 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,46 +474,40 @@
         <v>-0.6793485726317077</v>
       </c>
       <c r="D2">
-        <v>-0.07483363088081939</v>
+        <v>0.01900127196260097</v>
       </c>
       <c r="E2">
-        <v>0.0605837209325372</v>
-      </c>
-      <c r="F2">
-        <v>0.09165378621206373</v>
+        <v>0.03133420968383937</v>
       </c>
       <c r="G2">
-        <v>-0.562449651783383</v>
+        <v>-0.0477042345053833</v>
       </c>
       <c r="H2">
-        <v>0.1464443784388182</v>
+        <v>-0.5439427537686055</v>
       </c>
       <c r="I2">
-        <v>0.02185912962278377</v>
+        <v>0.1553851987311239</v>
       </c>
       <c r="J2">
-        <v>0.2710843207654442</v>
+        <v>0.1131364112321919</v>
       </c>
       <c r="K2">
-        <v>0.2647490013995931</v>
+        <v>0.2057170850524637</v>
       </c>
       <c r="L2">
-        <v>-0.5866536696558399</v>
+        <v>0.1159509303126199</v>
       </c>
       <c r="M2">
-        <v>0.162241127660825</v>
+        <v>0.1371597428581595</v>
       </c>
       <c r="N2">
-        <v>2.249869722626098e-16</v>
-      </c>
-      <c r="P2">
-        <v>-0.08806881822253153</v>
-      </c>
-      <c r="Q2">
-        <v>-0.1895151414319372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>-0.5543767033263282</v>
+      </c>
+      <c r="O2">
+        <v>0.26905567318685</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -536,697 +518,525 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.01759041093037989</v>
+        <v>0.122307086479505</v>
       </c>
       <c r="E3">
-        <v>-0.0389481114345613</v>
-      </c>
-      <c r="F3">
-        <v>-0.04520710184843514</v>
+        <v>-0.05103253008539288</v>
       </c>
       <c r="G3">
-        <v>0.17154646284977</v>
+        <v>-0.02297459802873116</v>
       </c>
       <c r="H3">
-        <v>0.01769585812541223</v>
+        <v>0.1692287229715604</v>
       </c>
       <c r="I3">
-        <v>-0.09550244895406114</v>
+        <v>0.10450000631897</v>
       </c>
       <c r="J3">
-        <v>-0.1728841612412639</v>
+        <v>-0.01458300361159326</v>
       </c>
       <c r="K3">
-        <v>-0.1510466670382437</v>
+        <v>-0.08193998243922827</v>
       </c>
       <c r="L3">
-        <v>0.128872195788243</v>
+        <v>0.1199192369009568</v>
       </c>
       <c r="M3">
-        <v>0.04297091481733515</v>
+        <v>-0.03534885142615566</v>
       </c>
       <c r="N3">
-        <v>-2.715101058052503e-15</v>
-      </c>
-      <c r="P3">
-        <v>0.2275216406864242</v>
-      </c>
-      <c r="Q3">
-        <v>0.2347338694710326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>0.1433422830469426</v>
+      </c>
+      <c r="O3">
+        <v>0.02048539321331624</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.07483363088081939</v>
+        <v>0.01900127196260097</v>
       </c>
       <c r="C4">
-        <v>0.01759041093037989</v>
+        <v>0.122307086479505</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.3420098061521938</v>
-      </c>
-      <c r="F4">
-        <v>0.353135168584302</v>
+        <v>0.2354056370797766</v>
       </c>
       <c r="G4">
-        <v>0.580610016843249</v>
+        <v>0.2498737033226461</v>
       </c>
       <c r="H4">
-        <v>-0.07265401819163401</v>
+        <v>0.3318561611563087</v>
       </c>
       <c r="I4">
-        <v>0.8725898785101567</v>
+        <v>-0.05491478164945206</v>
       </c>
       <c r="J4">
-        <v>0.1998123665698788</v>
+        <v>0.7932631754163975</v>
       </c>
       <c r="K4">
-        <v>0.2025017344299468</v>
+        <v>0.1062750935389879</v>
       </c>
       <c r="L4">
-        <v>0.5101667631379072</v>
+        <v>0.2139466172649623</v>
       </c>
       <c r="M4">
-        <v>-0.003420558237110482</v>
+        <v>0.08360639206827794</v>
       </c>
       <c r="N4">
-        <v>-2.333815279120254e-15</v>
-      </c>
-      <c r="P4">
-        <v>-0.309148673882749</v>
-      </c>
-      <c r="Q4">
-        <v>0.5665499698028594</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>0.2714215984760107</v>
+      </c>
+      <c r="O4">
+        <v>-0.1140418579292497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.0605837209325372</v>
+        <v>0.03133420968383937</v>
       </c>
       <c r="C5">
-        <v>-0.0389481114345613</v>
+        <v>-0.05103253008539288</v>
       </c>
       <c r="D5">
-        <v>0.3420098061521938</v>
+        <v>0.2354056370797766</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0.9911163314339113</v>
-      </c>
       <c r="G5">
-        <v>0.07709134557571934</v>
+        <v>0.9618377395238186</v>
       </c>
       <c r="H5">
-        <v>0.8002955906427053</v>
+        <v>0.1636268557122579</v>
       </c>
       <c r="I5">
-        <v>0.6463343830641423</v>
+        <v>0.4782570876330713</v>
       </c>
       <c r="J5">
-        <v>0.8715252866363846</v>
+        <v>0.5906609348370248</v>
       </c>
       <c r="K5">
-        <v>0.7867844224644608</v>
+        <v>0.2730505612153954</v>
       </c>
       <c r="L5">
-        <v>0.1777355721812599</v>
+        <v>-0.06191247515392957</v>
       </c>
       <c r="M5">
-        <v>0.6304443735716682</v>
+        <v>0.04141686748499608</v>
       </c>
       <c r="N5">
-        <v>3.925747808330758e-15</v>
-      </c>
-      <c r="P5">
-        <v>0.0661792759032966</v>
-      </c>
-      <c r="Q5">
-        <v>0.1287674320613623</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>0.2503040623995599</v>
+      </c>
+      <c r="O5">
+        <v>0.2384170687519154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.09165378621206373</v>
-      </c>
-      <c r="C6">
-        <v>-0.04520710184843514</v>
-      </c>
-      <c r="D6">
-        <v>0.353135168584302</v>
-      </c>
-      <c r="E6">
-        <v>0.9911163314339113</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0.07395560470160355</v>
-      </c>
-      <c r="H6">
-        <v>0.8161702251891376</v>
-      </c>
-      <c r="I6">
-        <v>0.6541207049692819</v>
-      </c>
-      <c r="J6">
-        <v>0.8891462131489527</v>
-      </c>
-      <c r="K6">
-        <v>0.8122046680302711</v>
-      </c>
-      <c r="L6">
-        <v>0.1807232220615936</v>
-      </c>
-      <c r="M6">
-        <v>0.6455048211576415</v>
-      </c>
-      <c r="N6">
-        <v>1.018567689104012e-15</v>
-      </c>
-      <c r="P6">
-        <v>0.07805401158856294</v>
-      </c>
-      <c r="Q6">
-        <v>0.1095712728080283</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.562449651783383</v>
+        <v>-0.0477042345053833</v>
       </c>
       <c r="C7">
-        <v>0.17154646284977</v>
+        <v>-0.02297459802873116</v>
       </c>
       <c r="D7">
-        <v>0.580610016843249</v>
+        <v>0.2498737033226461</v>
       </c>
       <c r="E7">
-        <v>0.07709134557571934</v>
-      </c>
-      <c r="F7">
-        <v>0.07395560470160355</v>
+        <v>0.9618377395238186</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>-0.1398429802650279</v>
+        <v>0.174290153604561</v>
       </c>
       <c r="I7">
-        <v>0.4818880281947166</v>
+        <v>0.5360412771898042</v>
       </c>
       <c r="J7">
-        <v>-0.04658204859367849</v>
+        <v>0.5929561090438665</v>
       </c>
       <c r="K7">
-        <v>-0.02976883674366824</v>
+        <v>0.4002555309067126</v>
       </c>
       <c r="L7">
-        <v>0.9538235177682507</v>
+        <v>-0.0118378875854869</v>
       </c>
       <c r="M7">
-        <v>-0.1399548127558044</v>
+        <v>0.1885865908069941</v>
       </c>
       <c r="N7">
-        <v>2.537854193292807e-16</v>
-      </c>
-      <c r="P7">
-        <v>-0.1337922073884447</v>
-      </c>
-      <c r="Q7">
-        <v>0.239705259217227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>0.280013478887079</v>
+      </c>
+      <c r="O7">
+        <v>0.3019889134354288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.1464443784388182</v>
+        <v>-0.5439427537686055</v>
       </c>
       <c r="C8">
-        <v>0.01769585812541223</v>
+        <v>0.1692287229715604</v>
       </c>
       <c r="D8">
-        <v>-0.07265401819163401</v>
+        <v>0.3318561611563087</v>
       </c>
       <c r="E8">
-        <v>0.8002955906427053</v>
-      </c>
-      <c r="F8">
-        <v>0.8161702251891376</v>
+        <v>0.1636268557122579</v>
       </c>
       <c r="G8">
-        <v>-0.1398429802650279</v>
+        <v>0.174290153604561</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.2754120436524903</v>
+        <v>-0.2147641611430284</v>
       </c>
       <c r="J8">
-        <v>0.846761988204267</v>
+        <v>0.2720035216628864</v>
       </c>
       <c r="K8">
-        <v>0.7631818664317043</v>
+        <v>-0.1925543949982361</v>
       </c>
       <c r="L8">
-        <v>-0.05804359256587605</v>
+        <v>-0.3503965652180463</v>
       </c>
       <c r="M8">
-        <v>0.8254033223257329</v>
+        <v>-0.2095977340418683</v>
       </c>
       <c r="N8">
-        <v>3.340238619119773e-15</v>
-      </c>
-      <c r="P8">
-        <v>0.2793358451268426</v>
-      </c>
-      <c r="Q8">
-        <v>-0.1896673385614313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>0.9352047839076291</v>
+      </c>
+      <c r="O8">
+        <v>-0.3578611828781976</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.02185912962278377</v>
+        <v>0.1553851987311239</v>
       </c>
       <c r="C9">
-        <v>-0.09550244895406114</v>
+        <v>0.10450000631897</v>
       </c>
       <c r="D9">
-        <v>0.8725898785101567</v>
+        <v>-0.05491478164945206</v>
       </c>
       <c r="E9">
-        <v>0.6463343830641423</v>
-      </c>
-      <c r="F9">
-        <v>0.6541207049692819</v>
+        <v>0.4782570876330713</v>
       </c>
       <c r="G9">
-        <v>0.4818880281947166</v>
+        <v>0.5360412771898042</v>
       </c>
       <c r="H9">
-        <v>0.2754120436524903</v>
+        <v>-0.2147641611430284</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.5109744879001165</v>
+        <v>0.2859367739022057</v>
       </c>
       <c r="K9">
-        <v>0.4665181780328841</v>
+        <v>0.7815602909356424</v>
       </c>
       <c r="L9">
-        <v>0.5076179904358895</v>
+        <v>0.08069945908224707</v>
       </c>
       <c r="M9">
-        <v>0.2213529491100038</v>
+        <v>0.649547050690388</v>
       </c>
       <c r="N9">
-        <v>5.01264877179206e-15</v>
-      </c>
-      <c r="P9">
-        <v>-0.1897581480668075</v>
-      </c>
-      <c r="Q9">
-        <v>0.4664317794183128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>-0.1594513069986778</v>
+      </c>
+      <c r="O9">
+        <v>0.8892982652186254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.2710843207654442</v>
+        <v>0.1131364112321919</v>
       </c>
       <c r="C10">
-        <v>-0.1728841612412639</v>
+        <v>-0.01458300361159326</v>
       </c>
       <c r="D10">
-        <v>0.1998123665698788</v>
+        <v>0.7932631754163975</v>
       </c>
       <c r="E10">
-        <v>0.8715252866363846</v>
-      </c>
-      <c r="F10">
-        <v>0.8891462131489527</v>
+        <v>0.5906609348370248</v>
       </c>
       <c r="G10">
-        <v>-0.04658204859367849</v>
+        <v>0.5929561090438665</v>
       </c>
       <c r="H10">
-        <v>0.846761988204267</v>
+        <v>0.2720035216628864</v>
       </c>
       <c r="I10">
-        <v>0.5109744879001165</v>
+        <v>0.2859367739022057</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.9714663814495552</v>
+        <v>0.3773490726383463</v>
       </c>
       <c r="L10">
-        <v>0.03527371022733559</v>
+        <v>0.01685034629720496</v>
       </c>
       <c r="M10">
-        <v>0.8166295398196073</v>
+        <v>0.2417256759958273</v>
       </c>
       <c r="N10">
-        <v>-4.40903262349265e-15</v>
-      </c>
-      <c r="P10">
-        <v>-0.08794789747066932</v>
-      </c>
-      <c r="Q10">
-        <v>-0.07865315985536867</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>0.3479939689216099</v>
+      </c>
+      <c r="O10">
+        <v>0.1646604080287465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.2647490013995931</v>
+        <v>0.2057170850524637</v>
       </c>
       <c r="C11">
-        <v>-0.1510466670382437</v>
+        <v>-0.08193998243922827</v>
       </c>
       <c r="D11">
-        <v>0.2025017344299468</v>
+        <v>0.1062750935389879</v>
       </c>
       <c r="E11">
-        <v>0.7867844224644608</v>
-      </c>
-      <c r="F11">
-        <v>0.8122046680302711</v>
+        <v>0.2730505612153954</v>
       </c>
       <c r="G11">
-        <v>-0.02976883674366824</v>
+        <v>0.4002555309067126</v>
       </c>
       <c r="H11">
-        <v>0.7631818664317043</v>
+        <v>-0.1925543949982361</v>
       </c>
       <c r="I11">
-        <v>0.4665181780328841</v>
+        <v>0.7815602909356424</v>
       </c>
       <c r="J11">
-        <v>0.9714663814495552</v>
+        <v>0.3773490726383463</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.03558639420618973</v>
+        <v>0.2446340294363746</v>
       </c>
       <c r="M11">
-        <v>0.8206947611547886</v>
+        <v>0.9551656688247424</v>
       </c>
       <c r="N11">
-        <v>7.872665950443372e-15</v>
-      </c>
-      <c r="P11">
-        <v>-0.1577182903303236</v>
-      </c>
-      <c r="Q11">
-        <v>-0.1056212839727931</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>-0.08324012735031351</v>
+      </c>
+      <c r="O11">
+        <v>0.8189802687102239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.5866536696558399</v>
+        <v>0.1159509303126199</v>
       </c>
       <c r="C12">
-        <v>0.128872195788243</v>
+        <v>0.1199192369009568</v>
       </c>
       <c r="D12">
-        <v>0.5101667631379072</v>
+        <v>0.2139466172649623</v>
       </c>
       <c r="E12">
-        <v>0.1777355721812599</v>
-      </c>
-      <c r="F12">
-        <v>0.1807232220615936</v>
+        <v>-0.06191247515392957</v>
       </c>
       <c r="G12">
-        <v>0.9538235177682507</v>
+        <v>-0.0118378875854869</v>
       </c>
       <c r="H12">
-        <v>-0.05804359256587605</v>
+        <v>-0.3503965652180463</v>
       </c>
       <c r="I12">
-        <v>0.5076179904358895</v>
+        <v>0.08069945908224707</v>
       </c>
       <c r="J12">
-        <v>0.03527371022733559</v>
+        <v>0.01685034629720496</v>
       </c>
       <c r="K12">
-        <v>0.03558639420618973</v>
+        <v>0.2446340294363746</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>-0.1469416240727789</v>
+        <v>0.2905973125235088</v>
       </c>
       <c r="N12">
-        <v>1.250638284875952e-17</v>
-      </c>
-      <c r="P12">
-        <v>-0.08212577364749574</v>
-      </c>
-      <c r="Q12">
-        <v>0.2026330678233056</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>-0.3247693555069746</v>
+      </c>
+      <c r="O12">
+        <v>0.06142832729052807</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.162241127660825</v>
+        <v>0.1371597428581595</v>
       </c>
       <c r="C13">
-        <v>0.04297091481733515</v>
+        <v>-0.03534885142615566</v>
       </c>
       <c r="D13">
-        <v>-0.003420558237110482</v>
+        <v>0.08360639206827794</v>
       </c>
       <c r="E13">
-        <v>0.6304443735716682</v>
-      </c>
-      <c r="F13">
-        <v>0.6455048211576415</v>
+        <v>0.04141686748499608</v>
       </c>
       <c r="G13">
-        <v>-0.1399548127558044</v>
+        <v>0.1885865908069941</v>
       </c>
       <c r="H13">
-        <v>0.8254033223257329</v>
+        <v>-0.2095977340418683</v>
       </c>
       <c r="I13">
-        <v>0.2213529491100038</v>
+        <v>0.649547050690388</v>
       </c>
       <c r="J13">
-        <v>0.8166295398196073</v>
+        <v>0.2417256759958273</v>
       </c>
       <c r="K13">
-        <v>0.8206947611547886</v>
+        <v>0.9551656688247424</v>
       </c>
       <c r="L13">
-        <v>-0.1469416240727789</v>
+        <v>0.2905973125235088</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-7.508266900537718e-15</v>
-      </c>
-      <c r="P13">
-        <v>0.002584792154808971</v>
-      </c>
-      <c r="Q13">
-        <v>-0.1667968886159874</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>-0.1272157600967193</v>
+      </c>
+      <c r="O13">
+        <v>0.7545561183743013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.249869722626098e-16</v>
+        <v>-0.5543767033263282</v>
       </c>
       <c r="C14">
-        <v>-2.715101058052503e-15</v>
+        <v>0.1433422830469426</v>
       </c>
       <c r="D14">
-        <v>-2.333815279120254e-15</v>
+        <v>0.2714215984760107</v>
       </c>
       <c r="E14">
-        <v>3.925747808330758e-15</v>
-      </c>
-      <c r="F14">
-        <v>1.018567689104012e-15</v>
+        <v>0.2503040623995599</v>
       </c>
       <c r="G14">
-        <v>2.537854193292807e-16</v>
+        <v>0.280013478887079</v>
       </c>
       <c r="H14">
-        <v>3.340238619119773e-15</v>
+        <v>0.9352047839076291</v>
       </c>
       <c r="I14">
-        <v>5.01264877179206e-15</v>
+        <v>-0.1594513069986778</v>
       </c>
       <c r="J14">
-        <v>-4.40903262349265e-15</v>
+        <v>0.3479939689216099</v>
       </c>
       <c r="K14">
-        <v>7.872665950443372e-15</v>
+        <v>-0.08324012735031351</v>
       </c>
       <c r="L14">
-        <v>1.250638284875952e-17</v>
+        <v>-0.3247693555069746</v>
       </c>
       <c r="M14">
-        <v>-7.508266900537718e-15</v>
+        <v>-0.1272157600967193</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
-      <c r="P14">
-        <v>1.19330235870952e-15</v>
-      </c>
-      <c r="Q14">
-        <v>-1.280626059053519e-15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="O14">
+        <v>-0.3344955454540742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>-0.08806881822253153</v>
-      </c>
-      <c r="C16">
-        <v>0.2275216406864242</v>
-      </c>
-      <c r="D16">
-        <v>-0.309148673882749</v>
-      </c>
-      <c r="E16">
-        <v>0.0661792759032966</v>
-      </c>
-      <c r="F16">
-        <v>0.07805401158856294</v>
-      </c>
-      <c r="G16">
-        <v>-0.1337922073884447</v>
-      </c>
-      <c r="H16">
-        <v>0.2793358451268426</v>
-      </c>
-      <c r="I16">
-        <v>-0.1897581480668075</v>
-      </c>
-      <c r="J16">
-        <v>-0.08794789747066932</v>
-      </c>
-      <c r="K16">
-        <v>-0.1577182903303236</v>
-      </c>
-      <c r="L16">
-        <v>-0.08212577364749574</v>
-      </c>
-      <c r="M16">
-        <v>0.002584792154808971</v>
-      </c>
-      <c r="N16">
-        <v>1.19330235870952e-15</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>-0.01196058651824267</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>-0.1895151414319372</v>
-      </c>
-      <c r="C17">
-        <v>0.2347338694710326</v>
-      </c>
-      <c r="D17">
-        <v>0.5665499698028594</v>
-      </c>
-      <c r="E17">
-        <v>0.1287674320613623</v>
-      </c>
-      <c r="F17">
-        <v>0.1095712728080283</v>
-      </c>
-      <c r="G17">
-        <v>0.239705259217227</v>
-      </c>
-      <c r="H17">
-        <v>-0.1896673385614313</v>
-      </c>
-      <c r="I17">
-        <v>0.4664317794183128</v>
-      </c>
-      <c r="J17">
-        <v>-0.07865315985536867</v>
-      </c>
-      <c r="K17">
-        <v>-0.1056212839727931</v>
-      </c>
-      <c r="L17">
-        <v>0.2026330678233056</v>
-      </c>
-      <c r="M17">
-        <v>-0.1667968886159874</v>
-      </c>
-      <c r="N17">
-        <v>-1.280626059053519e-15</v>
-      </c>
-      <c r="P17">
-        <v>-0.01196058651824267</v>
-      </c>
-      <c r="Q17">
+      <c r="B15">
+        <v>0.26905567318685</v>
+      </c>
+      <c r="C15">
+        <v>0.02048539321331624</v>
+      </c>
+      <c r="D15">
+        <v>-0.1140418579292497</v>
+      </c>
+      <c r="E15">
+        <v>0.2384170687519154</v>
+      </c>
+      <c r="G15">
+        <v>0.3019889134354288</v>
+      </c>
+      <c r="H15">
+        <v>-0.3578611828781976</v>
+      </c>
+      <c r="I15">
+        <v>0.8892982652186254</v>
+      </c>
+      <c r="J15">
+        <v>0.1646604080287465</v>
+      </c>
+      <c r="K15">
+        <v>0.8189802687102239</v>
+      </c>
+      <c r="L15">
+        <v>0.06142832729052807</v>
+      </c>
+      <c r="M15">
+        <v>0.7545561183743013</v>
+      </c>
+      <c r="N15">
+        <v>-0.3344955454540742</v>
+      </c>
+      <c r="O15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. newey we west standard errors. 2. cross-correaltion plot.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -474,37 +474,37 @@
         <v>-0.6793485726317077</v>
       </c>
       <c r="D2">
-        <v>0.01900127196260097</v>
+        <v>0.05284710587315838</v>
       </c>
       <c r="E2">
-        <v>0.03133420968383937</v>
+        <v>0.02550090984167503</v>
       </c>
       <c r="G2">
-        <v>-0.0477042345053833</v>
+        <v>-0.04502025361393325</v>
       </c>
       <c r="H2">
-        <v>-0.5439427537686055</v>
+        <v>-0.5352988047422513</v>
       </c>
       <c r="I2">
-        <v>0.1553851987311239</v>
+        <v>0.1490515468083845</v>
       </c>
       <c r="J2">
-        <v>0.1131364112321919</v>
+        <v>0.1371387993843627</v>
       </c>
       <c r="K2">
-        <v>0.2057170850524637</v>
+        <v>0.200626606284561</v>
       </c>
       <c r="L2">
-        <v>0.1159509303126199</v>
+        <v>0.1079330116962531</v>
       </c>
       <c r="M2">
-        <v>0.1371597428581595</v>
+        <v>0.129293823016267</v>
       </c>
       <c r="N2">
-        <v>-0.5543767033263282</v>
+        <v>-0.5502255047420385</v>
       </c>
       <c r="O2">
-        <v>0.26905567318685</v>
+        <v>0.2537685189959536</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -518,37 +518,37 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.122307086479505</v>
+        <v>0.1183818032404943</v>
       </c>
       <c r="E3">
-        <v>-0.05103253008539288</v>
+        <v>-0.0427249620654119</v>
       </c>
       <c r="G3">
-        <v>-0.02297459802873116</v>
+        <v>-0.01940981040636119</v>
       </c>
       <c r="H3">
-        <v>0.1692287229715604</v>
+        <v>0.1686289861464561</v>
       </c>
       <c r="I3">
-        <v>0.10450000631897</v>
+        <v>0.1051672521303078</v>
       </c>
       <c r="J3">
-        <v>-0.01458300361159326</v>
+        <v>-0.01637347079980878</v>
       </c>
       <c r="K3">
-        <v>-0.08193998243922827</v>
+        <v>-0.07889299984295564</v>
       </c>
       <c r="L3">
-        <v>0.1199192369009568</v>
+        <v>0.1237571271336534</v>
       </c>
       <c r="M3">
-        <v>-0.03534885142615566</v>
+        <v>-0.03019904530512181</v>
       </c>
       <c r="N3">
-        <v>0.1433422830469426</v>
+        <v>0.1411896716252118</v>
       </c>
       <c r="O3">
-        <v>0.02048539321331624</v>
+        <v>0.02761189664673756</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -556,43 +556,43 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.01900127196260097</v>
+        <v>0.05284710587315838</v>
       </c>
       <c r="C4">
-        <v>0.122307086479505</v>
+        <v>0.1183818032404943</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.2354056370797766</v>
+        <v>0.2862096796565572</v>
       </c>
       <c r="G4">
-        <v>0.2498737033226461</v>
+        <v>0.2858119586419813</v>
       </c>
       <c r="H4">
-        <v>0.3318561611563087</v>
+        <v>0.3208449815547014</v>
       </c>
       <c r="I4">
-        <v>-0.05491478164945206</v>
+        <v>-0.03615914419776285</v>
       </c>
       <c r="J4">
-        <v>0.7932631754163975</v>
+        <v>0.8042684740305435</v>
       </c>
       <c r="K4">
-        <v>0.1062750935389879</v>
+        <v>0.1010925659905756</v>
       </c>
       <c r="L4">
-        <v>0.2139466172649623</v>
+        <v>0.1766723565517075</v>
       </c>
       <c r="M4">
-        <v>0.08360639206827794</v>
+        <v>0.06202386746339025</v>
       </c>
       <c r="N4">
-        <v>0.2714215984760107</v>
+        <v>0.2608281976605054</v>
       </c>
       <c r="O4">
-        <v>-0.1140418579292497</v>
+        <v>-0.09255504229564779</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -600,43 +600,43 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.03133420968383937</v>
+        <v>0.02550090984167503</v>
       </c>
       <c r="C5">
-        <v>-0.05103253008539288</v>
+        <v>-0.0427249620654119</v>
       </c>
       <c r="D5">
-        <v>0.2354056370797766</v>
+        <v>0.2862096796565572</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.9618377395238186</v>
+        <v>0.9628637223458245</v>
       </c>
       <c r="H5">
-        <v>0.1636268557122579</v>
+        <v>0.1878429442749909</v>
       </c>
       <c r="I5">
-        <v>0.4782570876330713</v>
+        <v>0.4840581834101727</v>
       </c>
       <c r="J5">
-        <v>0.5906609348370248</v>
+        <v>0.622812431914202</v>
       </c>
       <c r="K5">
-        <v>0.2730505612153954</v>
+        <v>0.2977848790824405</v>
       </c>
       <c r="L5">
-        <v>-0.06191247515392957</v>
+        <v>-0.05749781206784608</v>
       </c>
       <c r="M5">
-        <v>0.04141686748499608</v>
+        <v>0.07471037506210082</v>
       </c>
       <c r="N5">
-        <v>0.2503040623995599</v>
+        <v>0.2627015921725792</v>
       </c>
       <c r="O5">
-        <v>0.2384170687519154</v>
+        <v>0.2515737508594499</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -649,43 +649,43 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.0477042345053833</v>
+        <v>-0.04502025361393325</v>
       </c>
       <c r="C7">
-        <v>-0.02297459802873116</v>
+        <v>-0.01940981040636119</v>
       </c>
       <c r="D7">
-        <v>0.2498737033226461</v>
+        <v>0.2858119586419813</v>
       </c>
       <c r="E7">
-        <v>0.9618377395238186</v>
+        <v>0.9628637223458245</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.174290153604561</v>
+        <v>0.1850100977435571</v>
       </c>
       <c r="I7">
-        <v>0.5360412771898042</v>
+        <v>0.5389219049867383</v>
       </c>
       <c r="J7">
-        <v>0.5929561090438665</v>
+        <v>0.6093980989173357</v>
       </c>
       <c r="K7">
-        <v>0.4002555309067126</v>
+        <v>0.4163707152817249</v>
       </c>
       <c r="L7">
-        <v>-0.0118378875854869</v>
+        <v>-0.01143832450566349</v>
       </c>
       <c r="M7">
-        <v>0.1885865908069941</v>
+        <v>0.2112297758292304</v>
       </c>
       <c r="N7">
-        <v>0.280013478887079</v>
+        <v>0.2815185517408797</v>
       </c>
       <c r="O7">
-        <v>0.3019889134354288</v>
+        <v>0.3159095033480881</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -693,43 +693,43 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.5439427537686055</v>
+        <v>-0.5352988047422513</v>
       </c>
       <c r="C8">
-        <v>0.1692287229715604</v>
+        <v>0.1686289861464561</v>
       </c>
       <c r="D8">
-        <v>0.3318561611563087</v>
+        <v>0.3208449815547014</v>
       </c>
       <c r="E8">
-        <v>0.1636268557122579</v>
+        <v>0.1878429442749909</v>
       </c>
       <c r="G8">
-        <v>0.174290153604561</v>
+        <v>0.1850100977435571</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>-0.2147641611430284</v>
+        <v>-0.2213412639926016</v>
       </c>
       <c r="J8">
-        <v>0.2720035216628864</v>
+        <v>0.2664628392334352</v>
       </c>
       <c r="K8">
-        <v>-0.1925543949982361</v>
+        <v>-0.1960758592444096</v>
       </c>
       <c r="L8">
-        <v>-0.3503965652180463</v>
+        <v>-0.347064490796336</v>
       </c>
       <c r="M8">
-        <v>-0.2095977340418683</v>
+        <v>-0.2171218224399398</v>
       </c>
       <c r="N8">
-        <v>0.9352047839076291</v>
+        <v>0.9352104838129371</v>
       </c>
       <c r="O8">
-        <v>-0.3578611828781976</v>
+        <v>-0.3576867119968038</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -737,43 +737,43 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1553851987311239</v>
+        <v>0.1490515468083845</v>
       </c>
       <c r="C9">
-        <v>0.10450000631897</v>
+        <v>0.1051672521303078</v>
       </c>
       <c r="D9">
-        <v>-0.05491478164945206</v>
+        <v>-0.03615914419776285</v>
       </c>
       <c r="E9">
-        <v>0.4782570876330713</v>
+        <v>0.4840581834101727</v>
       </c>
       <c r="G9">
-        <v>0.5360412771898042</v>
+        <v>0.5389219049867383</v>
       </c>
       <c r="H9">
-        <v>-0.2147641611430284</v>
+        <v>-0.2213412639926016</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.2859367739022057</v>
+        <v>0.2862144791013954</v>
       </c>
       <c r="K9">
-        <v>0.7815602909356424</v>
+        <v>0.7884343634426342</v>
       </c>
       <c r="L9">
-        <v>0.08069945908224707</v>
+        <v>0.08087592040379925</v>
       </c>
       <c r="M9">
-        <v>0.649547050690388</v>
+        <v>0.6644814596677858</v>
       </c>
       <c r="N9">
-        <v>-0.1594513069986778</v>
+        <v>-0.1612105954626258</v>
       </c>
       <c r="O9">
-        <v>0.8892982652186254</v>
+        <v>0.8915350258456595</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -781,43 +781,43 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1131364112321919</v>
+        <v>0.1371387993843627</v>
       </c>
       <c r="C10">
-        <v>-0.01458300361159326</v>
+        <v>-0.01637347079980878</v>
       </c>
       <c r="D10">
-        <v>0.7932631754163975</v>
+        <v>0.8042684740305435</v>
       </c>
       <c r="E10">
-        <v>0.5906609348370248</v>
+        <v>0.622812431914202</v>
       </c>
       <c r="G10">
-        <v>0.5929561090438665</v>
+        <v>0.6093980989173357</v>
       </c>
       <c r="H10">
-        <v>0.2720035216628864</v>
+        <v>0.2664628392334352</v>
       </c>
       <c r="I10">
-        <v>0.2859367739022057</v>
+        <v>0.2862144791013954</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.3773490726383463</v>
+        <v>0.3730356032872126</v>
       </c>
       <c r="L10">
-        <v>0.01685034629720496</v>
+        <v>-0.005120395540669093</v>
       </c>
       <c r="M10">
-        <v>0.2417256759958273</v>
+        <v>0.2336922242139398</v>
       </c>
       <c r="N10">
-        <v>0.3479939689216099</v>
+        <v>0.3370899062620499</v>
       </c>
       <c r="O10">
-        <v>0.1646604080287465</v>
+        <v>0.1816867800423102</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -825,43 +825,43 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.2057170850524637</v>
+        <v>0.200626606284561</v>
       </c>
       <c r="C11">
-        <v>-0.08193998243922827</v>
+        <v>-0.07889299984295564</v>
       </c>
       <c r="D11">
-        <v>0.1062750935389879</v>
+        <v>0.1010925659905756</v>
       </c>
       <c r="E11">
-        <v>0.2730505612153954</v>
+        <v>0.2977848790824405</v>
       </c>
       <c r="G11">
-        <v>0.4002555309067126</v>
+        <v>0.4163707152817249</v>
       </c>
       <c r="H11">
-        <v>-0.1925543949982361</v>
+        <v>-0.1960758592444096</v>
       </c>
       <c r="I11">
-        <v>0.7815602909356424</v>
+        <v>0.7884343634426342</v>
       </c>
       <c r="J11">
-        <v>0.3773490726383463</v>
+        <v>0.3730356032872126</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.2446340294363746</v>
+        <v>0.2273945170531899</v>
       </c>
       <c r="M11">
-        <v>0.9551656688247424</v>
+        <v>0.9569216284928839</v>
       </c>
       <c r="N11">
-        <v>-0.08324012735031351</v>
+        <v>-0.07720906754130509</v>
       </c>
       <c r="O11">
-        <v>0.8189802687102239</v>
+        <v>0.8213573610483902</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -869,43 +869,43 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1159509303126199</v>
+        <v>0.1079330116962531</v>
       </c>
       <c r="C12">
-        <v>0.1199192369009568</v>
+        <v>0.1237571271336534</v>
       </c>
       <c r="D12">
-        <v>0.2139466172649623</v>
+        <v>0.1766723565517075</v>
       </c>
       <c r="E12">
-        <v>-0.06191247515392957</v>
+        <v>-0.05749781206784608</v>
       </c>
       <c r="G12">
-        <v>-0.0118378875854869</v>
+        <v>-0.01143832450566349</v>
       </c>
       <c r="H12">
-        <v>-0.3503965652180463</v>
+        <v>-0.347064490796336</v>
       </c>
       <c r="I12">
-        <v>0.08069945908224707</v>
+        <v>0.08087592040379925</v>
       </c>
       <c r="J12">
-        <v>0.01685034629720496</v>
+        <v>-0.005120395540669093</v>
       </c>
       <c r="K12">
-        <v>0.2446340294363746</v>
+        <v>0.2273945170531899</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.2905973125235088</v>
+        <v>0.266688302155974</v>
       </c>
       <c r="N12">
-        <v>-0.3247693555069746</v>
+        <v>-0.3127709963931993</v>
       </c>
       <c r="O12">
-        <v>0.06142832729052807</v>
+        <v>0.044570176597717</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -913,43 +913,43 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.1371597428581595</v>
+        <v>0.129293823016267</v>
       </c>
       <c r="C13">
-        <v>-0.03534885142615566</v>
+        <v>-0.03019904530512181</v>
       </c>
       <c r="D13">
-        <v>0.08360639206827794</v>
+        <v>0.06202386746339025</v>
       </c>
       <c r="E13">
-        <v>0.04141686748499608</v>
+        <v>0.07471037506210082</v>
       </c>
       <c r="G13">
-        <v>0.1885865908069941</v>
+        <v>0.2112297758292304</v>
       </c>
       <c r="H13">
-        <v>-0.2095977340418683</v>
+        <v>-0.2171218224399398</v>
       </c>
       <c r="I13">
-        <v>0.649547050690388</v>
+        <v>0.6644814596677858</v>
       </c>
       <c r="J13">
-        <v>0.2417256759958273</v>
+        <v>0.2336922242139398</v>
       </c>
       <c r="K13">
-        <v>0.9551656688247424</v>
+        <v>0.9569216284928839</v>
       </c>
       <c r="L13">
-        <v>0.2905973125235088</v>
+        <v>0.266688302155974</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-0.1272157600967193</v>
+        <v>-0.1188419959597674</v>
       </c>
       <c r="O13">
-        <v>0.7545561183743013</v>
+        <v>0.7602727279385658</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -957,43 +957,43 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.5543767033263282</v>
+        <v>-0.5502255047420385</v>
       </c>
       <c r="C14">
-        <v>0.1433422830469426</v>
+        <v>0.1411896716252118</v>
       </c>
       <c r="D14">
-        <v>0.2714215984760107</v>
+        <v>0.2608281976605054</v>
       </c>
       <c r="E14">
-        <v>0.2503040623995599</v>
+        <v>0.2627015921725792</v>
       </c>
       <c r="G14">
-        <v>0.280013478887079</v>
+        <v>0.2815185517408797</v>
       </c>
       <c r="H14">
-        <v>0.9352047839076291</v>
+        <v>0.9352104838129371</v>
       </c>
       <c r="I14">
-        <v>-0.1594513069986778</v>
+        <v>-0.1612105954626258</v>
       </c>
       <c r="J14">
-        <v>0.3479939689216099</v>
+        <v>0.3370899062620499</v>
       </c>
       <c r="K14">
-        <v>-0.08324012735031351</v>
+        <v>-0.07720906754130509</v>
       </c>
       <c r="L14">
-        <v>-0.3247693555069746</v>
+        <v>-0.3127709963931993</v>
       </c>
       <c r="M14">
-        <v>-0.1272157600967193</v>
+        <v>-0.1188419959597674</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>-0.3344955454540742</v>
+        <v>-0.3259720137548081</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1001,40 +1001,40 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.26905567318685</v>
+        <v>0.2537685189959536</v>
       </c>
       <c r="C15">
-        <v>0.02048539321331624</v>
+        <v>0.02761189664673756</v>
       </c>
       <c r="D15">
-        <v>-0.1140418579292497</v>
+        <v>-0.09255504229564779</v>
       </c>
       <c r="E15">
-        <v>0.2384170687519154</v>
+        <v>0.2515737508594499</v>
       </c>
       <c r="G15">
-        <v>0.3019889134354288</v>
+        <v>0.3159095033480881</v>
       </c>
       <c r="H15">
-        <v>-0.3578611828781976</v>
+        <v>-0.3576867119968038</v>
       </c>
       <c r="I15">
-        <v>0.8892982652186254</v>
+        <v>0.8915350258456595</v>
       </c>
       <c r="J15">
-        <v>0.1646604080287465</v>
+        <v>0.1816867800423102</v>
       </c>
       <c r="K15">
-        <v>0.8189802687102239</v>
+        <v>0.8213573610483902</v>
       </c>
       <c r="L15">
-        <v>0.06142832729052807</v>
+        <v>0.044570176597717</v>
       </c>
       <c r="M15">
-        <v>0.7545561183743013</v>
+        <v>0.7602727279385658</v>
       </c>
       <c r="N15">
-        <v>-0.3344955454540742</v>
+        <v>-0.3259720137548081</v>
       </c>
       <c r="O15">
         <v>1</v>

</xml_diff>

<commit_message>
updated abstract including learning model.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -471,40 +471,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.6793485726317077</v>
+        <v>-0.7515833566942681</v>
       </c>
       <c r="D2">
-        <v>0.05284710587315838</v>
+        <v>-0.1211002744327765</v>
       </c>
       <c r="E2">
-        <v>0.02550090984167503</v>
+        <v>-0.03198733403962323</v>
       </c>
       <c r="G2">
-        <v>-0.04502025361393325</v>
+        <v>-0.03067636664815504</v>
       </c>
       <c r="H2">
-        <v>-0.5352988047422513</v>
+        <v>-0.2128317531051811</v>
       </c>
       <c r="I2">
-        <v>0.1490515468083845</v>
+        <v>-0.04909269184698396</v>
       </c>
       <c r="J2">
-        <v>0.1371387993843627</v>
+        <v>-0.109523284579041</v>
       </c>
       <c r="K2">
-        <v>0.200626606284561</v>
+        <v>0.07145745119241201</v>
       </c>
       <c r="L2">
-        <v>0.1079330116962531</v>
+        <v>-0.09569154803023676</v>
       </c>
       <c r="M2">
-        <v>0.129293823016267</v>
+        <v>0.03524498611133097</v>
       </c>
       <c r="N2">
-        <v>-0.5502255047420385</v>
+        <v>-0.238878242919409</v>
       </c>
       <c r="O2">
-        <v>0.2537685189959536</v>
+        <v>0.05244044240843464</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.6793485726317077</v>
+        <v>-0.7515833566942681</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -556,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.05284710587315838</v>
+        <v>-0.1211002744327765</v>
       </c>
       <c r="C4">
         <v>0.1183818032404943</v>
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.02550090984167503</v>
+        <v>-0.03198733403962323</v>
       </c>
       <c r="C5">
         <v>-0.0427249620654119</v>
@@ -649,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.04502025361393325</v>
+        <v>-0.03067636664815504</v>
       </c>
       <c r="C7">
         <v>-0.01940981040636119</v>
@@ -693,7 +693,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.5352988047422513</v>
+        <v>-0.2128317531051811</v>
       </c>
       <c r="C8">
         <v>0.1686289861464561</v>
@@ -737,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1490515468083845</v>
+        <v>-0.04909269184698396</v>
       </c>
       <c r="C9">
         <v>0.1051672521303078</v>
@@ -781,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1371387993843627</v>
+        <v>-0.109523284579041</v>
       </c>
       <c r="C10">
         <v>-0.01637347079980878</v>
@@ -825,7 +825,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.200626606284561</v>
+        <v>0.07145745119241201</v>
       </c>
       <c r="C11">
         <v>-0.07889299984295564</v>
@@ -869,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1079330116962531</v>
+        <v>-0.09569154803023676</v>
       </c>
       <c r="C12">
         <v>0.1237571271336534</v>
@@ -913,7 +913,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.129293823016267</v>
+        <v>0.03524498611133097</v>
       </c>
       <c r="C13">
         <v>-0.03019904530512181</v>
@@ -957,7 +957,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.5502255047420385</v>
+        <v>-0.238878242919409</v>
       </c>
       <c r="C14">
         <v>0.1411896716252118</v>
@@ -1001,7 +1001,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.2537685189959536</v>
+        <v>0.05244044240843464</v>
       </c>
       <c r="C15">
         <v>0.02761189664673756</v>

</xml_diff>

<commit_message>
draft with theory. Very rought. Need to debug reference, link, graph size.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>sp500</t>
   </si>
   <si>
     <t>VIXCLS</t>
+  </si>
+  <si>
+    <t>he</t>
   </si>
   <si>
     <t>expMed</t>
@@ -413,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +465,11 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,40 +480,43 @@
         <v>-0.7515833566942681</v>
       </c>
       <c r="D2">
+        <v>-0.2110384727942434</v>
+      </c>
+      <c r="E2">
         <v>-0.1211002744327765</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-0.03198733403962323</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-0.03067636664815504</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>-0.2128317531051811</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-0.04909269184698396</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-0.109523284579041</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.07145745119241201</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>-0.09569154803023676</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.03524498611133097</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>-0.238878242919409</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.05244044240843464</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -518,525 +527,608 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <v>0.1988341993235634</v>
+      </c>
+      <c r="E3">
         <v>0.1183818032404943</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-0.0427249620654119</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-0.01940981040636119</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.1686289861464561</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.1051672521303078</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-0.01637347079980878</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>-0.07889299984295564</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.1237571271336534</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>-0.03019904530512181</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.1411896716252118</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.02761189664673756</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.1211002744327765</v>
+        <v>-0.2110384727942434</v>
       </c>
       <c r="C4">
-        <v>0.1183818032404943</v>
+        <v>0.1988341993235634</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.2862096796565572</v>
-      </c>
-      <c r="G4">
-        <v>0.2858119586419813</v>
+        <v>0.4004509642697959</v>
+      </c>
+      <c r="F4">
+        <v>-0.2809081383745311</v>
       </c>
       <c r="H4">
-        <v>0.3208449815547014</v>
+        <v>-0.3160885375969492</v>
       </c>
       <c r="I4">
-        <v>-0.03615914419776285</v>
+        <v>0.432172463729226</v>
       </c>
       <c r="J4">
-        <v>0.8042684740305435</v>
+        <v>-0.6574251904662259</v>
       </c>
       <c r="K4">
-        <v>0.1010925659905756</v>
+        <v>-0.01695605734072748</v>
       </c>
       <c r="L4">
-        <v>0.1766723565517075</v>
+        <v>-0.5317768186373113</v>
       </c>
       <c r="M4">
-        <v>0.06202386746339025</v>
+        <v>0.1098763086986835</v>
       </c>
       <c r="N4">
-        <v>0.2608281976605054</v>
+        <v>-0.4077551084877684</v>
       </c>
       <c r="O4">
-        <v>-0.09255504229564779</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>0.3152940205507497</v>
+      </c>
+      <c r="P4">
+        <v>-0.6703348258304175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.03198733403962323</v>
+        <v>-0.1211002744327765</v>
       </c>
       <c r="C5">
-        <v>-0.0427249620654119</v>
+        <v>0.1183818032404943</v>
       </c>
       <c r="D5">
+        <v>0.4004509642697959</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>0.2862096796565572</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0.9628637223458245</v>
-      </c>
       <c r="H5">
-        <v>0.1878429442749909</v>
+        <v>0.2858119586419813</v>
       </c>
       <c r="I5">
-        <v>0.4840581834101727</v>
+        <v>0.3208449815547014</v>
       </c>
       <c r="J5">
-        <v>0.622812431914202</v>
+        <v>-0.03615914419776285</v>
       </c>
       <c r="K5">
-        <v>0.2977848790824405</v>
+        <v>0.8042684740305435</v>
       </c>
       <c r="L5">
-        <v>-0.05749781206784608</v>
+        <v>0.1010925659905756</v>
       </c>
       <c r="M5">
-        <v>0.07471037506210082</v>
+        <v>0.1766723565517075</v>
       </c>
       <c r="N5">
-        <v>0.2627015921725792</v>
+        <v>0.06202386746339025</v>
       </c>
       <c r="O5">
-        <v>0.2515737508594499</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>0.2608281976605054</v>
+      </c>
+      <c r="P5">
+        <v>-0.09255504229564779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="B6">
+        <v>-0.03198733403962323</v>
+      </c>
+      <c r="C6">
+        <v>-0.0427249620654119</v>
+      </c>
+      <c r="D6">
+        <v>-0.2809081383745311</v>
+      </c>
+      <c r="E6">
+        <v>0.2862096796565572</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.9628637223458245</v>
+      </c>
+      <c r="I6">
+        <v>0.1878429442749909</v>
+      </c>
+      <c r="J6">
+        <v>0.4840581834101727</v>
+      </c>
+      <c r="K6">
+        <v>0.622812431914202</v>
+      </c>
+      <c r="L6">
+        <v>0.2977848790824405</v>
+      </c>
+      <c r="M6">
+        <v>-0.05749781206784608</v>
+      </c>
+      <c r="N6">
+        <v>0.07471037506210082</v>
+      </c>
+      <c r="O6">
+        <v>0.2627015921725792</v>
+      </c>
+      <c r="P6">
+        <v>0.2515737508594499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>-0.03067636664815504</v>
-      </c>
-      <c r="C7">
-        <v>-0.01940981040636119</v>
-      </c>
-      <c r="D7">
-        <v>0.2858119586419813</v>
-      </c>
-      <c r="E7">
-        <v>0.9628637223458245</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0.1850100977435571</v>
-      </c>
-      <c r="I7">
-        <v>0.5389219049867383</v>
-      </c>
-      <c r="J7">
-        <v>0.6093980989173357</v>
-      </c>
-      <c r="K7">
-        <v>0.4163707152817249</v>
-      </c>
-      <c r="L7">
-        <v>-0.01143832450566349</v>
-      </c>
-      <c r="M7">
-        <v>0.2112297758292304</v>
-      </c>
-      <c r="N7">
-        <v>0.2815185517408797</v>
-      </c>
-      <c r="O7">
-        <v>0.3159095033480881</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.2128317531051811</v>
+        <v>-0.03067636664815504</v>
       </c>
       <c r="C8">
-        <v>0.1686289861464561</v>
+        <v>-0.01940981040636119</v>
       </c>
       <c r="D8">
-        <v>0.3208449815547014</v>
+        <v>-0.3160885375969492</v>
       </c>
       <c r="E8">
-        <v>0.1878429442749909</v>
-      </c>
-      <c r="G8">
+        <v>0.2858119586419813</v>
+      </c>
+      <c r="F8">
+        <v>0.9628637223458245</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>0.1850100977435571</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>-0.2213412639926016</v>
-      </c>
       <c r="J8">
-        <v>0.2664628392334352</v>
+        <v>0.5389219049867383</v>
       </c>
       <c r="K8">
-        <v>-0.1960758592444096</v>
+        <v>0.6093980989173357</v>
       </c>
       <c r="L8">
-        <v>-0.347064490796336</v>
+        <v>0.4163707152817249</v>
       </c>
       <c r="M8">
-        <v>-0.2171218224399398</v>
+        <v>-0.01143832450566349</v>
       </c>
       <c r="N8">
-        <v>0.9352104838129371</v>
+        <v>0.2112297758292304</v>
       </c>
       <c r="O8">
-        <v>-0.3576867119968038</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>0.2815185517408797</v>
+      </c>
+      <c r="P8">
+        <v>0.3159095033480881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.04909269184698396</v>
+        <v>-0.2128317531051811</v>
       </c>
       <c r="C9">
-        <v>0.1051672521303078</v>
+        <v>0.1686289861464561</v>
       </c>
       <c r="D9">
-        <v>-0.03615914419776285</v>
+        <v>0.432172463729226</v>
       </c>
       <c r="E9">
-        <v>0.4840581834101727</v>
-      </c>
-      <c r="G9">
-        <v>0.5389219049867383</v>
+        <v>0.3208449815547014</v>
+      </c>
+      <c r="F9">
+        <v>0.1878429442749909</v>
       </c>
       <c r="H9">
+        <v>0.1850100977435571</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>-0.2213412639926016</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.2862144791013954</v>
-      </c>
       <c r="K9">
-        <v>0.7884343634426342</v>
+        <v>0.2664628392334352</v>
       </c>
       <c r="L9">
-        <v>0.08087592040379925</v>
+        <v>-0.1960758592444096</v>
       </c>
       <c r="M9">
-        <v>0.6644814596677858</v>
+        <v>-0.347064490796336</v>
       </c>
       <c r="N9">
-        <v>-0.1612105954626258</v>
+        <v>-0.2171218224399398</v>
       </c>
       <c r="O9">
-        <v>0.8915350258456595</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>0.9352104838129371</v>
+      </c>
+      <c r="P9">
+        <v>-0.3576867119968038</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.109523284579041</v>
+        <v>-0.04909269184698396</v>
       </c>
       <c r="C10">
-        <v>-0.01637347079980878</v>
+        <v>0.1051672521303078</v>
       </c>
       <c r="D10">
-        <v>0.8042684740305435</v>
+        <v>-0.6574251904662259</v>
       </c>
       <c r="E10">
-        <v>0.622812431914202</v>
-      </c>
-      <c r="G10">
-        <v>0.6093980989173357</v>
+        <v>-0.03615914419776285</v>
+      </c>
+      <c r="F10">
+        <v>0.4840581834101727</v>
       </c>
       <c r="H10">
-        <v>0.2664628392334352</v>
+        <v>0.5389219049867383</v>
       </c>
       <c r="I10">
+        <v>-0.2213412639926016</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>0.2862144791013954</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>0.3730356032872126</v>
-      </c>
       <c r="L10">
-        <v>-0.005120395540669093</v>
+        <v>0.7884343634426342</v>
       </c>
       <c r="M10">
-        <v>0.2336922242139398</v>
+        <v>0.08087592040379925</v>
       </c>
       <c r="N10">
-        <v>0.3370899062620499</v>
+        <v>0.6644814596677858</v>
       </c>
       <c r="O10">
-        <v>0.1816867800423102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>-0.1612105954626258</v>
+      </c>
+      <c r="P10">
+        <v>0.8915350258456595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.07145745119241201</v>
+        <v>-0.109523284579041</v>
       </c>
       <c r="C11">
-        <v>-0.07889299984295564</v>
+        <v>-0.01637347079980878</v>
       </c>
       <c r="D11">
-        <v>0.1010925659905756</v>
+        <v>-0.01695605734072748</v>
       </c>
       <c r="E11">
-        <v>0.2977848790824405</v>
-      </c>
-      <c r="G11">
-        <v>0.4163707152817249</v>
+        <v>0.8042684740305435</v>
+      </c>
+      <c r="F11">
+        <v>0.622812431914202</v>
       </c>
       <c r="H11">
-        <v>-0.1960758592444096</v>
+        <v>0.6093980989173357</v>
       </c>
       <c r="I11">
-        <v>0.7884343634426342</v>
+        <v>0.2664628392334352</v>
       </c>
       <c r="J11">
+        <v>0.2862144791013954</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
         <v>0.3730356032872126</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>0.2273945170531899</v>
-      </c>
       <c r="M11">
-        <v>0.9569216284928839</v>
+        <v>-0.005120395540669093</v>
       </c>
       <c r="N11">
-        <v>-0.07720906754130509</v>
+        <v>0.2336922242139398</v>
       </c>
       <c r="O11">
-        <v>0.8213573610483902</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>0.3370899062620499</v>
+      </c>
+      <c r="P11">
+        <v>0.1816867800423102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.09569154803023676</v>
+        <v>0.07145745119241201</v>
       </c>
       <c r="C12">
-        <v>0.1237571271336534</v>
+        <v>-0.07889299984295564</v>
       </c>
       <c r="D12">
-        <v>0.1766723565517075</v>
+        <v>-0.5317768186373113</v>
       </c>
       <c r="E12">
-        <v>-0.05749781206784608</v>
-      </c>
-      <c r="G12">
-        <v>-0.01143832450566349</v>
+        <v>0.1010925659905756</v>
+      </c>
+      <c r="F12">
+        <v>0.2977848790824405</v>
       </c>
       <c r="H12">
-        <v>-0.347064490796336</v>
+        <v>0.4163707152817249</v>
       </c>
       <c r="I12">
-        <v>0.08087592040379925</v>
+        <v>-0.1960758592444096</v>
       </c>
       <c r="J12">
-        <v>-0.005120395540669093</v>
+        <v>0.7884343634426342</v>
       </c>
       <c r="K12">
+        <v>0.3730356032872126</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>0.2273945170531899</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0.266688302155974</v>
-      </c>
       <c r="N12">
-        <v>-0.3127709963931993</v>
+        <v>0.9569216284928839</v>
       </c>
       <c r="O12">
-        <v>0.044570176597717</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>-0.07720906754130509</v>
+      </c>
+      <c r="P12">
+        <v>0.8213573610483902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.03524498611133097</v>
+        <v>-0.09569154803023676</v>
       </c>
       <c r="C13">
-        <v>-0.03019904530512181</v>
+        <v>0.1237571271336534</v>
       </c>
       <c r="D13">
-        <v>0.06202386746339025</v>
+        <v>0.1098763086986835</v>
       </c>
       <c r="E13">
-        <v>0.07471037506210082</v>
-      </c>
-      <c r="G13">
-        <v>0.2112297758292304</v>
+        <v>0.1766723565517075</v>
+      </c>
+      <c r="F13">
+        <v>-0.05749781206784608</v>
       </c>
       <c r="H13">
-        <v>-0.2171218224399398</v>
+        <v>-0.01143832450566349</v>
       </c>
       <c r="I13">
-        <v>0.6644814596677858</v>
+        <v>-0.347064490796336</v>
       </c>
       <c r="J13">
-        <v>0.2336922242139398</v>
+        <v>0.08087592040379925</v>
       </c>
       <c r="K13">
-        <v>0.9569216284928839</v>
+        <v>-0.005120395540669093</v>
       </c>
       <c r="L13">
+        <v>0.2273945170531899</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>0.266688302155974</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>-0.1188419959597674</v>
-      </c>
       <c r="O13">
-        <v>0.7602727279385658</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>-0.3127709963931993</v>
+      </c>
+      <c r="P13">
+        <v>0.044570176597717</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.238878242919409</v>
+        <v>0.03524498611133097</v>
       </c>
       <c r="C14">
-        <v>0.1411896716252118</v>
+        <v>-0.03019904530512181</v>
       </c>
       <c r="D14">
-        <v>0.2608281976605054</v>
+        <v>-0.4077551084877684</v>
       </c>
       <c r="E14">
-        <v>0.2627015921725792</v>
-      </c>
-      <c r="G14">
-        <v>0.2815185517408797</v>
+        <v>0.06202386746339025</v>
+      </c>
+      <c r="F14">
+        <v>0.07471037506210082</v>
       </c>
       <c r="H14">
-        <v>0.9352104838129371</v>
+        <v>0.2112297758292304</v>
       </c>
       <c r="I14">
-        <v>-0.1612105954626258</v>
+        <v>-0.2171218224399398</v>
       </c>
       <c r="J14">
-        <v>0.3370899062620499</v>
+        <v>0.6644814596677858</v>
       </c>
       <c r="K14">
-        <v>-0.07720906754130509</v>
+        <v>0.2336922242139398</v>
       </c>
       <c r="L14">
-        <v>-0.3127709963931993</v>
+        <v>0.9569216284928839</v>
       </c>
       <c r="M14">
+        <v>0.266688302155974</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>-0.1188419959597674</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>-0.3259720137548081</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <v>0.7602727279385658</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
+        <v>-0.238878242919409</v>
+      </c>
+      <c r="C15">
+        <v>0.1411896716252118</v>
+      </c>
+      <c r="D15">
+        <v>0.3152940205507497</v>
+      </c>
+      <c r="E15">
+        <v>0.2608281976605054</v>
+      </c>
+      <c r="F15">
+        <v>0.2627015921725792</v>
+      </c>
+      <c r="H15">
+        <v>0.2815185517408797</v>
+      </c>
+      <c r="I15">
+        <v>0.9352104838129371</v>
+      </c>
+      <c r="J15">
+        <v>-0.1612105954626258</v>
+      </c>
+      <c r="K15">
+        <v>0.3370899062620499</v>
+      </c>
+      <c r="L15">
+        <v>-0.07720906754130509</v>
+      </c>
+      <c r="M15">
+        <v>-0.3127709963931993</v>
+      </c>
+      <c r="N15">
+        <v>-0.1188419959597674</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>-0.3259720137548081</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <v>0.05244044240843464</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0.02761189664673756</v>
       </c>
-      <c r="D15">
+      <c r="D16">
+        <v>-0.6703348258304175</v>
+      </c>
+      <c r="E16">
         <v>-0.09255504229564779</v>
       </c>
-      <c r="E15">
+      <c r="F16">
         <v>0.2515737508594499</v>
       </c>
-      <c r="G15">
+      <c r="H16">
         <v>0.3159095033480881</v>
       </c>
-      <c r="H15">
+      <c r="I16">
         <v>-0.3576867119968038</v>
       </c>
-      <c r="I15">
+      <c r="J16">
         <v>0.8915350258456595</v>
       </c>
-      <c r="J15">
+      <c r="K16">
         <v>0.1816867800423102</v>
       </c>
-      <c r="K15">
+      <c r="L16">
         <v>0.8213573610483902</v>
       </c>
-      <c r="L15">
+      <c r="M16">
         <v>0.044570176597717</v>
       </c>
-      <c r="M15">
+      <c r="N16">
         <v>0.7602727279385658</v>
       </c>
-      <c r="N15">
+      <c r="O16">
         <v>-0.3259720137548081</v>
       </c>
-      <c r="O15">
+      <c r="P16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. slides presentations for Apr27,2021. 2. Solving life cycle with MA codes. 3. SIPP stylized charts.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corr3mvM.xlsx
+++ b/WorkingFolder/Tables/corr3mvM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>sp500</t>
   </si>
@@ -31,9 +31,6 @@
     <t>iqrMed</t>
   </si>
   <si>
-    <t>skewMed</t>
-  </si>
-  <si>
     <t>varMed</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
   </si>
   <si>
     <t>iqrMean</t>
-  </si>
-  <si>
-    <t>skewMean</t>
   </si>
   <si>
     <t>varMean</t>
@@ -416,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,14 +456,8 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,658 +465,567 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.7515833566942681</v>
+        <v>-0.7342851760879413</v>
       </c>
       <c r="D2">
-        <v>-0.2110384727942434</v>
+        <v>-0.1637832418701619</v>
       </c>
       <c r="E2">
-        <v>-0.1211002744327765</v>
+        <v>-0.09369274312241575</v>
       </c>
       <c r="F2">
-        <v>-0.03198733403962323</v>
+        <v>-0.03238069579675275</v>
+      </c>
+      <c r="G2">
+        <v>-0.04536015141092318</v>
       </c>
       <c r="H2">
-        <v>-0.03067636664815504</v>
+        <v>-0.1561266264055378</v>
       </c>
       <c r="I2">
-        <v>-0.2128317531051811</v>
+        <v>-0.05555546805270414</v>
       </c>
       <c r="J2">
-        <v>-0.04909269184698396</v>
+        <v>-0.09152776117511119</v>
       </c>
       <c r="K2">
-        <v>-0.109523284579041</v>
+        <v>0.05706686836229626</v>
       </c>
       <c r="L2">
-        <v>0.07145745119241201</v>
+        <v>0.03011850634296642</v>
       </c>
       <c r="M2">
-        <v>-0.09569154803023676</v>
+        <v>-0.1450917091381959</v>
       </c>
       <c r="N2">
-        <v>0.03524498611133097</v>
-      </c>
-      <c r="O2">
-        <v>-0.238878242919409</v>
-      </c>
-      <c r="P2">
-        <v>0.05244044240843464</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>0.04461701553975975</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.7515833566942681</v>
+        <v>-0.7342851760879413</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1988341993235634</v>
+        <v>0.2005434104828867</v>
       </c>
       <c r="E3">
-        <v>0.1183818032404943</v>
+        <v>0.09228867089145851</v>
       </c>
       <c r="F3">
-        <v>-0.0427249620654119</v>
+        <v>-0.05400779891601992</v>
+      </c>
+      <c r="G3">
+        <v>-0.04739349506103868</v>
       </c>
       <c r="H3">
-        <v>-0.01940981040636119</v>
+        <v>0.1738587083941613</v>
       </c>
       <c r="I3">
-        <v>0.1686289861464561</v>
+        <v>0.06621385780928543</v>
       </c>
       <c r="J3">
-        <v>0.1051672521303078</v>
+        <v>-0.03868976266636538</v>
       </c>
       <c r="K3">
-        <v>-0.01637347079980878</v>
+        <v>-0.1096737141559664</v>
       </c>
       <c r="L3">
-        <v>-0.07889299984295564</v>
+        <v>-0.05778441854459836</v>
       </c>
       <c r="M3">
-        <v>0.1237571271336534</v>
+        <v>0.1408523987356279</v>
       </c>
       <c r="N3">
-        <v>-0.03019904530512181</v>
-      </c>
-      <c r="O3">
-        <v>0.1411896716252118</v>
-      </c>
-      <c r="P3">
-        <v>0.02761189664673756</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>-0.01038095594295483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.2110384727942434</v>
+        <v>-0.1637832418701619</v>
       </c>
       <c r="C4">
-        <v>0.1988341993235634</v>
+        <v>0.2005434104828867</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.4004509642697959</v>
+        <v>0.3888469167606836</v>
       </c>
       <c r="F4">
-        <v>-0.2809081383745311</v>
+        <v>-0.3149591612852934</v>
+      </c>
+      <c r="G4">
+        <v>-0.2991291631428855</v>
       </c>
       <c r="H4">
-        <v>-0.3160885375969492</v>
+        <v>0.4441775960196978</v>
       </c>
       <c r="I4">
-        <v>0.432172463729226</v>
+        <v>-0.6412169519045817</v>
       </c>
       <c r="J4">
-        <v>-0.6574251904662259</v>
+        <v>-0.06694479438367174</v>
       </c>
       <c r="K4">
-        <v>-0.01695605734072748</v>
+        <v>-0.5572105699425692</v>
       </c>
       <c r="L4">
-        <v>-0.5317768186373113</v>
+        <v>-0.4236786894885357</v>
       </c>
       <c r="M4">
-        <v>0.1098763086986835</v>
+        <v>0.4028751147396333</v>
       </c>
       <c r="N4">
-        <v>-0.4077551084877684</v>
-      </c>
-      <c r="O4">
-        <v>0.3152940205507497</v>
-      </c>
-      <c r="P4">
-        <v>-0.6703348258304175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>-0.6361146911579891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.1211002744327765</v>
+        <v>-0.09369274312241575</v>
       </c>
       <c r="C5">
-        <v>0.1183818032404943</v>
+        <v>0.09228867089145851</v>
       </c>
       <c r="D5">
-        <v>0.4004509642697959</v>
+        <v>0.3888469167606836</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.2862096796565572</v>
+        <v>0.2686112496280435</v>
+      </c>
+      <c r="G5">
+        <v>0.2877989144728421</v>
       </c>
       <c r="H5">
-        <v>0.2858119586419813</v>
+        <v>0.3571653415626364</v>
       </c>
       <c r="I5">
-        <v>0.3208449815547014</v>
+        <v>-0.07633023288678563</v>
       </c>
       <c r="J5">
-        <v>-0.03615914419776285</v>
+        <v>0.7911298232460501</v>
       </c>
       <c r="K5">
-        <v>0.8042684740305435</v>
+        <v>0.0140378454629565</v>
       </c>
       <c r="L5">
-        <v>0.1010925659905756</v>
+        <v>-0.03031907665812245</v>
       </c>
       <c r="M5">
-        <v>0.1766723565517075</v>
+        <v>0.3141868959392485</v>
       </c>
       <c r="N5">
-        <v>0.06202386746339025</v>
-      </c>
-      <c r="O5">
-        <v>0.2608281976605054</v>
-      </c>
-      <c r="P5">
-        <v>-0.09255504229564779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>-0.1784165964148658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.03198733403962323</v>
+        <v>-0.03238069579675275</v>
       </c>
       <c r="C6">
-        <v>-0.0427249620654119</v>
+        <v>-0.05400779891601992</v>
       </c>
       <c r="D6">
-        <v>-0.2809081383745311</v>
+        <v>-0.3149591612852934</v>
       </c>
       <c r="E6">
-        <v>0.2862096796565572</v>
+        <v>0.2686112496280435</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6">
+        <v>0.978026761606735</v>
+      </c>
       <c r="H6">
-        <v>0.9628637223458245</v>
+        <v>0.1063762981591651</v>
       </c>
       <c r="I6">
-        <v>0.1878429442749909</v>
+        <v>0.3475998932202026</v>
       </c>
       <c r="J6">
-        <v>0.4840581834101727</v>
+        <v>0.558027061705248</v>
       </c>
       <c r="K6">
-        <v>0.622812431914202</v>
+        <v>0.1202008293266585</v>
       </c>
       <c r="L6">
-        <v>0.2977848790824405</v>
+        <v>-0.12767441040606</v>
       </c>
       <c r="M6">
-        <v>-0.05749781206784608</v>
+        <v>0.09682421142294516</v>
       </c>
       <c r="N6">
-        <v>0.07471037506210082</v>
-      </c>
-      <c r="O6">
-        <v>0.2627015921725792</v>
-      </c>
-      <c r="P6">
-        <v>0.2515737508594499</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>0.1908475183058726</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="B7">
+        <v>-0.04536015141092318</v>
+      </c>
+      <c r="C7">
+        <v>-0.04739349506103868</v>
+      </c>
+      <c r="D7">
+        <v>-0.2991291631428855</v>
+      </c>
+      <c r="E7">
+        <v>0.2877989144728421</v>
+      </c>
+      <c r="F7">
+        <v>0.978026761606735</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.1394027466545903</v>
+      </c>
+      <c r="I7">
+        <v>0.4197692057913728</v>
+      </c>
+      <c r="J7">
+        <v>0.6045980014529664</v>
+      </c>
+      <c r="K7">
+        <v>0.2091764527153063</v>
+      </c>
+      <c r="L7">
+        <v>-0.03687555007865142</v>
+      </c>
+      <c r="M7">
+        <v>0.139637359323824</v>
+      </c>
+      <c r="N7">
+        <v>0.2230552944942695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.03067636664815504</v>
+        <v>-0.1561266264055378</v>
       </c>
       <c r="C8">
-        <v>-0.01940981040636119</v>
+        <v>0.1738587083941613</v>
       </c>
       <c r="D8">
-        <v>-0.3160885375969492</v>
+        <v>0.4441775960196978</v>
       </c>
       <c r="E8">
-        <v>0.2858119586419813</v>
+        <v>0.3571653415626364</v>
       </c>
       <c r="F8">
-        <v>0.9628637223458245</v>
+        <v>0.1063762981591651</v>
+      </c>
+      <c r="G8">
+        <v>0.1394027466545903</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.1850100977435571</v>
+        <v>-0.2149294589533946</v>
       </c>
       <c r="J8">
-        <v>0.5389219049867383</v>
+        <v>0.2577909383113714</v>
       </c>
       <c r="K8">
-        <v>0.6093980989173357</v>
+        <v>-0.2001197653127584</v>
       </c>
       <c r="L8">
-        <v>0.4163707152817249</v>
+        <v>-0.2103211622907177</v>
       </c>
       <c r="M8">
-        <v>-0.01143832450566349</v>
+        <v>0.9316313880638823</v>
       </c>
       <c r="N8">
-        <v>0.2112297758292304</v>
-      </c>
-      <c r="O8">
-        <v>0.2815185517408797</v>
-      </c>
-      <c r="P8">
-        <v>0.3159095033480881</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>-0.3105187693373601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.2128317531051811</v>
+        <v>-0.05555546805270414</v>
       </c>
       <c r="C9">
-        <v>0.1686289861464561</v>
+        <v>0.06621385780928543</v>
       </c>
       <c r="D9">
-        <v>0.432172463729226</v>
+        <v>-0.6412169519045817</v>
       </c>
       <c r="E9">
-        <v>0.3208449815547014</v>
+        <v>-0.07633023288678563</v>
       </c>
       <c r="F9">
-        <v>0.1878429442749909</v>
+        <v>0.3475998932202026</v>
+      </c>
+      <c r="G9">
+        <v>0.4197692057913728</v>
       </c>
       <c r="H9">
-        <v>0.1850100977435571</v>
+        <v>-0.2149294589533946</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>-0.2213412639926016</v>
+        <v>0.306701577001422</v>
       </c>
       <c r="K9">
-        <v>0.2664628392334352</v>
+        <v>0.8239091576213813</v>
       </c>
       <c r="L9">
-        <v>-0.1960758592444096</v>
+        <v>0.6977294633744532</v>
       </c>
       <c r="M9">
-        <v>-0.347064490796336</v>
+        <v>-0.2611156461962201</v>
       </c>
       <c r="N9">
-        <v>-0.2171218224399398</v>
-      </c>
-      <c r="O9">
-        <v>0.9352104838129371</v>
-      </c>
-      <c r="P9">
-        <v>-0.3576867119968038</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>0.8934817950955275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.04909269184698396</v>
+        <v>-0.09152776117511119</v>
       </c>
       <c r="C10">
-        <v>0.1051672521303078</v>
+        <v>-0.03868976266636538</v>
       </c>
       <c r="D10">
-        <v>-0.6574251904662259</v>
+        <v>-0.06694479438367174</v>
       </c>
       <c r="E10">
-        <v>-0.03615914419776285</v>
+        <v>0.7911298232460501</v>
       </c>
       <c r="F10">
-        <v>0.4840581834101727</v>
+        <v>0.558027061705248</v>
+      </c>
+      <c r="G10">
+        <v>0.6045980014529664</v>
       </c>
       <c r="H10">
-        <v>0.5389219049867383</v>
+        <v>0.2577909383113714</v>
       </c>
       <c r="I10">
-        <v>-0.2213412639926016</v>
+        <v>0.306701577001422</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.2862144791013954</v>
+        <v>0.3896656122977718</v>
       </c>
       <c r="L10">
-        <v>0.7884343634426342</v>
+        <v>0.2402093549498194</v>
       </c>
       <c r="M10">
-        <v>0.08087592040379925</v>
+        <v>0.2768564265223313</v>
       </c>
       <c r="N10">
-        <v>0.6644814596677858</v>
-      </c>
-      <c r="O10">
-        <v>-0.1612105954626258</v>
-      </c>
-      <c r="P10">
-        <v>0.8915350258456595</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>0.1921870599088166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.109523284579041</v>
+        <v>0.05706686836229626</v>
       </c>
       <c r="C11">
-        <v>-0.01637347079980878</v>
+        <v>-0.1096737141559664</v>
       </c>
       <c r="D11">
-        <v>-0.01695605734072748</v>
+        <v>-0.5572105699425692</v>
       </c>
       <c r="E11">
-        <v>0.8042684740305435</v>
+        <v>0.0140378454629565</v>
       </c>
       <c r="F11">
-        <v>0.622812431914202</v>
+        <v>0.1202008293266585</v>
+      </c>
+      <c r="G11">
+        <v>0.2091764527153063</v>
       </c>
       <c r="H11">
-        <v>0.6093980989173357</v>
+        <v>-0.2001197653127584</v>
       </c>
       <c r="I11">
-        <v>0.2664628392334352</v>
+        <v>0.8239091576213813</v>
       </c>
       <c r="J11">
-        <v>0.2862144791013954</v>
+        <v>0.3896656122977718</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.3730356032872126</v>
+        <v>0.9539313250320182</v>
       </c>
       <c r="M11">
-        <v>-0.005120395540669093</v>
+        <v>-0.1831662709773509</v>
       </c>
       <c r="N11">
-        <v>0.2336922242139398</v>
-      </c>
-      <c r="O11">
-        <v>0.3370899062620499</v>
-      </c>
-      <c r="P11">
-        <v>0.1816867800423102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>0.8427604695007406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.07145745119241201</v>
+        <v>0.03011850634296642</v>
       </c>
       <c r="C12">
-        <v>-0.07889299984295564</v>
+        <v>-0.05778441854459836</v>
       </c>
       <c r="D12">
-        <v>-0.5317768186373113</v>
+        <v>-0.4236786894885357</v>
       </c>
       <c r="E12">
-        <v>0.1010925659905756</v>
+        <v>-0.03031907665812245</v>
       </c>
       <c r="F12">
-        <v>0.2977848790824405</v>
+        <v>-0.12767441040606</v>
+      </c>
+      <c r="G12">
+        <v>-0.03687555007865142</v>
       </c>
       <c r="H12">
-        <v>0.4163707152817249</v>
+        <v>-0.2103211622907177</v>
       </c>
       <c r="I12">
-        <v>-0.1960758592444096</v>
+        <v>0.6977294633744532</v>
       </c>
       <c r="J12">
-        <v>0.7884343634426342</v>
+        <v>0.2402093549498194</v>
       </c>
       <c r="K12">
-        <v>0.3730356032872126</v>
+        <v>0.9539313250320182</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.2273945170531899</v>
+        <v>-0.1935356243054586</v>
       </c>
       <c r="N12">
-        <v>0.9569216284928839</v>
-      </c>
-      <c r="O12">
-        <v>-0.07720906754130509</v>
-      </c>
-      <c r="P12">
-        <v>0.8213573610483902</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>0.7824819260056153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.09569154803023676</v>
+        <v>-0.1450917091381959</v>
       </c>
       <c r="C13">
-        <v>0.1237571271336534</v>
+        <v>0.1408523987356279</v>
       </c>
       <c r="D13">
-        <v>0.1098763086986835</v>
+        <v>0.4028751147396333</v>
       </c>
       <c r="E13">
-        <v>0.1766723565517075</v>
+        <v>0.3141868959392485</v>
       </c>
       <c r="F13">
-        <v>-0.05749781206784608</v>
+        <v>0.09682421142294516</v>
+      </c>
+      <c r="G13">
+        <v>0.139637359323824</v>
       </c>
       <c r="H13">
-        <v>-0.01143832450566349</v>
+        <v>0.9316313880638823</v>
       </c>
       <c r="I13">
-        <v>-0.347064490796336</v>
+        <v>-0.2611156461962201</v>
       </c>
       <c r="J13">
-        <v>0.08087592040379925</v>
+        <v>0.2768564265223313</v>
       </c>
       <c r="K13">
-        <v>-0.005120395540669093</v>
+        <v>-0.1831662709773509</v>
       </c>
       <c r="L13">
-        <v>0.2273945170531899</v>
+        <v>-0.1935356243054586</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.266688302155974</v>
-      </c>
-      <c r="O13">
-        <v>-0.3127709963931993</v>
-      </c>
-      <c r="P13">
-        <v>0.044570176597717</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>-0.3372276940927075</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.03524498611133097</v>
+        <v>0.04461701553975975</v>
       </c>
       <c r="C14">
-        <v>-0.03019904530512181</v>
+        <v>-0.01038095594295483</v>
       </c>
       <c r="D14">
-        <v>-0.4077551084877684</v>
+        <v>-0.6361146911579891</v>
       </c>
       <c r="E14">
-        <v>0.06202386746339025</v>
+        <v>-0.1784165964148658</v>
       </c>
       <c r="F14">
-        <v>0.07471037506210082</v>
+        <v>0.1908475183058726</v>
+      </c>
+      <c r="G14">
+        <v>0.2230552944942695</v>
       </c>
       <c r="H14">
-        <v>0.2112297758292304</v>
+        <v>-0.3105187693373601</v>
       </c>
       <c r="I14">
-        <v>-0.2171218224399398</v>
+        <v>0.8934817950955275</v>
       </c>
       <c r="J14">
-        <v>0.6644814596677858</v>
+        <v>0.1921870599088166</v>
       </c>
       <c r="K14">
-        <v>0.2336922242139398</v>
+        <v>0.8427604695007406</v>
       </c>
       <c r="L14">
-        <v>0.9569216284928839</v>
+        <v>0.7824819260056153</v>
       </c>
       <c r="M14">
-        <v>0.266688302155974</v>
+        <v>-0.3372276940927075</v>
       </c>
       <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>-0.1188419959597674</v>
-      </c>
-      <c r="P14">
-        <v>0.7602727279385658</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>-0.238878242919409</v>
-      </c>
-      <c r="C15">
-        <v>0.1411896716252118</v>
-      </c>
-      <c r="D15">
-        <v>0.3152940205507497</v>
-      </c>
-      <c r="E15">
-        <v>0.2608281976605054</v>
-      </c>
-      <c r="F15">
-        <v>0.2627015921725792</v>
-      </c>
-      <c r="H15">
-        <v>0.2815185517408797</v>
-      </c>
-      <c r="I15">
-        <v>0.9352104838129371</v>
-      </c>
-      <c r="J15">
-        <v>-0.1612105954626258</v>
-      </c>
-      <c r="K15">
-        <v>0.3370899062620499</v>
-      </c>
-      <c r="L15">
-        <v>-0.07720906754130509</v>
-      </c>
-      <c r="M15">
-        <v>-0.3127709963931993</v>
-      </c>
-      <c r="N15">
-        <v>-0.1188419959597674</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>-0.3259720137548081</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>0.05244044240843464</v>
-      </c>
-      <c r="C16">
-        <v>0.02761189664673756</v>
-      </c>
-      <c r="D16">
-        <v>-0.6703348258304175</v>
-      </c>
-      <c r="E16">
-        <v>-0.09255504229564779</v>
-      </c>
-      <c r="F16">
-        <v>0.2515737508594499</v>
-      </c>
-      <c r="H16">
-        <v>0.3159095033480881</v>
-      </c>
-      <c r="I16">
-        <v>-0.3576867119968038</v>
-      </c>
-      <c r="J16">
-        <v>0.8915350258456595</v>
-      </c>
-      <c r="K16">
-        <v>0.1816867800423102</v>
-      </c>
-      <c r="L16">
-        <v>0.8213573610483902</v>
-      </c>
-      <c r="M16">
-        <v>0.044570176597717</v>
-      </c>
-      <c r="N16">
-        <v>0.7602727279385658</v>
-      </c>
-      <c r="O16">
-        <v>-0.3259720137548081</v>
-      </c>
-      <c r="P16">
         <v>1</v>
       </c>
     </row>

</xml_diff>